<commit_message>
Some corrections in the turbine losses calculation
</commit_message>
<xml_diff>
--- a/Results/inputGrassmann.xlsx
+++ b/Results/inputGrassmann.xlsx
@@ -187,7 +187,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -668,11 +668,11 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -793,7 +793,7 @@
         </row>
         <row r="4">
           <cell r="B4">
-            <v>4926962.3663933296</v>
+            <v>4926962.3663933398</v>
           </cell>
           <cell r="C4">
             <v>1620.76269483027</v>
@@ -825,13 +825,13 @@
             <v>7281.9582682034898</v>
           </cell>
           <cell r="D6">
-            <v>5536939.8527830401</v>
+            <v>5536939.8527830504</v>
           </cell>
           <cell r="E6">
             <v>678972.67730250105</v>
           </cell>
           <cell r="F6">
-            <v>787797.88567637803</v>
+            <v>787797.88567637699</v>
           </cell>
           <cell r="G6">
             <v>2835006.8651367999</v>
@@ -857,7 +857,7 @@
             <v>383528.80281094002</v>
           </cell>
           <cell r="F8">
-            <v>749069.08589824499</v>
+            <v>749069.08589824603</v>
           </cell>
           <cell r="G8">
             <v>1670471.3403771501</v>
@@ -909,10 +909,10 @@
             <v>78783.645445033602</v>
           </cell>
           <cell r="F10">
-            <v>84594.647443257098</v>
+            <v>84594.647443257301</v>
           </cell>
           <cell r="G10">
-            <v>423325.36575127702</v>
+            <v>423325.365751278</v>
           </cell>
           <cell r="H10">
             <v>414728.588719577</v>
@@ -970,7 +970,7 @@
             <v>1190548.2310515901</v>
           </cell>
           <cell r="I18">
-            <v>632835.53900760901</v>
+            <v>632835.53900760994</v>
           </cell>
         </row>
         <row r="22">
@@ -1131,28 +1131,28 @@
         </row>
         <row r="48">
           <cell r="B48">
-            <v>195276.908345654</v>
+            <v>195276.90834565301</v>
           </cell>
           <cell r="C48">
-            <v>175.29581019732299</v>
+            <v>175.295810197322</v>
           </cell>
           <cell r="D48">
-            <v>153985.11329395001</v>
+            <v>153985.11329394899</v>
           </cell>
           <cell r="E48">
-            <v>18035.987546669799</v>
+            <v>18035.987546669701</v>
           </cell>
           <cell r="F48">
-            <v>23080.511694837202</v>
+            <v>23080.511694837001</v>
           </cell>
           <cell r="G48">
-            <v>82841.3342498438</v>
+            <v>82841.334249843494</v>
           </cell>
           <cell r="H48">
-            <v>80544.112909459305</v>
+            <v>80544.112909459</v>
           </cell>
           <cell r="I48">
-            <v>31891.461186351102</v>
+            <v>31891.461186351</v>
           </cell>
         </row>
         <row r="54">
@@ -1160,7 +1160,7 @@
             <v>5913328.1486983597</v>
           </cell>
           <cell r="C54">
-            <v>1903.2842146630301</v>
+            <v>1903.2842146630201</v>
           </cell>
           <cell r="D54">
             <v>4496054.8969572196</v>
@@ -1169,7 +1169,7 @@
             <v>529298.60657545296</v>
           </cell>
           <cell r="F54">
-            <v>886071.36095103796</v>
+            <v>886071.36095103703</v>
           </cell>
           <cell r="G54">
             <v>2283658.8161976999</v>
@@ -1204,7 +1204,7 @@
             <v>1776437.48987486</v>
           </cell>
           <cell r="I55">
-            <v>895127.74186373502</v>
+            <v>895127.74186373595</v>
           </cell>
         </row>
         <row r="97">
@@ -1227,10 +1227,10 @@
             <v>1839861.2049453601</v>
           </cell>
           <cell r="H97">
-            <v>1846217.2963107801</v>
+            <v>1846217.2963107701</v>
           </cell>
           <cell r="I97">
-            <v>731595.57359962596</v>
+            <v>731595.57359962701</v>
           </cell>
         </row>
         <row r="479">
@@ -2024,8 +2024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P162"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B161" sqref="B161:E162"/>
+    <sheetView topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="D149" sqref="D149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2042,14 +2042,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2"/>
+      <c r="D1" s="4"/>
       <c r="E1" t="s">
         <v>2</v>
       </c>
@@ -2234,7 +2234,7 @@
       </c>
       <c r="M4" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!I$18,0,0)</f>
-        <v>632835.53900760901</v>
+        <v>632835.53900760994</v>
       </c>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
@@ -2308,7 +2308,7 @@
       </c>
       <c r="F6" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$4,0,0)</f>
-        <v>4926962.3663933296</v>
+        <v>4926962.3663933398</v>
       </c>
       <c r="G6" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!C$4,0,0)</f>
@@ -2418,7 +2418,7 @@
       </c>
       <c r="H8" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!D$6,0,0)</f>
-        <v>5536939.8527830401</v>
+        <v>5536939.8527830504</v>
       </c>
       <c r="I8" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!E$6,0,0)</f>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="J8" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!F$6,0,0)</f>
-        <v>787797.88567637803</v>
+        <v>787797.88567637699</v>
       </c>
       <c r="K8" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$6,0,0)</f>
@@ -2461,35 +2461,35 @@
       </c>
       <c r="F9" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$48,0,0)</f>
-        <v>195276.908345654</v>
+        <v>195276.90834565301</v>
       </c>
       <c r="G9" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!C$48,0,0)</f>
-        <v>175.29581019732299</v>
+        <v>175.295810197322</v>
       </c>
       <c r="H9" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!D$48,0,0)</f>
-        <v>153985.11329395001</v>
+        <v>153985.11329394899</v>
       </c>
       <c r="I9" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!E$48,0,0)</f>
-        <v>18035.987546669799</v>
+        <v>18035.987546669701</v>
       </c>
       <c r="J9" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!F$48,0,0)</f>
-        <v>23080.511694837202</v>
+        <v>23080.511694837001</v>
       </c>
       <c r="K9" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$48,0,0)</f>
-        <v>82841.3342498438</v>
+        <v>82841.334249843494</v>
       </c>
       <c r="L9" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!H$48,0,0)</f>
-        <v>80544.112909459305</v>
+        <v>80544.112909459</v>
       </c>
       <c r="M9" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!I$48,0,0)</f>
-        <v>31891.461186351102</v>
+        <v>31891.461186351</v>
       </c>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -2528,7 +2528,7 @@
       </c>
       <c r="J10" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!F$8,0,0)</f>
-        <v>749069.08589824499</v>
+        <v>749069.08589824603</v>
       </c>
       <c r="K10" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$8,0,0)</f>
@@ -2579,11 +2579,11 @@
       </c>
       <c r="J11" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!F$10,0,0)</f>
-        <v>84594.647443257098</v>
+        <v>84594.647443257301</v>
       </c>
       <c r="K11" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$10,0,0)</f>
-        <v>423325.36575127702</v>
+        <v>423325.365751278</v>
       </c>
       <c r="L11" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!H$10,0,0)</f>
@@ -2642,7 +2642,7 @@
       </c>
       <c r="M12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>96647.310018072953</v>
+        <v>96647.310018072021</v>
       </c>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -2693,7 +2693,7 @@
       </c>
       <c r="M13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>56424.63383355306</v>
+        <v>56424.633833553991</v>
       </c>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
@@ -3275,7 +3275,7 @@
       </c>
       <c r="J25" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!F$11,47,0)</f>
-        <v>1792053.8481864301</v>
+        <v>1792053.8481864401</v>
       </c>
       <c r="K25" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$11,47,0)</f>
@@ -3308,11 +3308,11 @@
       </c>
       <c r="F26" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$6,47,0)</f>
-        <v>8004848.38229034</v>
+        <v>8004848.3822903298</v>
       </c>
       <c r="G26" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!C$6,47,0)</f>
-        <v>6244.2920093736202</v>
+        <v>6244.2920093736302</v>
       </c>
       <c r="H26" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!D$6,47,0)</f>
@@ -3328,7 +3328,7 @@
       </c>
       <c r="K26" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$6,47,0)</f>
-        <v>3320015.5441802</v>
+        <v>3320015.5441801902</v>
       </c>
       <c r="L26" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!H$6,47,0)</f>
@@ -3361,7 +3361,7 @@
       </c>
       <c r="G27" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!C$48,47,0)</f>
-        <v>142.12114810237699</v>
+        <v>142.121148102376</v>
       </c>
       <c r="H27" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!D$48,47,0)</f>
@@ -3369,23 +3369,23 @@
       </c>
       <c r="I27" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!E$48,47,0)</f>
-        <v>18985.668424801901</v>
+        <v>18985.668424801799</v>
       </c>
       <c r="J27" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!F$48,47,0)</f>
-        <v>22358.610901442102</v>
+        <v>22358.610901442</v>
       </c>
       <c r="K27" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$48,47,0)</f>
-        <v>89987.391464632106</v>
+        <v>89987.391464631801</v>
       </c>
       <c r="L27" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!H$48,47,0)</f>
-        <v>87035.375106322303</v>
+        <v>87035.375106321895</v>
       </c>
       <c r="M27" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!I$48,47,0)</f>
-        <v>34387.393442515197</v>
+        <v>34387.393442515102</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3434,7 +3434,7 @@
       </c>
       <c r="M28" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!I$8,47,0)</f>
-        <v>895127.74186373502</v>
+        <v>895127.74186373595</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3467,11 +3467,11 @@
       </c>
       <c r="I29" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!E$10,47,0)</f>
-        <v>82332.755590927802</v>
+        <v>82332.755590927904</v>
       </c>
       <c r="J29" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!F$10,47,0)</f>
-        <v>90173.793796393496</v>
+        <v>90173.7937963937</v>
       </c>
       <c r="K29" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$10,47,0)</f>
@@ -3651,7 +3651,7 @@
       </c>
       <c r="F33" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$36,47,0)</f>
-        <v>2063758.34458016</v>
+        <v>2063758.34458015</v>
       </c>
       <c r="G33" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!C$36,47,0)</f>
@@ -3700,7 +3700,7 @@
       </c>
       <c r="F34" s="1">
         <f t="shared" ref="F34:M34" ca="1" si="4">F33</f>
-        <v>2063758.34458016</v>
+        <v>2063758.34458015</v>
       </c>
       <c r="G34" s="1">
         <f t="shared" ca="1" si="4"/>
@@ -3847,11 +3847,11 @@
       </c>
       <c r="F37" s="1">
         <f t="shared" ref="F37:M37" ca="1" si="6">F26-F38</f>
-        <v>3587174.3074345896</v>
+        <v>3587174.3074345794</v>
       </c>
       <c r="G37" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>3869.4917156394604</v>
+        <v>3869.4917156394704</v>
       </c>
       <c r="H37" s="1">
         <f t="shared" ca="1" si="6"/>
@@ -3867,15 +3867,15 @@
       </c>
       <c r="K37" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>1480154.3392348399</v>
+        <v>1480154.3392348301</v>
       </c>
       <c r="L37" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>1500612.7352264198</v>
+        <v>1500612.7352264298</v>
       </c>
       <c r="M37" s="1">
         <f t="shared" ca="1" si="6"/>
-        <v>606407.23297331401</v>
+        <v>606407.23297331296</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3920,11 +3920,11 @@
       </c>
       <c r="L38" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!H$97,0,0)</f>
-        <v>1846217.2963107801</v>
+        <v>1846217.2963107701</v>
       </c>
       <c r="M38" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!I$97,0,0)</f>
-        <v>731595.57359962596</v>
+        <v>731595.57359962701</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4206,7 +4206,7 @@
       </c>
       <c r="J44" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!F$4,98,0)</f>
-        <v>795864.81847150903</v>
+        <v>795864.81847150996</v>
       </c>
       <c r="K44" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$4,98,0)</f>
@@ -4316,7 +4316,7 @@
       </c>
       <c r="M46" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!I$6,98,0)</f>
-        <v>1182013.90334582</v>
+        <v>1182013.90334583</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4341,7 +4341,7 @@
       </c>
       <c r="G47" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!C$48,98,0)</f>
-        <v>198.17375518569901</v>
+        <v>198.17375518569801</v>
       </c>
       <c r="H47" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!D$48,98,0)</f>
@@ -4353,19 +4353,19 @@
       </c>
       <c r="J47" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!F$48,98,0)</f>
-        <v>21054.6792875264</v>
+        <v>21054.679287526302</v>
       </c>
       <c r="K47" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$48,98,0)</f>
-        <v>86525.234106772099</v>
+        <v>86525.234106771793</v>
       </c>
       <c r="L47" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!H$48,98,0)</f>
-        <v>89215.648887374497</v>
+        <v>89215.648887374206</v>
       </c>
       <c r="M47" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!I$48,98,0)</f>
-        <v>33931.666720622903</v>
+        <v>33931.666720622801</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4398,7 +4398,7 @@
       </c>
       <c r="I48" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!E$8,98,0)</f>
-        <v>329050.441386191</v>
+        <v>329050.44138619199</v>
       </c>
       <c r="J48" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!F$8,98,0)</f>
@@ -4414,7 +4414,7 @@
       </c>
       <c r="M48" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!I$8,98,0)</f>
-        <v>944866.13792910497</v>
+        <v>944866.13792910601</v>
       </c>
     </row>
     <row r="49" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4435,7 +4435,7 @@
       </c>
       <c r="F49" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$10,98,0)</f>
-        <v>961887.21341221803</v>
+        <v>961887.21341221896</v>
       </c>
       <c r="G49" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!C$10,98,0)</f>
@@ -4443,15 +4443,15 @@
       </c>
       <c r="H49" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!D$10,98,0)</f>
-        <v>840823.54453015199</v>
+        <v>840823.54453015304</v>
       </c>
       <c r="I49" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!E$10,98,0)</f>
-        <v>62641.485399866302</v>
+        <v>62641.485399866397</v>
       </c>
       <c r="J49" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!F$10,98,0)</f>
-        <v>58218.550275174297</v>
+        <v>58218.550275174399</v>
       </c>
       <c r="K49" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$10,98,0)</f>
@@ -4835,7 +4835,7 @@
       </c>
       <c r="H57" s="1">
         <f t="shared" ca="1" si="10"/>
-        <v>2659017.0612852494</v>
+        <v>2659017.0612852396</v>
       </c>
       <c r="I57" s="1">
         <f t="shared" ca="1" si="10"/>
@@ -4843,7 +4843,7 @@
       </c>
       <c r="J57" s="1">
         <f t="shared" ca="1" si="10"/>
-        <v>227900.48403580103</v>
+        <v>227900.48403580004</v>
       </c>
       <c r="K57" s="1">
         <f t="shared" ca="1" si="10"/>
@@ -4855,7 +4855,7 @@
       </c>
       <c r="M57" s="1">
         <f t="shared" ca="1" si="10"/>
-        <v>457511.31276463508</v>
+        <v>457511.31276464509</v>
       </c>
     </row>
     <row r="58" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4884,7 +4884,7 @@
       </c>
       <c r="H58" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!D$97,51,0)</f>
-        <v>3475771.7231674301</v>
+        <v>3475771.7231674399</v>
       </c>
       <c r="I58" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!E$97,51,0)</f>
@@ -4892,7 +4892,7 @@
       </c>
       <c r="J58" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!F$97,51,0)</f>
-        <v>452265.983084918</v>
+        <v>452265.98308491899</v>
       </c>
       <c r="K58" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$97,51,0)</f>
@@ -5239,7 +5239,7 @@
       </c>
       <c r="K65" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$11,149,0)</f>
-        <v>5318984.49041209</v>
+        <v>5318984.4904121002</v>
       </c>
       <c r="L65" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!H$11,149,0)</f>
@@ -5317,15 +5317,15 @@
       </c>
       <c r="F67" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$48,149,0)</f>
-        <v>192880.15894588301</v>
+        <v>192880.15894588199</v>
       </c>
       <c r="G67" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!C$48,149,0)</f>
-        <v>131.29396842901599</v>
+        <v>131.29396842901701</v>
       </c>
       <c r="H67" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!D$48,149,0)</f>
-        <v>157250.336467229</v>
+        <v>157250.33646722799</v>
       </c>
       <c r="I67" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!E$48,149,0)</f>
@@ -5333,19 +5333,19 @@
       </c>
       <c r="J67" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!F$48,149,0)</f>
-        <v>20172.081486608698</v>
+        <v>20172.0814866086</v>
       </c>
       <c r="K67" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$48,149,0)</f>
-        <v>81387.8837074982</v>
+        <v>81387.883707497895</v>
       </c>
       <c r="L67" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!H$48,149,0)</f>
-        <v>81120.021886810398</v>
+        <v>81120.021886810093</v>
       </c>
       <c r="M67" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!I$48,149,0)</f>
-        <v>30372.253351575098</v>
+        <v>30372.253351575</v>
       </c>
     </row>
     <row r="68" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5423,15 +5423,15 @@
       </c>
       <c r="H69" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!D$10,149,0)</f>
-        <v>758259.23271263496</v>
+        <v>758259.232712636</v>
       </c>
       <c r="I69" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!E$10,149,0)</f>
-        <v>53560.052402110698</v>
+        <v>53560.052402110799</v>
       </c>
       <c r="J69" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!F$10,149,0)</f>
-        <v>42506.999370678401</v>
+        <v>42506.999370678597</v>
       </c>
       <c r="K69" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$10,149,0)</f>
@@ -5439,7 +5439,7 @@
       </c>
       <c r="L69" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!H$10,149,0)</f>
-        <v>379294.57366594102</v>
+        <v>379294.57366594201</v>
       </c>
       <c r="M69" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!I$10,149,0)</f>
@@ -5635,7 +5635,7 @@
       </c>
       <c r="L73" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!H$36,149,0)</f>
-        <v>830821.66332895204</v>
+        <v>830821.66332895099</v>
       </c>
       <c r="M73" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!I$36,149,0)</f>
@@ -5684,7 +5684,7 @@
       </c>
       <c r="L74" s="1">
         <f t="shared" ca="1" si="12"/>
-        <v>830821.66332895204</v>
+        <v>830821.66332895099</v>
       </c>
       <c r="M74" s="1">
         <f t="shared" ca="1" si="12"/>
@@ -6149,10 +6149,10 @@
         <v>11</v>
       </c>
       <c r="C85" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="D85" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="E85" t="s">
         <v>7</v>
@@ -6208,35 +6208,35 @@
       </c>
       <c r="F86" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$48,196,0)</f>
-        <v>1064298.1706487699</v>
+        <v>164783.60676464101</v>
       </c>
       <c r="G86" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!C$48,196,0)</f>
-        <v>234001.97508336999</v>
+        <v>31049.529045089599</v>
       </c>
       <c r="H86" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!D$48,196,0)</f>
-        <v>685419.197093411</v>
+        <v>110117.949803447</v>
       </c>
       <c r="I86" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!E$48,196,0)</f>
-        <v>106344.37070568099</v>
+        <v>18787.174253938301</v>
       </c>
       <c r="J86" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!F$48,196,0)</f>
-        <v>38532.627766313497</v>
+        <v>4828.95366216613</v>
       </c>
       <c r="K86" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$48,196,0)</f>
-        <v>516242.602444202</v>
+        <v>79176.844905754901</v>
       </c>
       <c r="L86" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!H$48,196,0)</f>
-        <v>380296.953873694</v>
+        <v>63021.811148844703</v>
       </c>
       <c r="M86" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!I$48,196,0)</f>
-        <v>167758.61433088299</v>
+        <v>22584.9507100423</v>
       </c>
     </row>
     <row r="87" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7178,10 +7178,10 @@
         <v>11</v>
       </c>
       <c r="C106" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="D106" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="E106" t="s">
         <v>7</v>
@@ -7237,35 +7237,35 @@
       </c>
       <c r="F107" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$48,250,0)</f>
-        <v>798453.85992296296</v>
+        <v>124645.87588512601</v>
       </c>
       <c r="G107" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!C$48,250,0)</f>
-        <v>201950.00321692901</v>
+        <v>27845.870832592002</v>
       </c>
       <c r="H107" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!D$48,250,0)</f>
-        <v>482841.34984277003</v>
+        <v>77892.227512252895</v>
       </c>
       <c r="I107" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!E$48,250,0)</f>
-        <v>77524.747486646593</v>
+        <v>14410.172696444</v>
       </c>
       <c r="J107" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!F$48,250,0)</f>
-        <v>36137.759376616697</v>
+        <v>4497.6048438380403</v>
       </c>
       <c r="K107" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$48,250,0)</f>
-        <v>334137.89500664099</v>
+        <v>52343.341004908798</v>
       </c>
       <c r="L107" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!H$48,250,0)</f>
-        <v>347359.40341447497</v>
+        <v>56997.564695631801</v>
       </c>
       <c r="M107" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!I$48,250,0)</f>
-        <v>116956.56150184599</v>
+        <v>15304.970184586</v>
       </c>
     </row>
     <row r="108" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -8207,10 +8207,10 @@
         <v>11</v>
       </c>
       <c r="C127" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="D127" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="E127" t="s">
         <v>7</v>
@@ -8266,35 +8266,35 @@
       </c>
       <c r="F128" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$48,304,0)</f>
-        <v>537730.339069332</v>
+        <v>72317.438855280299</v>
       </c>
       <c r="G128" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!C$48,304,0)</f>
-        <v>446702.516273644</v>
+        <v>51851.917145802698</v>
       </c>
       <c r="H128" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!D$48,304,0)</f>
-        <v>31595.4809647818</v>
+        <v>7391.8745131793903</v>
       </c>
       <c r="I128" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!E$48,304,0)</f>
-        <v>59137.303123974598</v>
+        <v>13003.454753244399</v>
       </c>
       <c r="J128" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!F$48,304,0)</f>
-        <v>295.03870693226997</v>
+        <v>70.192443053612493</v>
       </c>
       <c r="K128" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$48,304,0)</f>
-        <v>220587.88756447399</v>
+        <v>28451.5857397691</v>
       </c>
       <c r="L128" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!H$48,304,0)</f>
-        <v>231457.01804339499</v>
+        <v>33585.520153721103</v>
       </c>
       <c r="M128" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!I$48,304,0)</f>
-        <v>85685.433461465203</v>
+        <v>10280.33296179</v>
       </c>
     </row>
     <row r="129" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -9236,10 +9236,10 @@
         <v>11</v>
       </c>
       <c r="C148" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="D148" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="E148" t="s">
         <v>7</v>
@@ -9295,35 +9295,35 @@
       </c>
       <c r="F149" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$48,358,0)</f>
-        <v>637211.99539853795</v>
+        <v>101056.329907345</v>
       </c>
       <c r="G149" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!C$48,358,0)</f>
-        <v>155028.83945419599</v>
+        <v>20986.629572596201</v>
       </c>
       <c r="H149" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!D$48,358,0)</f>
-        <v>392069.76879029197</v>
+        <v>63968.509609004002</v>
       </c>
       <c r="I149" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!E$48,358,0)</f>
-        <v>74797.168412714804</v>
+        <v>13968.5751451206</v>
       </c>
       <c r="J149" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!F$48,358,0)</f>
-        <v>15316.218741332301</v>
+        <v>2132.6155806236102</v>
       </c>
       <c r="K149" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$48,358,0)</f>
-        <v>318525.35892903898</v>
+        <v>49125.068752930798</v>
       </c>
       <c r="L149" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!H$48,358,0)</f>
-        <v>237872.10289844099</v>
+        <v>40581.182840110698</v>
       </c>
       <c r="M149" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!I$48,358,0)</f>
-        <v>80814.533571053995</v>
+        <v>11350.0783143031</v>
       </c>
     </row>
     <row r="150" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -9989,14 +9989,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2"/>
+      <c r="D1" s="4"/>
       <c r="E1" t="s">
         <v>2</v>
       </c>
@@ -10049,35 +10049,35 @@
       <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <f ca="1">SUMIFS('Engines indvidual'!F$1:F$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B2,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D2)*0.000001</f>
         <v>0.16386071481350747</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$1:G$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B2,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D2)*0.000001</f>
         <v>1.9719628228085149E-4</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$1:H$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B2,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D2)*0.000001</f>
         <v>0.14063041002530968</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$1:I$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B2,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D2)*0.000001</f>
         <v>1.2831814379719392E-2</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$1:J$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B2,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D2)*0.000001</f>
         <v>1.0201294126197261E-2</v>
       </c>
-      <c r="K2" s="4">
+      <c r="K2" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$1:K$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B2,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D2)*0.000001</f>
         <v>0.10164813340963609</v>
       </c>
-      <c r="L2" s="4">
+      <c r="L2" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$1:L$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B2,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D2)*0.000001</f>
         <v>4.8027000150418199E-2</v>
       </c>
-      <c r="M2" s="4">
+      <c r="M2" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$1:M$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B2,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D2)*0.000001</f>
         <v>1.418558125345251E-2</v>
       </c>
@@ -10098,35 +10098,35 @@
       <c r="E3" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <f ca="1">SUMIFS('Engines indvidual'!F$1:F$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B3,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D3)*0.000001</f>
         <v>13.639312433587621</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$1:G$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B3,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D3)*0.000001</f>
         <v>3.679393801285766E-3</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$1:H$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B3,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D3)*0.000001</f>
         <v>9.9323962269435686</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$1:I$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B3,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D3)*0.000001</f>
         <v>1.1480391577433668</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$1:J$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B3,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D3)*0.000001</f>
         <v>2.5551976550994078</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$1:K$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B3,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D3)*0.000001</f>
         <v>4.9763761772052995</v>
       </c>
-      <c r="L3" s="4">
+      <c r="L3" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$1:L$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B3,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D3)*0.000001</f>
         <v>5.6261658461808803</v>
       </c>
-      <c r="M3" s="4">
+      <c r="M3" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$1:M$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B3,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D3)*0.000001</f>
         <v>3.0367704102014295</v>
       </c>
@@ -10147,37 +10147,37 @@
       <c r="E4" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <f ca="1">SUMIFS('Engines indvidual'!F$1:F$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B4,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D4)*0.000001</f>
         <v>12.198228833399719</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$1:G$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B4,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D4)*0.000001</f>
         <v>3.679393801285766E-3</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$1:H$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B4,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D4)*0.000001</f>
         <v>9.0082507907532303</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$1:I$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B4,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D4)*0.000001</f>
         <v>1.0227721315962379</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$1:J$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B4,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D4)*0.000001</f>
         <v>2.1635265172489788</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$1:K$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B4,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D4)*0.000001</f>
         <v>4.4756902797934401</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$1:L$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B4,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D4)*0.000001</f>
         <v>5.0793506648311197</v>
       </c>
-      <c r="M4" s="4">
+      <c r="M4" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$1:M$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B4,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D4)*0.000001</f>
-        <v>2.6431878887751417</v>
+        <v>2.6431878887751425</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -10196,35 +10196,35 @@
       <c r="E5" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <f ca="1">SUMIFS('Engines indvidual'!F$1:F$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B5,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D5)*0.000001</f>
         <v>11.040106573366259</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$1:G$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B5,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D5)*0.000001</f>
         <v>3.5746950898187537E-3</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$1:H$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B5,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D5)*0.000001</f>
         <v>8.1439778681534492</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$1:I$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B5,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D5)*0.000001</f>
         <v>0.93224761761628394</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$1:J$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B5,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D5)*0.000001</f>
         <v>1.960306392506687</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$1:K$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B5,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D5)*0.000001</f>
         <v>4.0194507217505793</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$1:L$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B5,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D5)*0.000001</f>
         <v>4.6194418340471692</v>
       </c>
-      <c r="M5" s="4">
+      <c r="M5" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$1:M$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B5,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D5)*0.000001</f>
         <v>2.4012140175684848</v>
       </c>
@@ -10245,35 +10245,35 @@
       <c r="E6" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <f ca="1">SUMIFS('Engines indvidual'!F$1:F$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B6,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D6)*0.000001</f>
-        <v>20.160474022235952</v>
-      </c>
-      <c r="G6" s="4">
+        <v>20.16047402223596</v>
+      </c>
+      <c r="G6" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$1:G$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B6,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D6)*0.000001</f>
         <v>6.0276289007896904E-3</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$1:H$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B6,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D6)*0.000001</f>
         <v>15.28748599812274</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$1:I$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B6,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D6)*0.000001</f>
         <v>1.6594663559578018</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$1:J$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B6,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D6)*0.000001</f>
-        <v>3.2074940392546409</v>
-      </c>
-      <c r="K6" s="4">
+        <v>3.2074940392546418</v>
+      </c>
+      <c r="K6" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$1:K$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B6,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D6)*0.000001</f>
         <v>7.5394231847760791</v>
       </c>
-      <c r="L6" s="4">
+      <c r="L6" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$1:L$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B6,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D6)*0.000001</f>
         <v>8.5227643390825492</v>
       </c>
-      <c r="M6" s="4">
+      <c r="M6" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$1:M$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B6,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D6)*0.000001</f>
         <v>4.0982864983773073</v>
       </c>
@@ -10294,35 +10294,35 @@
       <c r="E7" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <f ca="1">SUMIFS('Engines indvidual'!F$1:F$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B7,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D7)*0.000001</f>
         <v>55.911030650748593</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$1:G$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B7,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D7)*0.000001</f>
         <v>3.6645310122340895E-2</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$1:H$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B7,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D7)*0.000001</f>
         <v>43.951247622512795</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$1:I$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B7,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D7)*0.000001</f>
         <v>4.8386222968817298</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$1:J$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B7,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D7)*0.000001</f>
-        <v>7.0845154212317896</v>
-      </c>
-      <c r="K7" s="4">
+        <v>7.0845154212318002</v>
+      </c>
+      <c r="K7" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$1:K$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B7,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D7)*0.000001</f>
-        <v>22.176646742267572</v>
-      </c>
-      <c r="L7" s="4">
+        <v>22.176646742267582</v>
+      </c>
+      <c r="L7" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$1:L$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B7,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D7)*0.000001</f>
         <v>23.407681014971686</v>
       </c>
-      <c r="M7" s="4">
+      <c r="M7" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$1:M$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B7,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D7)*0.000001</f>
         <v>10.326702893509498</v>
       </c>
@@ -10343,37 +10343,37 @@
       <c r="E8" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
         <f ca="1">SUMIFS('Engines indvidual'!F$1:F$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B8,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D8)*0.000001</f>
-        <v>15.445539722999669</v>
-      </c>
-      <c r="G8" s="4">
+        <v>15.445539722999658</v>
+      </c>
+      <c r="G8" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$1:G$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B8,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D8)*0.000001</f>
-        <v>1.3902856013831649E-2</v>
-      </c>
-      <c r="H8" s="4">
+        <v>1.390285601383166E-2</v>
+      </c>
+      <c r="H8" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$1:H$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B8,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D8)*0.000001</f>
         <v>12.620583332967549</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$1:I$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B8,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D8)*0.000001</f>
         <v>1.352791544803575</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J8" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$1:J$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B8,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D8)*0.000001</f>
         <v>1.458261989214692</v>
       </c>
-      <c r="K8" s="4">
+      <c r="K8" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$1:K$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B8,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D8)*0.000001</f>
-        <v>6.6053954754219593</v>
-      </c>
-      <c r="L8" s="4">
+        <v>6.6053954754219495</v>
+      </c>
+      <c r="L8" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$1:L$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B8,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D8)*0.000001</f>
         <v>6.3201275376589088</v>
       </c>
-      <c r="M8" s="4">
+      <c r="M8" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$1:M$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B8,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D8)*0.000001</f>
-        <v>2.5200167099187598</v>
+        <v>2.52001670991877</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -10392,37 +10392,37 @@
       <c r="E9" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="2">
         <f ca="1">SUMIFS('Engines indvidual'!F$1:F$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B9,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D9)*0.000001</f>
-        <v>0.80923977701977601</v>
-      </c>
-      <c r="G9" s="4">
+        <v>0.80923977701977401</v>
+      </c>
+      <c r="G9" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$1:G$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B9,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D9)*0.000001</f>
-        <v>6.4688468191441493E-4</v>
-      </c>
-      <c r="H9" s="4">
+        <v>6.4688468191441298E-4</v>
+      </c>
+      <c r="H9" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$1:H$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B9,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D9)*0.000001</f>
-        <v>0.65301080262627098</v>
-      </c>
-      <c r="I9" s="4">
+        <v>0.65301080262626887</v>
+      </c>
+      <c r="I9" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$1:I$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B9,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D9)*0.000001</f>
-        <v>6.8916206341175693E-2</v>
-      </c>
-      <c r="J9" s="4">
+        <v>6.8916206341175484E-2</v>
+      </c>
+      <c r="J9" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$1:J$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B9,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D9)*0.000001</f>
-        <v>8.6665883370414407E-2</v>
-      </c>
-      <c r="K9" s="4">
+        <v>8.6665883370413907E-2</v>
+      </c>
+      <c r="K9" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$1:K$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B9,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D9)*0.000001</f>
-        <v>0.3407418435287462</v>
-      </c>
-      <c r="L9" s="4">
+        <v>0.34074184352874498</v>
+      </c>
+      <c r="L9" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$1:L$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B9,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D9)*0.000001</f>
-        <v>0.33791515878996647</v>
-      </c>
-      <c r="M9" s="4">
+        <v>0.3379151587899652</v>
+      </c>
+      <c r="M9" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$1:M$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B9,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D9)*0.000001</f>
-        <v>0.1305827747010643</v>
+        <v>0.13058277470106389</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -10441,37 +10441,37 @@
       <c r="E10" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="2">
         <f ca="1">SUMIFS('Engines indvidual'!F$1:F$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B10,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D10)*0.000001</f>
         <v>17.439247824180359</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$1:G$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B10,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D10)*0.000001</f>
         <v>4.3218348741539282E-3</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$1:H$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B10,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D10)*0.000001</f>
         <v>13.178877246739969</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$1:I$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B10,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D10)*0.000001</f>
-        <v>1.4253570965813069</v>
-      </c>
-      <c r="J10" s="4">
+        <v>1.425357096581308</v>
+      </c>
+      <c r="J10" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$1:J$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B10,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D10)*0.000001</f>
-        <v>2.8306916459849107</v>
-      </c>
-      <c r="K10" s="4">
+        <v>2.8306916459849121</v>
+      </c>
+      <c r="K10" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$1:K$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B10,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D10)*0.000001</f>
         <v>6.5568994212321599</v>
       </c>
-      <c r="L10" s="4">
+      <c r="L10" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$1:L$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B10,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D10)*0.000001</f>
         <v>7.3234366661389894</v>
       </c>
-      <c r="M10" s="4">
+      <c r="M10" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$1:M$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B10,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D10)*0.000001</f>
-        <v>3.5589117368091929</v>
+        <v>3.5589117368091947</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -10490,35 +10490,35 @@
       <c r="E11" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="2">
         <f ca="1">SUMIFS('Engines indvidual'!F$1:F$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B11,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D11)*0.000001</f>
-        <v>3.7999353905927191</v>
-      </c>
-      <c r="G11" s="4">
+        <v>3.79993539059272</v>
+      </c>
+      <c r="G11" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$1:G$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B11,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D11)*0.000001</f>
         <v>6.4244107286816213E-4</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$1:H$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B11,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D11)*0.000001</f>
-        <v>3.2464810197964136</v>
-      </c>
-      <c r="I11" s="4">
+        <v>3.2464810197964162</v>
+      </c>
+      <c r="I11" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$1:I$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B11,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D11)*0.000001</f>
-        <v>0.27731793883793843</v>
-      </c>
-      <c r="J11" s="4">
+        <v>0.2773179388379387</v>
+      </c>
+      <c r="J11" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$1:J$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B11,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D11)*0.000001</f>
-        <v>0.2754939908855033</v>
-      </c>
-      <c r="K11" s="4">
+        <v>0.27549399088550397</v>
+      </c>
+      <c r="K11" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$1:K$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B11,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D11)*0.000001</f>
-        <v>1.5805232440268437</v>
-      </c>
-      <c r="L11" s="4">
+        <v>1.5805232440268449</v>
+      </c>
+      <c r="L11" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$1:L$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B11,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D11)*0.000001</f>
-        <v>1.6972708199581121</v>
-      </c>
-      <c r="M11" s="4">
+        <v>1.697270819958113</v>
+      </c>
+      <c r="M11" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$1:M$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B11,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D11)*0.000001</f>
         <v>0.52214132660776491</v>
       </c>
@@ -10539,37 +10539,37 @@
       <c r="E12" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="2">
         <f ca="1">SUMIFS('Engines indvidual'!F$1:F$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B12,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D12)*0.000001</f>
         <v>1.4410836001879008</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$1:G$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B12,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D12)*0.000001</f>
         <v>0</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$1:H$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B12,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D12)*0.000001</f>
         <v>0.92414543619034062</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$1:I$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B12,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D12)*0.000001</f>
         <v>0.12526702614712898</v>
       </c>
-      <c r="J12" s="4">
+      <c r="J12" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$1:J$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B12,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D12)*0.000001</f>
         <v>0.3916711378504289</v>
       </c>
-      <c r="K12" s="4">
+      <c r="K12" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$1:K$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B12,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D12)*0.000001</f>
         <v>0.50068589741185954</v>
       </c>
-      <c r="L12" s="4">
+      <c r="L12" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$1:L$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B12,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D12)*0.000001</f>
         <v>0.5468151813497597</v>
       </c>
-      <c r="M12" s="4">
+      <c r="M12" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$1:M$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B12,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D12)*0.000001</f>
-        <v>0.39358252142628697</v>
+        <v>0.39358252142628608</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -10588,37 +10588,37 @@
       <c r="E13" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="2">
         <f ca="1">SUMIFS('Engines indvidual'!F$1:F$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B13,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D13)*0.000001</f>
         <v>1.1581222600334597</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$1:G$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B13,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D13)*0.000001</f>
         <v>1.0469871146701222E-4</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H13" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$1:H$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B13,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D13)*0.000001</f>
         <v>0.86427292259977961</v>
       </c>
-      <c r="I13" s="4">
+      <c r="I13" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$1:I$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B13,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D13)*0.000001</f>
         <v>9.0524513979953966E-2</v>
       </c>
-      <c r="J13" s="4">
+      <c r="J13" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$1:J$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B13,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D13)*0.000001</f>
         <v>0.20322012474229192</v>
       </c>
-      <c r="K13" s="4">
+      <c r="K13" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$1:K$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B13,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D13)*0.000001</f>
         <v>0.4562395580428602</v>
       </c>
-      <c r="L13" s="4">
+      <c r="L13" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$1:L$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B13,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D13)*0.000001</f>
         <v>0.4599088307839499</v>
       </c>
-      <c r="M13" s="4">
+      <c r="M13" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$1:M$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B13,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D13)*0.000001</f>
-        <v>0.24197387120665703</v>
+        <v>0.24197387120665795</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -10637,35 +10637,35 @@
       <c r="E14" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="2">
         <f ca="1">SUMIFS('Engines indvidual'!F$1:F$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B14,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D14)*0.000001</f>
         <v>4.1823320352104592</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$1:G$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B14,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D14)*0.000001</f>
         <v>1.1291328671038299E-2</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H14" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$1:H$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B14,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D14)*0.000001</f>
         <v>3.4417821278516798</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I14" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$1:I$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B14,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D14)*0.000001</f>
         <v>0.44310532453040291</v>
       </c>
-      <c r="J14" s="4">
+      <c r="J14" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$1:J$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B14,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D14)*0.000001</f>
         <v>0.28615325415735399</v>
       </c>
-      <c r="K14" s="4">
+      <c r="K14" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$1:K$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B14,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D14)*0.000001</f>
         <v>1.8598148184418097</v>
       </c>
-      <c r="L14" s="4">
+      <c r="L14" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$1:L$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B14,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D14)*0.000001</f>
         <v>1.7576341160035802</v>
       </c>
-      <c r="M14" s="4">
+      <c r="M14" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$1:M$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B14,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D14)*0.000001</f>
         <v>0.56488310076506898</v>
       </c>
@@ -10686,35 +10686,35 @@
       <c r="E15" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="2">
         <f ca="1">SUMIFS('Engines indvidual'!F$1:F$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B15,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D15)*0.000001</f>
-        <v>8.1259232912256909</v>
-      </c>
-      <c r="G15" s="4">
+        <v>8.1259232912256785</v>
+      </c>
+      <c r="G15" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$1:G$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B15,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D15)*0.000001</f>
         <v>2.2322974530833511E-2</v>
       </c>
-      <c r="H15" s="4">
+      <c r="H15" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$1:H$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B15,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D15)*0.000001</f>
         <v>6.6596411762525296</v>
       </c>
-      <c r="I15" s="4">
+      <c r="I15" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$1:I$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B15,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D15)*0.000001</f>
         <v>0.87944958405774687</v>
       </c>
-      <c r="J15" s="4">
+      <c r="J15" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$1:J$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B15,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D15)*0.000001</f>
         <v>0.56450955638455291</v>
       </c>
-      <c r="K15" s="4">
+      <c r="K15" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$1:K$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B15,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D15)*0.000001</f>
         <v>3.4243016210753079</v>
       </c>
-      <c r="L15" s="4">
+      <c r="L15" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$1:L$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B15,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D15)*0.000001</f>
-        <v>3.5135599195541181</v>
-      </c>
-      <c r="M15" s="4">
+        <v>3.5135599195541172</v>
+      </c>
+      <c r="M15" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$1:M$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B15,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D15)*0.000001</f>
         <v>1.188061750596257</v>
       </c>
@@ -10735,35 +10735,35 @@
       <c r="E16" t="s">
         <v>14</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="2">
         <f ca="1">SUMIFS('Engines indvidual'!F$1:F$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B16,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D16)*0.000001</f>
-        <v>8.1259232912256909</v>
-      </c>
-      <c r="G16" s="4">
+        <v>8.1259232912256785</v>
+      </c>
+      <c r="G16" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$1:G$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B16,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D16)*0.000001</f>
         <v>2.2322974530833511E-2</v>
       </c>
-      <c r="H16" s="4">
+      <c r="H16" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$1:H$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B16,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D16)*0.000001</f>
         <v>6.6596411762525296</v>
       </c>
-      <c r="I16" s="4">
+      <c r="I16" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$1:I$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B16,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D16)*0.000001</f>
         <v>0.87944958405774687</v>
       </c>
-      <c r="J16" s="4">
+      <c r="J16" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$1:J$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B16,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D16)*0.000001</f>
         <v>0.56450955638455291</v>
       </c>
-      <c r="K16" s="4">
+      <c r="K16" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$1:K$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B16,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D16)*0.000001</f>
         <v>3.4243016210753079</v>
       </c>
-      <c r="L16" s="4">
+      <c r="L16" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$1:L$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B16,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D16)*0.000001</f>
-        <v>3.5135599195541181</v>
-      </c>
-      <c r="M16" s="4">
+        <v>3.5135599195541172</v>
+      </c>
+      <c r="M16" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$1:M$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B16,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D16)*0.000001</f>
         <v>1.188061750596257</v>
       </c>
@@ -10784,35 +10784,35 @@
       <c r="E17" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17" s="2">
         <f ca="1">SUMIFS('Engines indvidual'!F$1:F$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B17,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D17)*0.000001</f>
         <v>4.1823320352104592</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$1:G$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B17,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D17)*0.000001</f>
         <v>1.1291328671038299E-2</v>
       </c>
-      <c r="H17" s="4">
+      <c r="H17" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$1:H$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B17,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D17)*0.000001</f>
         <v>3.4417821278516798</v>
       </c>
-      <c r="I17" s="4">
+      <c r="I17" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$1:I$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B17,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D17)*0.000001</f>
         <v>0.44310532453040291</v>
       </c>
-      <c r="J17" s="4">
+      <c r="J17" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$1:J$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B17,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D17)*0.000001</f>
         <v>0.28615325415735399</v>
       </c>
-      <c r="K17" s="4">
+      <c r="K17" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$1:K$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B17,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D17)*0.000001</f>
         <v>1.8598148184418097</v>
       </c>
-      <c r="L17" s="4">
+      <c r="L17" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$1:L$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B17,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D17)*0.000001</f>
         <v>1.7576341160035802</v>
       </c>
-      <c r="M17" s="4">
+      <c r="M17" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$1:M$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B17,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D17)*0.000001</f>
         <v>0.56488310076506898</v>
       </c>
@@ -10833,35 +10833,35 @@
       <c r="E18" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18" s="2">
         <f ca="1">SUMIFS('Engines indvidual'!F$1:F$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B18,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D18)*0.000001</f>
         <v>0.63345057197239685</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$1:G$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B18,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D18)*0.000001</f>
         <v>1.6954033130108512E-3</v>
       </c>
-      <c r="H18" s="4">
+      <c r="H18" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$1:H$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B18,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D18)*0.000001</f>
         <v>0.52506213237605304</v>
       </c>
-      <c r="I18" s="4">
+      <c r="I18" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$1:I$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B18,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D18)*0.000001</f>
         <v>6.7168086842310695E-2</v>
       </c>
-      <c r="J18" s="4">
+      <c r="J18" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$1:J$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B18,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D18)*0.000001</f>
         <v>3.9524949441020023E-2</v>
       </c>
-      <c r="K18" s="4">
+      <c r="K18" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$1:K$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B18,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D18)*0.000001</f>
         <v>0.27486381354582634</v>
       </c>
-      <c r="L18" s="4">
+      <c r="L18" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$1:L$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B18,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D18)*0.000001</f>
         <v>0.27107131412870117</v>
       </c>
-      <c r="M18" s="4">
+      <c r="M18" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$1:M$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B18,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D18)*0.000001</f>
         <v>8.7515444297869394E-2</v>
       </c>
@@ -10882,37 +10882,37 @@
       <c r="E19" t="s">
         <v>14</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19" s="2">
         <f ca="1">SUMIFS('Engines indvidual'!F$1:F$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B19,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D19)*0.000001</f>
-        <v>6.7558857411468685</v>
-      </c>
-      <c r="G19" s="4">
+        <v>6.7558857411468587</v>
+      </c>
+      <c r="G19" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$1:G$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B19,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D19)*0.000001</f>
-        <v>8.2836082274089697E-3</v>
-      </c>
-      <c r="H19" s="4">
+        <v>8.2836082274089784E-3</v>
+      </c>
+      <c r="H19" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$1:H$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B19,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D19)*0.000001</f>
-        <v>5.6220287798171897</v>
-      </c>
-      <c r="I19" s="4">
+        <v>5.62202877981718</v>
+      </c>
+      <c r="I19" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$1:I$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B19,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D19)*0.000001</f>
         <v>0.62805092498667214</v>
       </c>
-      <c r="J19" s="4">
+      <c r="J19" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$1:J$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B19,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D19)*0.000001</f>
-        <v>0.49752242811557301</v>
-      </c>
-      <c r="K19" s="4">
+        <v>0.49752242811557201</v>
+      </c>
+      <c r="K19" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$1:K$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B19,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D19)*0.000001</f>
-        <v>3.0150875435358202</v>
-      </c>
-      <c r="L19" s="4">
+        <v>3.01508754353581</v>
+      </c>
+      <c r="L19" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$1:L$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B19,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D19)*0.000001</f>
-        <v>2.6768796518730498</v>
-      </c>
-      <c r="M19" s="4">
+        <v>2.6768796518730595</v>
+      </c>
+      <c r="M19" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$1:M$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B19,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D19)*0.000001</f>
-        <v>1.0639185457379492</v>
+        <v>1.0639185457379581</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -10931,37 +10931,37 @@
       <c r="E20" t="s">
         <v>7</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20" s="2">
         <f ca="1">SUMIFS('Engines indvidual'!F$1:F$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B20,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D20)*0.000001</f>
         <v>8.6896539818527998</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$1:G$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B20,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D20)*0.000001</f>
         <v>5.6192477864226804E-3</v>
       </c>
-      <c r="H20" s="4">
+      <c r="H20" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$1:H$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B20,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D20)*0.000001</f>
-        <v>6.9985545531503588</v>
-      </c>
-      <c r="I20" s="4">
+        <v>6.9985545531503695</v>
+      </c>
+      <c r="I20" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$1:I$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B20,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D20)*0.000001</f>
         <v>0.72474061981690296</v>
       </c>
-      <c r="J20" s="4">
+      <c r="J20" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$1:J$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B20,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D20)*0.000001</f>
-        <v>0.96073956109911895</v>
-      </c>
-      <c r="K20" s="4">
+        <v>0.96073956109911995</v>
+      </c>
+      <c r="K20" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$1:K$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B20,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D20)*0.000001</f>
         <v>3.5903079318861399</v>
       </c>
-      <c r="L20" s="4">
+      <c r="L20" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$1:L$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B20,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D20)*0.000001</f>
-        <v>3.6432478857858599</v>
-      </c>
-      <c r="M20" s="4">
+        <v>3.6432478857858497</v>
+      </c>
+      <c r="M20" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$1:M$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B20,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D20)*0.000001</f>
-        <v>1.4560981641808111</v>
+        <v>1.4560981641808119</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -10980,35 +10980,35 @@
       <c r="E21" t="s">
         <v>12</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F21" s="2">
         <f ca="1">SUMIFS('Engines indvidual'!F$1:F$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B21,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D21)*0.000001</f>
         <v>107.3860783611231</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G21" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$1:G$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B21,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D21)*0.000001</f>
         <v>0.14080811555711298</v>
       </c>
-      <c r="H21" s="4">
+      <c r="H21" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$1:H$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B21,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D21)*0.000001</f>
         <v>85.15762600797359</v>
       </c>
-      <c r="I21" s="4">
+      <c r="I21" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$1:I$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B21,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D21)*0.000001</f>
         <v>10.14086317310241</v>
       </c>
-      <c r="J21" s="4">
+      <c r="J21" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$1:J$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B21,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D21)*0.000001</f>
         <v>11.946781064489919</v>
       </c>
-      <c r="K21" s="4">
+      <c r="K21" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$1:K$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B21,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D21)*0.000001</f>
         <v>42.237598987237305</v>
       </c>
-      <c r="L21" s="4">
+      <c r="L21" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$1:L$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B21,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D21)*0.000001</f>
         <v>45.915966443070204</v>
       </c>
-      <c r="M21" s="4">
+      <c r="M21" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$1:M$77,'Engines indvidual'!$B$1:$B$77,'Full system - simplified'!$B21,'Engines indvidual'!$D$1:$D$77,'Full system - simplified'!$D21)*0.000001</f>
         <v>19.232512930815332</v>
       </c>
@@ -11029,35 +11029,35 @@
       <c r="E23" t="s">
         <v>7</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F23" s="2">
         <f ca="1">SUMIFS('Engines indvidual'!F$79:F$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B23,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D23)*0.000001</f>
         <v>5.3390023466401496E-3</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G23" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$79:G$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B23,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D23)*0.000001</f>
         <v>1.7647518533353628E-3</v>
       </c>
-      <c r="H23" s="4">
+      <c r="H23" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$79:H$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B23,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D23)*0.000001</f>
         <v>2.8592053696498703E-3</v>
       </c>
-      <c r="I23" s="4">
+      <c r="I23" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$79:I$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B23,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D23)*0.000001</f>
         <v>6.2470588714104598E-4</v>
       </c>
-      <c r="J23" s="4">
+      <c r="J23" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$79:J$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B23,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D23)*0.000001</f>
         <v>9.033923651389685E-5</v>
       </c>
-      <c r="K23" s="4">
+      <c r="K23" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$79:K$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B23,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D23)*0.000001</f>
         <v>3.1690637449949067E-3</v>
       </c>
-      <c r="L23" s="4">
+      <c r="L23" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$79:L$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B23,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D23)*0.000001</f>
         <v>1.321796824874261E-3</v>
       </c>
-      <c r="M23" s="4">
+      <c r="M23" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$79:M$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B23,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D23)*0.000001</f>
         <v>8.4814177677100988E-4</v>
       </c>
@@ -11078,35 +11078,35 @@
       <c r="E24" t="s">
         <v>7</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F24" s="2">
         <f ca="1">SUMIFS('Engines indvidual'!F$79:F$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B24,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D24)*0.000001</f>
         <v>7.9139880154120394</v>
       </c>
-      <c r="G24" s="4">
+      <c r="G24" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$79:G$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B24,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D24)*0.000001</f>
         <v>2.9596816149046283</v>
       </c>
-      <c r="H24" s="4">
+      <c r="H24" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$79:H$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B24,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D24)*0.000001</f>
         <v>4.0076953078316215</v>
       </c>
-      <c r="I24" s="4">
+      <c r="I24" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$79:I$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B24,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D24)*0.000001</f>
         <v>0.65899314144736187</v>
       </c>
-      <c r="J24" s="4">
+      <c r="J24" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$79:J$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B24,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D24)*0.000001</f>
         <v>0.2876179512284277</v>
       </c>
-      <c r="K24" s="4">
+      <c r="K24" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$79:K$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B24,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D24)*0.000001</f>
         <v>3.391627075330137</v>
       </c>
-      <c r="L24" s="4">
+      <c r="L24" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$79:L$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B24,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D24)*0.000001</f>
         <v>3.0905017728267912</v>
       </c>
-      <c r="M24" s="4">
+      <c r="M24" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$79:M$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B24,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D24)*0.000001</f>
         <v>1.4318591672551058</v>
       </c>
@@ -11127,35 +11127,35 @@
       <c r="E25" t="s">
         <v>7</v>
       </c>
-      <c r="F25" s="3">
+      <c r="F25" s="2">
         <f ca="1">SUMIFS('Engines indvidual'!F$79:F$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B25,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D25)*0.000001</f>
         <v>7.6539575759840881</v>
       </c>
-      <c r="G25" s="4">
+      <c r="G25" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$79:G$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B25,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D25)*0.000001</f>
         <v>2.8347460668352746</v>
       </c>
-      <c r="H25" s="4">
+      <c r="H25" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$79:H$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B25,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D25)*0.000001</f>
         <v>3.9061504056598988</v>
       </c>
-      <c r="I25" s="4">
+      <c r="I25" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$79:I$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B25,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D25)*0.000001</f>
         <v>0.64382031033245068</v>
       </c>
-      <c r="J25" s="4">
+      <c r="J25" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$79:J$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B25,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D25)*0.000001</f>
         <v>0.26924079315646982</v>
       </c>
-      <c r="K25" s="4">
+      <c r="K25" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$79:K$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B25,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D25)*0.000001</f>
         <v>3.3020865868830103</v>
       </c>
-      <c r="L25" s="4">
+      <c r="L25" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$79:L$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B25,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D25)*0.000001</f>
         <v>3.0169168224492449</v>
       </c>
-      <c r="M25" s="4">
+      <c r="M25" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$79:M$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B25,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D25)*0.000001</f>
         <v>1.3349541666518501</v>
       </c>
@@ -11176,35 +11176,35 @@
       <c r="E26" t="s">
         <v>7</v>
       </c>
-      <c r="F26" s="3">
+      <c r="F26" s="2">
         <f ca="1">SUMIFS('Engines indvidual'!F$79:F$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B26,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D26)*0.000001</f>
         <v>7.0942529442990301</v>
       </c>
-      <c r="G26" s="4">
+      <c r="G26" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$79:G$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B26,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D26)*0.000001</f>
         <v>2.5893737025639694</v>
       </c>
-      <c r="H26" s="4">
+      <c r="H26" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$79:H$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B26,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D26)*0.000001</f>
         <v>3.6503214177712899</v>
       </c>
-      <c r="I26" s="4">
+      <c r="I26" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$79:I$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B26,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D26)*0.000001</f>
         <v>0.60642866725531253</v>
       </c>
-      <c r="J26" s="4">
+      <c r="J26" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$79:J$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B26,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D26)*0.000001</f>
         <v>0.24812915670846236</v>
       </c>
-      <c r="K26" s="4">
+      <c r="K26" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$79:K$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B26,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D26)*0.000001</f>
         <v>3.0658590862675781</v>
       </c>
-      <c r="L26" s="4">
+      <c r="L26" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$79:L$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B26,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D26)*0.000001</f>
         <v>2.8015818906107328</v>
       </c>
-      <c r="M26" s="4">
+      <c r="M26" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$79:M$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B26,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D26)*0.000001</f>
         <v>1.226811967420731</v>
       </c>
@@ -11225,35 +11225,35 @@
       <c r="E27" t="s">
         <v>12</v>
       </c>
-      <c r="F27" s="3">
+      <c r="F27" s="2">
         <f ca="1">SUMIFS('Engines indvidual'!F$79:F$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B27,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D27)*0.000001</f>
         <v>9.5364176727926981</v>
       </c>
-      <c r="G27" s="4">
+      <c r="G27" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$79:G$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B27,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D27)*0.000001</f>
         <v>3.5039868770766796</v>
       </c>
-      <c r="H27" s="4">
+      <c r="H27" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$79:H$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B27,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D27)*0.000001</f>
         <v>4.8533039514378622</v>
       </c>
-      <c r="I27" s="4">
+      <c r="I27" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$79:I$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B27,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D27)*0.000001</f>
         <v>0.84098554290987837</v>
       </c>
-      <c r="J27" s="4">
+      <c r="J27" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$79:J$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B27,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D27)*0.000001</f>
         <v>0.33814130136827431</v>
       </c>
-      <c r="K27" s="4">
+      <c r="K27" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$79:K$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B27,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D27)*0.000001</f>
         <v>4.0872284832192607</v>
       </c>
-      <c r="L27" s="4">
+      <c r="L27" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$79:L$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B27,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D27)*0.000001</f>
         <v>3.7618290347118957</v>
       </c>
-      <c r="M27" s="4">
+      <c r="M27" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$79:M$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B27,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D27)*0.000001</f>
         <v>1.6873601548615587</v>
       </c>
@@ -11274,35 +11274,35 @@
       <c r="E28" t="s">
         <v>7</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F28" s="2">
         <f ca="1">SUMIFS('Engines indvidual'!F$79:F$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B28,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D28)*0.000001</f>
         <v>36.262821022740511</v>
       </c>
-      <c r="G28" s="4">
+      <c r="G28" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$79:G$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B28,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D28)*0.000001</f>
         <v>11.77607902491666</v>
       </c>
-      <c r="H28" s="4">
+      <c r="H28" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$79:H$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B28,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D28)*0.000001</f>
         <v>19.814986182287427</v>
       </c>
-      <c r="I28" s="4">
+      <c r="I28" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$79:I$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B28,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D28)*0.000001</f>
         <v>3.5923805906475161</v>
       </c>
-      <c r="J28" s="4">
+      <c r="J28" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$79:J$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B28,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D28)*0.000001</f>
         <v>1.0793752248889839</v>
       </c>
-      <c r="K28" s="4">
+      <c r="K28" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$79:K$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B28,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D28)*0.000001</f>
         <v>15.70523713262302</v>
       </c>
-      <c r="L28" s="4">
+      <c r="L28" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$79:L$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B28,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D28)*0.000001</f>
         <v>14.96082523003734</v>
       </c>
-      <c r="M28" s="4">
+      <c r="M28" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$79:M$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B28,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D28)*0.000001</f>
         <v>5.5967586600801198</v>
       </c>
@@ -11323,37 +11323,37 @@
       <c r="E29" t="s">
         <v>7</v>
       </c>
-      <c r="F29" s="3">
-        <f>SUMIFS('Engines indvidual'!F$79:F$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B29,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D29)*0.000001</f>
-        <v>0</v>
-      </c>
-      <c r="G29" s="4">
-        <f>SUMIFS('Engines indvidual'!G$79:G$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B29,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D29)*0.000001</f>
-        <v>0</v>
-      </c>
-      <c r="H29" s="4">
-        <f>SUMIFS('Engines indvidual'!H$79:H$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B29,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D29)*0.000001</f>
-        <v>0</v>
-      </c>
-      <c r="I29" s="4">
-        <f>SUMIFS('Engines indvidual'!I$79:I$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B29,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D29)*0.000001</f>
-        <v>0</v>
-      </c>
-      <c r="J29" s="4">
-        <f>SUMIFS('Engines indvidual'!J$79:J$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B29,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D29)*0.000001</f>
-        <v>0</v>
-      </c>
-      <c r="K29" s="4">
-        <f>SUMIFS('Engines indvidual'!K$79:K$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B29,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D29)*0.000001</f>
-        <v>0</v>
-      </c>
-      <c r="L29" s="4">
-        <f>SUMIFS('Engines indvidual'!L$79:L$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B29,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D29)*0.000001</f>
-        <v>0</v>
-      </c>
-      <c r="M29" s="4">
-        <f>SUMIFS('Engines indvidual'!M$79:M$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B29,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D29)*0.000001</f>
-        <v>0</v>
+      <c r="F29" s="2">
+        <f ca="1">SUMIFS('Engines indvidual'!F$79:F$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B29,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D29)*0.000001</f>
+        <v>21.042478099276252</v>
+      </c>
+      <c r="G29" s="3">
+        <f ca="1">SUMIFS('Engines indvidual'!G$79:G$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B29,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D29)*0.000001</f>
+        <v>6.3783446079999528</v>
+      </c>
+      <c r="H29" s="3">
+        <f ca="1">SUMIFS('Engines indvidual'!H$79:H$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B29,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D29)*0.000001</f>
+        <v>11.93621371945814</v>
+      </c>
+      <c r="I29" s="3">
+        <f ca="1">SUMIFS('Engines indvidual'!I$79:I$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B29,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D29)*0.000001</f>
+        <v>2.156508836437427</v>
+      </c>
+      <c r="J29" s="3">
+        <f ca="1">SUMIFS('Engines indvidual'!J$79:J$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B29,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D29)*0.000001</f>
+        <v>0.57141093538073773</v>
+      </c>
+      <c r="K29" s="3">
+        <f ca="1">SUMIFS('Engines indvidual'!K$79:K$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B29,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D29)*0.000001</f>
+        <v>9.1655041587943096</v>
+      </c>
+      <c r="L29" s="3">
+        <f ca="1">SUMIFS('Engines indvidual'!L$79:L$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B29,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D29)*0.000001</f>
+        <v>8.8659218308067711</v>
+      </c>
+      <c r="M29" s="3">
+        <f ca="1">SUMIFS('Engines indvidual'!M$79:M$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B29,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D29)*0.000001</f>
+        <v>3.0110521096751639</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -11372,37 +11372,37 @@
       <c r="E30" t="s">
         <v>14</v>
       </c>
-      <c r="F30" s="3">
+      <c r="F30" s="2">
         <f ca="1">SUMIFS('Engines indvidual'!F$79:F$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B30,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D30)*0.000001</f>
-        <v>3.0376943650396027</v>
-      </c>
-      <c r="G30" s="4">
+        <v>0.46280325141239226</v>
+      </c>
+      <c r="G30" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$79:G$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B30,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D30)*0.000001</f>
-        <v>1.0376833340281391</v>
-      </c>
-      <c r="H30" s="4">
+        <v>0.13173394659608048</v>
+      </c>
+      <c r="H30" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$79:H$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B30,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D30)*0.000001</f>
-        <v>1.5919257966912546</v>
-      </c>
-      <c r="I30" s="4">
+        <v>0.25937056143788328</v>
+      </c>
+      <c r="I30" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$79:I$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B30,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D30)*0.000001</f>
-        <v>0.31780358972901696</v>
-      </c>
-      <c r="J30" s="4">
+        <v>6.0169376848747298E-2</v>
+      </c>
+      <c r="J30" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$79:J$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B30,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D30)*0.000001</f>
-        <v>9.0281644591194768E-2</v>
-      </c>
-      <c r="K30" s="4">
+        <v>1.1529366529681392E-2</v>
+      </c>
+      <c r="K30" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$79:K$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B30,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D30)*0.000001</f>
-        <v>1.389493743944356</v>
-      </c>
-      <c r="L30" s="4">
+        <v>0.20909684040336357</v>
+      </c>
+      <c r="L30" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$79:L$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B30,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D30)*0.000001</f>
-        <v>1.1969854782300049</v>
-      </c>
-      <c r="M30" s="4">
+        <v>0.1941860788383083</v>
+      </c>
+      <c r="M30" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$79:M$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B30,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D30)*0.000001</f>
-        <v>0.45121514286524811</v>
+        <v>5.9520332170721404E-2</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -11421,35 +11421,35 @@
       <c r="E31" t="s">
         <v>7</v>
       </c>
-      <c r="F31" s="3">
+      <c r="F31" s="2">
         <f ca="1">SUMIFS('Engines indvidual'!F$79:F$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B31,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D31)*0.000001</f>
         <v>7.9139880154120394</v>
       </c>
-      <c r="G31" s="4">
+      <c r="G31" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$79:G$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B31,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D31)*0.000001</f>
         <v>2.9596816149046283</v>
       </c>
-      <c r="H31" s="4">
+      <c r="H31" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$79:H$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B31,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D31)*0.000001</f>
         <v>4.0076953078316215</v>
       </c>
-      <c r="I31" s="4">
+      <c r="I31" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$79:I$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B31,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D31)*0.000001</f>
         <v>0.65899314144736187</v>
       </c>
-      <c r="J31" s="4">
+      <c r="J31" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$79:J$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B31,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D31)*0.000001</f>
         <v>0.2876179512284277</v>
       </c>
-      <c r="K31" s="4">
+      <c r="K31" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$79:K$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B31,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D31)*0.000001</f>
         <v>3.391627075330137</v>
       </c>
-      <c r="L31" s="4">
+      <c r="L31" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$79:L$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B31,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D31)*0.000001</f>
         <v>3.0905017728267912</v>
       </c>
-      <c r="M31" s="4">
+      <c r="M31" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$79:M$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B31,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D31)*0.000001</f>
         <v>1.4318591672551058</v>
       </c>
@@ -11470,35 +11470,35 @@
       <c r="E32" t="s">
         <v>7</v>
       </c>
-      <c r="F32" s="3">
+      <c r="F32" s="2">
         <f ca="1">SUMIFS('Engines indvidual'!F$79:F$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B32,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D32)*0.000001</f>
         <v>0</v>
       </c>
-      <c r="G32" s="4">
+      <c r="G32" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$79:G$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B32,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D32)*0.000001</f>
         <v>0</v>
       </c>
-      <c r="H32" s="4">
+      <c r="H32" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$79:H$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B32,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D32)*0.000001</f>
         <v>0</v>
       </c>
-      <c r="I32" s="4">
+      <c r="I32" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$79:I$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B32,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D32)*0.000001</f>
         <v>0</v>
       </c>
-      <c r="J32" s="4">
+      <c r="J32" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$79:J$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B32,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D32)*0.000001</f>
         <v>0</v>
       </c>
-      <c r="K32" s="4">
+      <c r="K32" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$79:K$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B32,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D32)*0.000001</f>
         <v>0</v>
       </c>
-      <c r="L32" s="4">
+      <c r="L32" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$79:L$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B32,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D32)*0.000001</f>
         <v>0</v>
       </c>
-      <c r="M32" s="4">
+      <c r="M32" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$79:M$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B32,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D32)*0.000001</f>
         <v>0</v>
       </c>
@@ -11519,35 +11519,35 @@
       <c r="E33" t="s">
         <v>14</v>
       </c>
-      <c r="F33" s="3">
+      <c r="F33" s="2">
         <f ca="1">SUMIFS('Engines indvidual'!F$79:F$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B33,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D33)*0.000001</f>
         <v>0.26003043942794996</v>
       </c>
-      <c r="G33" s="4">
+      <c r="G33" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$79:G$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B33,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D33)*0.000001</f>
         <v>0.12493554806935403</v>
       </c>
-      <c r="H33" s="4">
+      <c r="H33" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$79:H$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B33,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D33)*0.000001</f>
         <v>0.10154490217172224</v>
       </c>
-      <c r="I33" s="4">
+      <c r="I33" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$79:I$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B33,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D33)*0.000001</f>
         <v>1.5172831114911196E-2</v>
       </c>
-      <c r="J33" s="4">
+      <c r="J33" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$79:J$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B33,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D33)*0.000001</f>
         <v>1.8377158071957826E-2</v>
       </c>
-      <c r="K33" s="4">
+      <c r="K33" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$79:K$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B33,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D33)*0.000001</f>
         <v>8.9540488447126754E-2</v>
       </c>
-      <c r="L33" s="4">
+      <c r="L33" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$79:L$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B33,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D33)*0.000001</f>
         <v>7.3584950377546129E-2</v>
       </c>
-      <c r="M33" s="4">
+      <c r="M33" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$79:M$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B33,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D33)*0.000001</f>
         <v>9.6905000603255992E-2</v>
       </c>
@@ -11568,35 +11568,35 @@
       <c r="E34" t="s">
         <v>14</v>
       </c>
-      <c r="F34" s="3">
+      <c r="F34" s="2">
         <f ca="1">SUMIFS('Engines indvidual'!F$79:F$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B34,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D34)*0.000001</f>
         <v>0.55970463168505968</v>
       </c>
-      <c r="G34" s="4">
+      <c r="G34" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$79:G$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B34,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D34)*0.000001</f>
         <v>0.24537236427130607</v>
       </c>
-      <c r="H34" s="4">
+      <c r="H34" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$79:H$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B34,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D34)*0.000001</f>
         <v>0.25582898788860914</v>
       </c>
-      <c r="I34" s="4">
+      <c r="I34" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$79:I$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B34,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D34)*0.000001</f>
         <v>3.7391643077138187E-2</v>
       </c>
-      <c r="J34" s="4">
+      <c r="J34" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$79:J$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B34,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D34)*0.000001</f>
         <v>2.1111636448007485E-2</v>
       </c>
-      <c r="K34" s="4">
+      <c r="K34" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$79:K$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B34,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D34)*0.000001</f>
         <v>0.23622750061543205</v>
       </c>
-      <c r="L34" s="4">
+      <c r="L34" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$79:L$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B34,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D34)*0.000001</f>
         <v>0.21533493183851207</v>
       </c>
-      <c r="M34" s="4">
+      <c r="M34" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$79:M$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B34,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D34)*0.000001</f>
         <v>0.10814219923111901</v>
       </c>
@@ -11617,35 +11617,35 @@
       <c r="E35" t="s">
         <v>14</v>
       </c>
-      <c r="F35" s="3">
+      <c r="F35" s="2">
         <f ca="1">SUMIFS('Engines indvidual'!F$79:F$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B35,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D35)*0.000001</f>
         <v>3.1373384055217297</v>
       </c>
-      <c r="G35" s="4">
+      <c r="G35" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$79:G$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B35,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D35)*0.000001</f>
         <v>0.96147420231622294</v>
       </c>
-      <c r="H35" s="4">
+      <c r="H35" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$79:H$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B35,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D35)*0.000001</f>
         <v>1.756744755703155</v>
       </c>
-      <c r="I35" s="4">
+      <c r="I35" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$79:I$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B35,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D35)*0.000001</f>
         <v>0.34421383763347191</v>
       </c>
-      <c r="J35" s="4">
+      <c r="J35" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$79:J$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B35,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D35)*0.000001</f>
         <v>7.4905609868858525E-2</v>
       </c>
-      <c r="K35" s="4">
+      <c r="K35" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$79:K$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B35,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D35)*0.000001</f>
         <v>1.4758357184061859</v>
       </c>
-      <c r="L35" s="4">
+      <c r="L35" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$79:L$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B35,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D35)*0.000001</f>
         <v>1.2745873020685159</v>
       </c>
-      <c r="M35" s="4">
+      <c r="M35" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$79:M$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B35,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D35)*0.000001</f>
         <v>0.38691538504700607</v>
       </c>
@@ -11666,35 +11666,35 @@
       <c r="E36" t="s">
         <v>14</v>
       </c>
-      <c r="F36" s="3">
+      <c r="F36" s="2">
         <f ca="1">SUMIFS('Engines indvidual'!F$79:F$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B36,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D36)*0.000001</f>
         <v>5.8399909108127108</v>
       </c>
-      <c r="G36" s="4">
+      <c r="G36" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$79:G$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B36,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D36)*0.000001</f>
         <v>1.7713015248069959</v>
       </c>
-      <c r="H36" s="4">
+      <c r="H36" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$79:H$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B36,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D36)*0.000001</f>
         <v>3.2686799202521661</v>
       </c>
-      <c r="I36" s="4">
+      <c r="I36" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$79:I$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B36,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D36)*0.000001</f>
         <v>0.65631594983988406</v>
       </c>
-      <c r="J36" s="4">
+      <c r="J36" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$79:J$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B36,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D36)*0.000001</f>
         <v>0.1436935159136537</v>
       </c>
-      <c r="K36" s="4">
+      <c r="K36" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$79:K$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B36,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D36)*0.000001</f>
         <v>2.6080520744797098</v>
       </c>
-      <c r="L36" s="4">
+      <c r="L36" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$79:L$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B36,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D36)*0.000001</f>
         <v>2.4511736660152832</v>
       </c>
-      <c r="M36" s="4">
+      <c r="M36" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$79:M$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B36,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D36)*0.000001</f>
         <v>0.78076517031770287</v>
       </c>
@@ -11715,35 +11715,35 @@
       <c r="E37" t="s">
         <v>14</v>
       </c>
-      <c r="F37" s="3">
+      <c r="F37" s="2">
         <f ca="1">SUMIFS('Engines indvidual'!F$79:F$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B37,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D37)*0.000001</f>
         <v>5.8399909108127108</v>
       </c>
-      <c r="G37" s="4">
+      <c r="G37" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$79:G$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B37,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D37)*0.000001</f>
         <v>1.7713015248069959</v>
       </c>
-      <c r="H37" s="4">
+      <c r="H37" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$79:H$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B37,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D37)*0.000001</f>
         <v>3.2686799202521661</v>
       </c>
-      <c r="I37" s="4">
+      <c r="I37" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$79:I$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B37,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D37)*0.000001</f>
         <v>0.65631594983988406</v>
       </c>
-      <c r="J37" s="4">
+      <c r="J37" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$79:J$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B37,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D37)*0.000001</f>
         <v>0.1436935159136537</v>
       </c>
-      <c r="K37" s="4">
+      <c r="K37" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$79:K$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B37,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D37)*0.000001</f>
         <v>2.6080520744797098</v>
       </c>
-      <c r="L37" s="4">
+      <c r="L37" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$79:L$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B37,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D37)*0.000001</f>
         <v>2.4511736660152832</v>
       </c>
-      <c r="M37" s="4">
+      <c r="M37" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$79:M$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B37,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D37)*0.000001</f>
         <v>0.78076517031770287</v>
       </c>
@@ -11764,35 +11764,35 @@
       <c r="E38" t="s">
         <v>14</v>
       </c>
-      <c r="F38" s="3">
+      <c r="F38" s="2">
         <f ca="1">SUMIFS('Engines indvidual'!F$79:F$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B38,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D38)*0.000001</f>
         <v>3.1373384055217297</v>
       </c>
-      <c r="G38" s="4">
+      <c r="G38" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$79:G$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B38,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D38)*0.000001</f>
         <v>0.96147420231622294</v>
       </c>
-      <c r="H38" s="4">
+      <c r="H38" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$79:H$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B38,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D38)*0.000001</f>
         <v>1.756744755703155</v>
       </c>
-      <c r="I38" s="4">
+      <c r="I38" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$79:I$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B38,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D38)*0.000001</f>
         <v>0.34421383763347191</v>
       </c>
-      <c r="J38" s="4">
+      <c r="J38" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$79:J$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B38,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D38)*0.000001</f>
         <v>7.4905609868858525E-2</v>
       </c>
-      <c r="K38" s="4">
+      <c r="K38" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$79:K$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B38,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D38)*0.000001</f>
         <v>1.4758357184061859</v>
       </c>
-      <c r="L38" s="4">
+      <c r="L38" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$79:L$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B38,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D38)*0.000001</f>
         <v>1.2745873020685159</v>
       </c>
-      <c r="M38" s="4">
+      <c r="M38" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$79:M$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B38,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D38)*0.000001</f>
         <v>0.38691538504700607</v>
       </c>
@@ -11813,35 +11813,35 @@
       <c r="E39" t="s">
         <v>14</v>
       </c>
-      <c r="F39" s="3">
+      <c r="F39" s="2">
         <f ca="1">SUMIFS('Engines indvidual'!F$79:F$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B39,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D39)*0.000001</f>
         <v>0.36890869617646871</v>
       </c>
-      <c r="G39" s="4">
+      <c r="G39" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$79:G$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B39,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D39)*0.000001</f>
         <v>9.6015483091249895E-2</v>
       </c>
-      <c r="H39" s="4">
+      <c r="H39" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$79:H$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B39,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D39)*0.000001</f>
         <v>0.21737518641766049</v>
       </c>
-      <c r="I39" s="4">
+      <c r="I39" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$79:I$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B39,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D39)*0.000001</f>
         <v>4.7177125114565108E-2</v>
       </c>
-      <c r="J39" s="4">
+      <c r="J39" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$79:J$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B39,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D39)*0.000001</f>
         <v>8.3409015529947537E-3</v>
       </c>
-      <c r="K39" s="4">
+      <c r="K39" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$79:K$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B39,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D39)*0.000001</f>
         <v>0.16595651910759779</v>
       </c>
-      <c r="L39" s="4">
+      <c r="L39" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$79:L$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B39,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D39)*0.000001</f>
         <v>0.15912728777770299</v>
       </c>
-      <c r="M39" s="4">
+      <c r="M39" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$79:M$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B39,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D39)*0.000001</f>
         <v>4.3824889291169782E-2</v>
       </c>
@@ -11862,35 +11862,35 @@
       <c r="E40" t="s">
         <v>14</v>
       </c>
-      <c r="F40" s="3">
+      <c r="F40" s="2">
         <f ca="1">SUMIFS('Engines indvidual'!F$79:F$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B40,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D40)*0.000001</f>
         <v>9.6218260323394293</v>
       </c>
-      <c r="G40" s="4">
+      <c r="G40" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$79:G$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B40,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D40)*0.000001</f>
         <v>2.8692549161887833</v>
       </c>
-      <c r="H40" s="4">
+      <c r="H40" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$79:H$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B40,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D40)*0.000001</f>
         <v>5.5040193618164501</v>
       </c>
-      <c r="I40" s="4">
+      <c r="I40" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$79:I$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B40,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D40)*0.000001</f>
         <v>1.0110670874328809</v>
       </c>
-      <c r="J40" s="4">
+      <c r="J40" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$79:J$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B40,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D40)*0.000001</f>
         <v>0.23748466690132874</v>
       </c>
-      <c r="K40" s="4">
+      <c r="K40" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$79:K$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B40,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D40)*0.000001</f>
         <v>4.3085586678437124</v>
       </c>
-      <c r="L40" s="4">
+      <c r="L40" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$79:L$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B40,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D40)*0.000001</f>
         <v>3.9010572563274795</v>
       </c>
-      <c r="M40" s="4">
+      <c r="M40" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$79:M$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B40,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D40)*0.000001</f>
         <v>1.412210108168291</v>
       </c>
@@ -11911,35 +11911,35 @@
       <c r="E41" t="s">
         <v>7</v>
       </c>
-      <c r="F41" s="3">
+      <c r="F41" s="2">
         <f ca="1">SUMIFS('Engines indvidual'!F$79:F$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B41,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D41)*0.000001</f>
         <v>11.420652066936821</v>
       </c>
-      <c r="G41" s="4">
+      <c r="G41" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$79:G$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B41,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D41)*0.000001</f>
         <v>3.5090896918111696</v>
       </c>
-      <c r="H41" s="4">
+      <c r="H41" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$79:H$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B41,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D41)*0.000001</f>
         <v>6.4321943576416905</v>
       </c>
-      <c r="I41" s="4">
+      <c r="I41" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$79:I$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B41,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D41)*0.000001</f>
         <v>1.1454417490045459</v>
       </c>
-      <c r="J41" s="4">
+      <c r="J41" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$79:J$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B41,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D41)*0.000001</f>
         <v>0.33392626847940904</v>
       </c>
-      <c r="K41" s="4">
+      <c r="K41" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$79:K$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B41,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D41)*0.000001</f>
         <v>4.8569454909505971</v>
       </c>
-      <c r="L41" s="4">
+      <c r="L41" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$79:L$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B41,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D41)*0.000001</f>
         <v>4.9648645744792912</v>
       </c>
-      <c r="M41" s="4">
+      <c r="M41" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$79:M$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B41,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D41)*0.000001</f>
         <v>1.5988420015068729</v>
       </c>
@@ -11960,35 +11960,35 @@
       <c r="E42" t="s">
         <v>12</v>
       </c>
-      <c r="F42" s="3">
+      <c r="F42" s="2">
         <f ca="1">SUMIFS('Engines indvidual'!F$79:F$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B42,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D42)*0.000001</f>
         <v>62.015060713286694</v>
       </c>
-      <c r="G42" s="4">
+      <c r="G42" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$79:G$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B42,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D42)*0.000001</f>
         <v>20.781102004670501</v>
       </c>
-      <c r="H42" s="4">
+      <c r="H42" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$79:H$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B42,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D42)*0.000001</f>
         <v>34.328062288766255</v>
       </c>
-      <c r="I42" s="4">
+      <c r="I42" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$79:I$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B42,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D42)*0.000001</f>
         <v>6.2492192962949575</v>
       </c>
-      <c r="J42" s="4">
+      <c r="J42" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$79:J$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B42,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D42)*0.000001</f>
         <v>1.8514970157839417</v>
       </c>
-      <c r="K42" s="4">
+      <c r="K42" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$79:K$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B42,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D42)*0.000001</f>
         <v>26.971293296935141</v>
       </c>
-      <c r="L42" s="4">
+      <c r="L42" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$79:L$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B42,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D42)*0.000001</f>
         <v>26.344290974584506</v>
       </c>
-      <c r="M42" s="4">
+      <c r="M42" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$79:M$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B42,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D42)*0.000001</f>
         <v>9.8942963339961096</v>
       </c>
@@ -12009,35 +12009,35 @@
       <c r="E43" t="s">
         <v>14</v>
       </c>
-      <c r="F43" s="3">
+      <c r="F43" s="2">
         <f ca="1">SUMIFS('Engines indvidual'!F$79:F$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B43,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D43)*0.000001</f>
         <v>0.64737262381221894</v>
       </c>
-      <c r="G43" s="4">
+      <c r="G43" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$79:G$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B43,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D43)*0.000001</f>
         <v>0.18961566820772591</v>
       </c>
-      <c r="H43" s="4">
+      <c r="H43" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$79:H$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B43,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D43)*0.000001</f>
         <v>0.36437431234988571</v>
       </c>
-      <c r="I43" s="4">
+      <c r="I43" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$79:I$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B43,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D43)*0.000001</f>
         <v>7.7605858359894392E-2</v>
       </c>
-      <c r="J43" s="4">
+      <c r="J43" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$79:J$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B43,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D43)*0.000001</f>
         <v>1.5776784894709996E-2</v>
       </c>
-      <c r="K43" s="4">
+      <c r="K43" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$79:K$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B43,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D43)*0.000001</f>
         <v>0.28631308845600689</v>
       </c>
-      <c r="L43" s="4">
+      <c r="L43" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$79:L$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B43,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D43)*0.000001</f>
         <v>0.27869383415732607</v>
       </c>
-      <c r="M43" s="4">
+      <c r="M43" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$79:M$161,'Engines indvidual'!$B$79:$B$161,'Full system - simplified'!$B43,'Engines indvidual'!$D$79:$D$161,'Full system - simplified'!$D43)*0.000001</f>
         <v>8.2365701198884797E-2</v>
       </c>
@@ -12058,37 +12058,37 @@
       <c r="E45" t="s">
         <v>14</v>
       </c>
-      <c r="F45" s="3">
+      <c r="F45" s="2">
         <f t="shared" ref="F45:M45" ca="1" si="0">F12+F16+F33+F37-F46</f>
-        <v>12.422624021708751</v>
-      </c>
-      <c r="G45" s="3">
+        <v>12.422624021708739</v>
+      </c>
+      <c r="G45" s="2">
         <f t="shared" ca="1" si="0"/>
         <v>1.4569712855244032</v>
       </c>
-      <c r="H45" s="3">
+      <c r="H45" s="2">
         <f t="shared" ca="1" si="0"/>
         <v>8.6274107299374592</v>
       </c>
-      <c r="I45" s="3">
+      <c r="I45" s="2">
         <f t="shared" ca="1" si="0"/>
         <v>1.3640920780791912</v>
       </c>
-      <c r="J45" s="3">
+      <c r="J45" s="2">
         <f t="shared" ca="1" si="0"/>
         <v>0.97414992816775625</v>
       </c>
-      <c r="K45" s="3">
+      <c r="K45" s="2">
         <f t="shared" ca="1" si="0"/>
         <v>5.0972009778770051</v>
       </c>
-      <c r="L45" s="3">
+      <c r="L45" s="2">
         <f t="shared" ca="1" si="0"/>
         <v>5.2474772962100262</v>
       </c>
-      <c r="M45" s="3">
+      <c r="M45" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.0779457476217629</v>
+        <v>2.077945747621762</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -12107,35 +12107,35 @@
       <c r="E46" t="s">
         <v>14</v>
       </c>
-      <c r="F46" s="3">
+      <c r="F46" s="2">
         <f>([1]aggregated_flows_exergy!B$479-[1]aggregated_flows_exergy!B$482)*0.000001</f>
         <v>3.2444042199455012</v>
       </c>
-      <c r="G46" s="3">
+      <c r="G46" s="2">
         <f>([1]aggregated_flows_exergy!C$479-[1]aggregated_flows_exergy!C$482)*0.000001</f>
         <v>0.46158876188278009</v>
       </c>
-      <c r="H46" s="3">
+      <c r="H46" s="2">
         <f>([1]aggregated_flows_exergy!D$479-[1]aggregated_flows_exergy!D$482)*0.000001</f>
         <v>2.3266007049292994</v>
       </c>
-      <c r="I46" s="3">
+      <c r="I46" s="2">
         <f>([1]aggregated_flows_exergy!E$479-[1]aggregated_flows_exergy!E$482)*0.000001</f>
         <v>0.31211331308048007</v>
       </c>
-      <c r="J46" s="3">
+      <c r="J46" s="2">
         <f>([1]aggregated_flows_exergy!F$479-[1]aggregated_flows_exergy!F$482)*0.000001</f>
         <v>0.14410144005283701</v>
       </c>
-      <c r="K46" s="3">
+      <c r="K46" s="2">
         <f>([1]aggregated_flows_exergy!G$479-[1]aggregated_flows_exergy!G$482)*0.000001</f>
         <v>1.5253791035369988</v>
       </c>
-      <c r="L46" s="3">
+      <c r="L46" s="2">
         <f>([1]aggregated_flows_exergy!H$479-[1]aggregated_flows_exergy!H$482)*0.000001</f>
         <v>1.3376564210866801</v>
       </c>
-      <c r="M46" s="3">
+      <c r="M46" s="2">
         <f>([1]aggregated_flows_exergy!I$479-[1]aggregated_flows_exergy!I$482)*0.000001</f>
         <v>0.38136869532173989</v>
       </c>
@@ -12156,35 +12156,35 @@
       <c r="E47" t="s">
         <v>14</v>
       </c>
-      <c r="F47" s="3">
+      <c r="F47" s="2">
         <f>([1]aggregated_flows_exergy!B$498-[1]aggregated_flows_exergy!B$499)*0.000001</f>
         <v>10.870576729180531</v>
       </c>
-      <c r="G47" s="3">
+      <c r="G47" s="2">
         <f>([1]aggregated_flows_exergy!C$498-[1]aggregated_flows_exergy!C$499)*0.000001</f>
         <v>4.9418622286567819</v>
       </c>
-      <c r="H47" s="3">
+      <c r="H47" s="2">
         <f>([1]aggregated_flows_exergy!D$498-[1]aggregated_flows_exergy!D$499)*0.000001</f>
         <v>5.0877626892342755</v>
       </c>
-      <c r="I47" s="3">
+      <c r="I47" s="2">
         <f>([1]aggregated_flows_exergy!E$498-[1]aggregated_flows_exergy!E$499)*0.000001</f>
         <v>0.75081095889419491</v>
       </c>
-      <c r="J47" s="3">
+      <c r="J47" s="2">
         <f>([1]aggregated_flows_exergy!F$498-[1]aggregated_flows_exergy!F$499)*0.000001</f>
         <v>9.014085239542298E-2</v>
       </c>
-      <c r="K47" s="3">
+      <c r="K47" s="2">
         <f>([1]aggregated_flows_exergy!G$498-[1]aggregated_flows_exergy!G$499)*0.000001</f>
         <v>6.5149143259059699</v>
       </c>
-      <c r="L47" s="3">
+      <c r="L47" s="2">
         <f>([1]aggregated_flows_exergy!H$498-[1]aggregated_flows_exergy!H$499)*0.000001</f>
         <v>3.820487374233541</v>
       </c>
-      <c r="M47" s="3">
+      <c r="M47" s="2">
         <f>([1]aggregated_flows_exergy!I$498-[1]aggregated_flows_exergy!I$499)*0.000001</f>
         <v>0.53517502904116687</v>
       </c>
@@ -12205,35 +12205,35 @@
       <c r="E48" t="s">
         <v>7</v>
       </c>
-      <c r="F48" s="3">
+      <c r="F48" s="2">
         <f>([1]aggregated_flows_exergy!B$510-[1]aggregated_flows_exergy!B$509)*0.000001</f>
         <v>18.55076862377264</v>
       </c>
-      <c r="G48" s="3">
+      <c r="G48" s="2">
         <f>([1]aggregated_flows_exergy!C$510-[1]aggregated_flows_exergy!C$509)*0.000001</f>
         <v>6.867940353536218</v>
       </c>
-      <c r="H48" s="3">
+      <c r="H48" s="2">
         <f>([1]aggregated_flows_exergy!D$510-[1]aggregated_flows_exergy!D$509)*0.000001</f>
         <v>9.6723936486684998</v>
       </c>
-      <c r="I48" s="3">
+      <c r="I48" s="2">
         <f>([1]aggregated_flows_exergy!E$510-[1]aggregated_flows_exergy!E$509)*0.000001</f>
         <v>1.4805635202428682</v>
       </c>
-      <c r="J48" s="3">
+      <c r="J48" s="2">
         <f>([1]aggregated_flows_exergy!F$510-[1]aggregated_flows_exergy!F$509)*0.000001</f>
         <v>0.5298711013249543</v>
       </c>
-      <c r="K48" s="3">
+      <c r="K48" s="2">
         <f>([1]aggregated_flows_exergy!G$510-[1]aggregated_flows_exergy!G$509)*0.000001</f>
         <v>9.6492629930296321</v>
       </c>
-      <c r="L48" s="3">
+      <c r="L48" s="2">
         <f>([1]aggregated_flows_exergy!H$510-[1]aggregated_flows_exergy!H$509)*0.000001</f>
         <v>6.9676009801942822</v>
       </c>
-      <c r="M48" s="3">
+      <c r="M48" s="2">
         <f>([1]aggregated_flows_exergy!I$510-[1]aggregated_flows_exergy!I$509)*0.000001</f>
         <v>1.9339046505485058</v>
       </c>
@@ -12254,35 +12254,35 @@
       <c r="E49" t="s">
         <v>7</v>
       </c>
-      <c r="F49" s="3">
+      <c r="F49" s="2">
         <f>[1]aggregated_flows_exergy!B$506*0.000001</f>
         <v>1.5103823533040599</v>
       </c>
-      <c r="G49" s="3">
+      <c r="G49" s="2">
         <f>[1]aggregated_flows_exergy!C$506*0.000001</f>
         <v>1.0434617423271599</v>
       </c>
-      <c r="H49" s="3">
+      <c r="H49" s="2">
         <f>[1]aggregated_flows_exergy!D$506*0.000001</f>
         <v>0.38408615846056199</v>
       </c>
-      <c r="I49" s="3">
+      <c r="I49" s="2">
         <f>[1]aggregated_flows_exergy!E$506*0.000001</f>
         <v>8.2362099874332392E-2</v>
       </c>
-      <c r="J49" s="3">
+      <c r="J49" s="2">
         <f>[1]aggregated_flows_exergy!F$506*0.000001</f>
         <v>4.7235264201508497E-4</v>
       </c>
-      <c r="K49" s="3">
+      <c r="K49" s="2">
         <f>[1]aggregated_flows_exergy!G$506*0.000001</f>
         <v>0.98527050887994394</v>
       </c>
-      <c r="L49" s="3">
+      <c r="L49" s="2">
         <f>[1]aggregated_flows_exergy!H$506*0.000001</f>
         <v>0.49795417806773701</v>
       </c>
-      <c r="M49" s="3">
+      <c r="M49" s="2">
         <f>[1]aggregated_flows_exergy!I$506*0.000001</f>
         <v>2.7157666356389398E-2</v>
       </c>
@@ -12303,35 +12303,35 @@
       <c r="E50" t="s">
         <v>14</v>
       </c>
-      <c r="F50" s="3">
+      <c r="F50" s="2">
         <f>[1]aggregated_flows_exergy!B$571*0.000001</f>
         <v>3.4069030093520496</v>
       </c>
-      <c r="G50" s="3">
+      <c r="G50" s="2">
         <f>[1]aggregated_flows_exergy!C$571*0.000001</f>
         <v>1.2194992725623299</v>
       </c>
-      <c r="H50" s="3">
+      <c r="H50" s="2">
         <f>[1]aggregated_flows_exergy!D$571*0.000001</f>
         <v>1.8935791158047999</v>
       </c>
-      <c r="I50" s="3">
+      <c r="I50" s="2">
         <f>[1]aggregated_flows_exergy!E$571*0.000001</f>
         <v>0.246404928112197</v>
       </c>
-      <c r="J50" s="3">
+      <c r="J50" s="2">
         <f>[1]aggregated_flows_exergy!F$571*0.000001</f>
         <v>4.7419692872702396E-2</v>
       </c>
-      <c r="K50" s="3">
+      <c r="K50" s="2">
         <f>[1]aggregated_flows_exergy!G$571*0.000001</f>
         <v>2.2944500609015397</v>
       </c>
-      <c r="L50" s="3">
+      <c r="L50" s="2">
         <f>[1]aggregated_flows_exergy!H$571*0.000001</f>
         <v>1.1124529484505099</v>
       </c>
-      <c r="M50" s="3">
+      <c r="M50" s="2">
         <f>[1]aggregated_flows_exergy!I$571*0.000001</f>
         <v>0</v>
       </c>
@@ -12352,35 +12352,35 @@
       <c r="E51" t="s">
         <v>14</v>
       </c>
-      <c r="F51" s="3">
+      <c r="F51" s="2">
         <f>[1]aggregated_flows_exergy!B$572*0.000001</f>
         <v>0.27643994972985997</v>
       </c>
-      <c r="G51" s="3">
+      <c r="G51" s="2">
         <f>[1]aggregated_flows_exergy!C$572*0.000001</f>
         <v>9.06263288582497E-2</v>
       </c>
-      <c r="H51" s="3">
+      <c r="H51" s="2">
         <f>[1]aggregated_flows_exergy!D$572*0.000001</f>
         <v>0.13064685866679099</v>
       </c>
-      <c r="I51" s="3">
+      <c r="I51" s="2">
         <f>[1]aggregated_flows_exergy!E$572*0.000001</f>
         <v>2.7867139357235397E-2</v>
       </c>
-      <c r="J51" s="3">
+      <c r="J51" s="2">
         <f>[1]aggregated_flows_exergy!F$572*0.000001</f>
         <v>2.72996228475842E-2</v>
       </c>
-      <c r="K51" s="3">
+      <c r="K51" s="2">
         <f>[1]aggregated_flows_exergy!G$572*0.000001</f>
         <v>0</v>
       </c>
-      <c r="L51" s="3">
+      <c r="L51" s="2">
         <f>[1]aggregated_flows_exergy!H$572*0.000001</f>
         <v>0</v>
       </c>
-      <c r="M51" s="3">
+      <c r="M51" s="2">
         <f>[1]aggregated_flows_exergy!I$572*0.000001</f>
         <v>0.27643994972985997</v>
       </c>
@@ -12401,35 +12401,35 @@
       <c r="E52" t="s">
         <v>14</v>
       </c>
-      <c r="F52" s="3">
+      <c r="F52" s="2">
         <f>[1]aggregated_flows_exergy!B$570*0.000001</f>
         <v>1.9583056043579798</v>
       </c>
-      <c r="G52" s="3">
+      <c r="G52" s="2">
         <f>[1]aggregated_flows_exergy!C$570*0.000001</f>
         <v>0.63937363885036791</v>
       </c>
-      <c r="H52" s="3">
+      <c r="H52" s="2">
         <f>[1]aggregated_flows_exergy!D$570*0.000001</f>
         <v>1.09161802930435</v>
       </c>
-      <c r="I52" s="3">
+      <c r="I52" s="2">
         <f>[1]aggregated_flows_exergy!E$570*0.000001</f>
         <v>0.17453951207662799</v>
       </c>
-      <c r="J52" s="3">
+      <c r="J52" s="2">
         <f>[1]aggregated_flows_exergy!F$570*0.000001</f>
         <v>5.27744241266737E-2</v>
       </c>
-      <c r="K52" s="3">
+      <c r="K52" s="2">
         <f>[1]aggregated_flows_exergy!G$570*0.000001</f>
         <v>0.84126451599489493</v>
       </c>
-      <c r="L52" s="3">
+      <c r="L52" s="2">
         <f>[1]aggregated_flows_exergy!H$570*0.000001</f>
         <v>0.81174428901624096</v>
       </c>
-      <c r="M52" s="3">
+      <c r="M52" s="2">
         <f>[1]aggregated_flows_exergy!I$570*0.000001</f>
         <v>0.30529679934687598</v>
       </c>
@@ -12450,35 +12450,35 @@
       <c r="E53" t="s">
         <v>14</v>
       </c>
-      <c r="F53" s="3">
+      <c r="F53" s="2">
         <f>[1]aggregated_flows_exergy!B$576*0.000001</f>
         <v>0.17739045768655498</v>
       </c>
-      <c r="G53" s="3">
+      <c r="G53" s="2">
         <f>[1]aggregated_flows_exergy!C$576*0.000001</f>
         <v>6.2239265787400994E-2</v>
       </c>
-      <c r="H53" s="3">
+      <c r="H53" s="2">
         <f>[1]aggregated_flows_exergy!D$576*0.000001</f>
         <v>9.6608521996453894E-2</v>
       </c>
-      <c r="I53" s="3">
+      <c r="I53" s="2">
         <f>[1]aggregated_flows_exergy!E$576*0.000001</f>
         <v>1.43407038077223E-2</v>
       </c>
-      <c r="J53" s="3">
+      <c r="J53" s="2">
         <f>[1]aggregated_flows_exergy!F$576*0.000001</f>
         <v>4.2019660949773399E-3</v>
       </c>
-      <c r="K53" s="3">
+      <c r="K53" s="2">
         <f>[1]aggregated_flows_exergy!G$576*0.000001</f>
         <v>8.848073737441349E-2</v>
       </c>
-      <c r="L53" s="3">
+      <c r="L53" s="2">
         <f>[1]aggregated_flows_exergy!H$576*0.000001</f>
         <v>7.2034193946725986E-2</v>
       </c>
-      <c r="M53" s="3">
+      <c r="M53" s="2">
         <f>[1]aggregated_flows_exergy!I$576*0.000001</f>
         <v>1.6875526365414801E-2</v>
       </c>
@@ -12499,35 +12499,35 @@
       <c r="E54" t="s">
         <v>14</v>
       </c>
-      <c r="F54" s="3">
+      <c r="F54" s="2">
         <f>[1]aggregated_flows_exergy!B$575*0.000001</f>
         <v>0.36513430088944998</v>
       </c>
-      <c r="G54" s="3">
+      <c r="G54" s="2">
         <f>[1]aggregated_flows_exergy!C$575*0.000001</f>
         <v>0.12762239469109099</v>
       </c>
-      <c r="H54" s="3">
+      <c r="H54" s="2">
         <f>[1]aggregated_flows_exergy!D$575*0.000001</f>
         <v>0.19749372237287499</v>
       </c>
-      <c r="I54" s="3">
+      <c r="I54" s="2">
         <f>[1]aggregated_flows_exergy!E$575*0.000001</f>
         <v>3.0310478440709498E-2</v>
       </c>
-      <c r="J54" s="3">
+      <c r="J54" s="2">
         <f>[1]aggregated_flows_exergy!F$575*0.000001</f>
         <v>9.7077053847736891E-3</v>
       </c>
-      <c r="K54" s="3">
+      <c r="K54" s="2">
         <f>[1]aggregated_flows_exergy!G$575*0.000001</f>
         <v>0.163130953549875</v>
       </c>
-      <c r="L54" s="3">
+      <c r="L54" s="2">
         <f>[1]aggregated_flows_exergy!H$575*0.000001</f>
         <v>0.15777022026843199</v>
       </c>
-      <c r="M54" s="3">
+      <c r="M54" s="2">
         <f>[1]aggregated_flows_exergy!I$575*0.000001</f>
         <v>4.4233127071141499E-2</v>
       </c>
@@ -12548,35 +12548,35 @@
       <c r="E55" t="s">
         <v>14</v>
       </c>
-      <c r="F55" s="3">
+      <c r="F55" s="2">
         <f>[1]aggregated_flows_exergy!B$577*0.000001</f>
         <v>0.29389645906742901</v>
       </c>
-      <c r="G55" s="3">
+      <c r="G55" s="2">
         <f>[1]aggregated_flows_exergy!C$577*0.000001</f>
         <v>3.6964912978471001E-2</v>
       </c>
-      <c r="H55" s="3">
+      <c r="H55" s="2">
         <f>[1]aggregated_flows_exergy!D$577*0.000001</f>
         <v>0.20780884410724598</v>
       </c>
-      <c r="I55" s="3">
+      <c r="I55" s="2">
         <f>[1]aggregated_flows_exergy!E$577*0.000001</f>
         <v>2.8580759289889502E-2</v>
       </c>
-      <c r="J55" s="3">
+      <c r="J55" s="2">
         <f>[1]aggregated_flows_exergy!F$577*0.000001</f>
         <v>2.0541942691823498E-2</v>
       </c>
-      <c r="K55" s="3">
+      <c r="K55" s="2">
         <f>[1]aggregated_flows_exergy!G$577*0.000001</f>
         <v>0.128599540424509</v>
       </c>
-      <c r="L55" s="3">
+      <c r="L55" s="2">
         <f>[1]aggregated_flows_exergy!H$577*0.000001</f>
         <v>0.121497793508528</v>
       </c>
-      <c r="M55" s="3">
+      <c r="M55" s="2">
         <f>[1]aggregated_flows_exergy!I$577*0.000001</f>
         <v>4.3799125134392193E-2</v>
       </c>
@@ -12597,35 +12597,35 @@
       <c r="E56" t="s">
         <v>14</v>
       </c>
-      <c r="F56" s="3">
+      <c r="F56" s="2">
         <f>[1]aggregated_flows_exergy!B$573*0.000001</f>
         <v>0.22964173896057499</v>
       </c>
-      <c r="G56" s="3">
+      <c r="G56" s="2">
         <f>[1]aggregated_flows_exergy!C$573*0.000001</f>
         <v>8.0328910487552904E-2</v>
       </c>
-      <c r="H56" s="3">
+      <c r="H56" s="2">
         <f>[1]aggregated_flows_exergy!D$573*0.000001</f>
         <v>0.12438722010898599</v>
       </c>
-      <c r="I56" s="3">
+      <c r="I56" s="2">
         <f>[1]aggregated_flows_exergy!E$573*0.000001</f>
         <v>1.8959072180331899E-2</v>
       </c>
-      <c r="J56" s="3">
+      <c r="J56" s="2">
         <f>[1]aggregated_flows_exergy!F$573*0.000001</f>
         <v>5.9665361837027402E-3</v>
       </c>
-      <c r="K56" s="3">
+      <c r="K56" s="2">
         <f>[1]aggregated_flows_exergy!G$573*0.000001</f>
         <v>0.105088983763517</v>
       </c>
-      <c r="L56" s="3">
+      <c r="L56" s="2">
         <f>[1]aggregated_flows_exergy!H$573*0.000001</f>
         <v>9.7979453279093298E-2</v>
       </c>
-      <c r="M56" s="3">
+      <c r="M56" s="2">
         <f>[1]aggregated_flows_exergy!I$573*0.000001</f>
         <v>2.65733019179623E-2</v>
       </c>
@@ -12646,35 +12646,35 @@
       <c r="E57" t="s">
         <v>14</v>
       </c>
-      <c r="F57" s="3">
+      <c r="F57" s="2">
         <f>[1]aggregated_flows_exergy!B$578*0.000001</f>
         <v>1.5930956022585399</v>
       </c>
-      <c r="G57" s="3">
+      <c r="G57" s="2">
         <f>[1]aggregated_flows_exergy!C$578*0.000001</f>
         <v>0.43963520161171799</v>
       </c>
-      <c r="H57" s="3">
+      <c r="H57" s="2">
         <f>[1]aggregated_flows_exergy!D$578*0.000001</f>
         <v>0.97548546689526094</v>
       </c>
-      <c r="I57" s="3">
+      <c r="I57" s="2">
         <f>[1]aggregated_flows_exergy!E$578*0.000001</f>
         <v>0.14226219825891501</v>
       </c>
-      <c r="J57" s="3">
+      <c r="J57" s="2">
         <f>[1]aggregated_flows_exergy!F$578*0.000001</f>
         <v>3.57127354926456E-2</v>
       </c>
-      <c r="K57" s="3">
+      <c r="K57" s="2">
         <f>[1]aggregated_flows_exergy!G$578*0.000001</f>
         <v>0.71349585107152691</v>
       </c>
-      <c r="L57" s="3">
+      <c r="L57" s="2">
         <f>[1]aggregated_flows_exergy!H$578*0.000001</f>
         <v>0.68914940986570206</v>
       </c>
-      <c r="M57" s="3">
+      <c r="M57" s="2">
         <f>[1]aggregated_flows_exergy!I$578*0.000001</f>
         <v>0.19045034132130198</v>
       </c>
@@ -12695,35 +12695,35 @@
       <c r="E58" t="s">
         <v>14</v>
       </c>
-      <c r="F58" s="3">
+      <c r="F58" s="2">
         <f>[1]aggregated_flows_exergy!B$573*0.000001</f>
         <v>0.22964173896057499</v>
       </c>
-      <c r="G58" s="3">
+      <c r="G58" s="2">
         <f>[1]aggregated_flows_exergy!C$573*0.000001</f>
         <v>8.0328910487552904E-2</v>
       </c>
-      <c r="H58" s="3">
+      <c r="H58" s="2">
         <f>[1]aggregated_flows_exergy!D$573*0.000001</f>
         <v>0.12438722010898599</v>
       </c>
-      <c r="I58" s="3">
+      <c r="I58" s="2">
         <f>[1]aggregated_flows_exergy!E$573*0.000001</f>
         <v>1.8959072180331899E-2</v>
       </c>
-      <c r="J58" s="3">
+      <c r="J58" s="2">
         <f>[1]aggregated_flows_exergy!F$573*0.000001</f>
         <v>5.9665361837027402E-3</v>
       </c>
-      <c r="K58" s="3">
+      <c r="K58" s="2">
         <f>[1]aggregated_flows_exergy!G$573*0.000001</f>
         <v>0.105088983763517</v>
       </c>
-      <c r="L58" s="3">
+      <c r="L58" s="2">
         <f>[1]aggregated_flows_exergy!H$573*0.000001</f>
         <v>9.7979453279093298E-2</v>
       </c>
-      <c r="M58" s="3">
+      <c r="M58" s="2">
         <f>[1]aggregated_flows_exergy!I$573*0.000001</f>
         <v>2.65733019179623E-2</v>
       </c>
@@ -12744,35 +12744,35 @@
       <c r="E59" t="s">
         <v>12</v>
       </c>
-      <c r="F59" s="3">
+      <c r="F59" s="2">
         <f>[1]aggregated_flows_exergy!B$563*0.000001</f>
         <v>0.93750587795543494</v>
       </c>
-      <c r="G59" s="3">
+      <c r="G59" s="2">
         <f>[1]aggregated_flows_exergy!C$563*0.000001</f>
         <v>0</v>
       </c>
-      <c r="H59" s="3">
+      <c r="H59" s="2">
         <f>[1]aggregated_flows_exergy!D$563*0.000001</f>
         <v>0</v>
       </c>
-      <c r="I59" s="3">
+      <c r="I59" s="2">
         <f>[1]aggregated_flows_exergy!E$563*0.000001</f>
         <v>0.93750587795543494</v>
       </c>
-      <c r="J59" s="3">
+      <c r="J59" s="2">
         <f>[1]aggregated_flows_exergy!F$563*0.000001</f>
         <v>0</v>
       </c>
-      <c r="K59" s="3">
+      <c r="K59" s="2">
         <f>[1]aggregated_flows_exergy!G$563*0.000001</f>
         <v>0.35598315745528797</v>
       </c>
-      <c r="L59" s="3">
+      <c r="L59" s="2">
         <f>[1]aggregated_flows_exergy!H$563*0.000001</f>
         <v>0.43040035297186197</v>
       </c>
-      <c r="M59" s="3">
+      <c r="M59" s="2">
         <f>[1]aggregated_flows_exergy!I$563*0.000001</f>
         <v>0.15112236752828601</v>
       </c>
@@ -12793,35 +12793,35 @@
       <c r="E60" t="s">
         <v>12</v>
       </c>
-      <c r="F60" s="3">
+      <c r="F60" s="2">
         <f>[1]aggregated_flows_exergy!B$564*0.000001</f>
         <v>1.79104433624467</v>
       </c>
-      <c r="G60" s="3">
+      <c r="G60" s="2">
         <f>[1]aggregated_flows_exergy!C$564*0.000001</f>
         <v>0.58755787633946899</v>
       </c>
-      <c r="H60" s="3">
+      <c r="H60" s="2">
         <f>[1]aggregated_flows_exergy!D$564*0.000001</f>
         <v>0.84524501221639803</v>
       </c>
-      <c r="I60" s="3">
+      <c r="I60" s="2">
         <f>[1]aggregated_flows_exergy!E$564*0.000001</f>
         <v>0.181935036356171</v>
       </c>
-      <c r="J60" s="3">
+      <c r="J60" s="2">
         <f>[1]aggregated_flows_exergy!F$564*0.000001</f>
         <v>0.176306411332635</v>
       </c>
-      <c r="K60" s="3">
+      <c r="K60" s="2">
         <f>[1]aggregated_flows_exergy!G$564*0.000001</f>
         <v>0</v>
       </c>
-      <c r="L60" s="3">
+      <c r="L60" s="2">
         <f>[1]aggregated_flows_exergy!H$564*0.000001</f>
         <v>0</v>
       </c>
-      <c r="M60" s="3">
+      <c r="M60" s="2">
         <f>[1]aggregated_flows_exergy!I$564*0.000001</f>
         <v>1.79104433624467</v>
       </c>
@@ -12842,35 +12842,35 @@
       <c r="E61" t="s">
         <v>12</v>
       </c>
-      <c r="F61" s="3">
+      <c r="F61" s="2">
         <f>[1]aggregated_flows_exergy!B$565*0.000001</f>
         <v>59.286510499086603</v>
       </c>
-      <c r="G61" s="3">
+      <c r="G61" s="2">
         <f>[1]aggregated_flows_exergy!C$565*0.000001</f>
         <v>19.991299900900298</v>
       </c>
-      <c r="H61" s="3">
+      <c r="H61" s="2">
         <f>[1]aggregated_flows_exergy!D$565*0.000001</f>
         <v>32.660205873217699</v>
       </c>
-      <c r="I61" s="3">
+      <c r="I61" s="2">
         <f>[1]aggregated_flows_exergy!E$565*0.000001</f>
         <v>4.9940078210969503</v>
       </c>
-      <c r="J61" s="3">
+      <c r="J61" s="2">
         <f>[1]aggregated_flows_exergy!F$565*0.000001</f>
         <v>1.6409969038717298</v>
       </c>
-      <c r="K61" s="3">
+      <c r="K61" s="2">
         <f>[1]aggregated_flows_exergy!G$565*0.000001</f>
         <v>26.055225100767899</v>
       </c>
-      <c r="L61" s="3">
+      <c r="L61" s="2">
         <f>[1]aggregated_flows_exergy!H$565*0.000001</f>
         <v>25.448506615958099</v>
       </c>
-      <c r="M61" s="3">
+      <c r="M61" s="2">
         <f>[1]aggregated_flows_exergy!I$565*0.000001</f>
         <v>7.7827787823608201</v>
       </c>
@@ -12891,35 +12891,35 @@
       <c r="E62" t="s">
         <v>12</v>
       </c>
-      <c r="F62" s="3">
+      <c r="F62" s="2">
         <f>([1]aggregated_flows_exergy!B$567+[1]aggregated_flows_exergy!B$568)*0.000001</f>
         <v>104.1859732259615</v>
       </c>
-      <c r="G62" s="3">
+      <c r="G62" s="2">
         <f>([1]aggregated_flows_exergy!C$567+[1]aggregated_flows_exergy!C$568)*0.000001</f>
         <v>0.13661203371351111</v>
       </c>
-      <c r="H62" s="3">
+      <c r="H62" s="2">
         <f>([1]aggregated_flows_exergy!D$567+[1]aggregated_flows_exergy!D$568)*0.000001</f>
         <v>82.619928752936005</v>
       </c>
-      <c r="I62" s="3">
+      <c r="I62" s="2">
         <f>([1]aggregated_flows_exergy!E$567+[1]aggregated_flows_exergy!E$568)*0.000001</f>
         <v>9.8386654505439513</v>
       </c>
-      <c r="J62" s="3">
+      <c r="J62" s="2">
         <f>([1]aggregated_flows_exergy!F$567+[1]aggregated_flows_exergy!F$568)*0.000001</f>
         <v>11.590766988768118</v>
       </c>
-      <c r="K62" s="3">
+      <c r="K62" s="2">
         <f>([1]aggregated_flows_exergy!G$567+[1]aggregated_flows_exergy!G$568)*0.000001</f>
         <v>40.978918537417599</v>
       </c>
-      <c r="L62" s="3">
+      <c r="L62" s="2">
         <f>([1]aggregated_flows_exergy!H$567+[1]aggregated_flows_exergy!H$568)*0.000001</f>
         <v>44.547670643066894</v>
       </c>
-      <c r="M62" s="3">
+      <c r="M62" s="2">
         <f>([1]aggregated_flows_exergy!I$567+[1]aggregated_flows_exergy!I$568)*0.000001</f>
         <v>18.65938404547704</v>
       </c>
@@ -12940,35 +12940,35 @@
       <c r="E63" t="s">
         <v>14</v>
       </c>
-      <c r="F63" s="3">
+      <c r="F63" s="2">
         <f t="shared" ref="F63:M63" ca="1" si="1">F21-F62</f>
         <v>3.2001051351615928</v>
       </c>
-      <c r="G63" s="3">
+      <c r="G63" s="2">
         <f t="shared" ca="1" si="1"/>
         <v>4.1960818436018732E-3</v>
       </c>
-      <c r="H63" s="3">
+      <c r="H63" s="2">
         <f t="shared" ca="1" si="1"/>
         <v>2.5376972550375854</v>
       </c>
-      <c r="I63" s="3">
+      <c r="I63" s="2">
         <f t="shared" ca="1" si="1"/>
         <v>0.30219772255845889</v>
       </c>
-      <c r="J63" s="3">
+      <c r="J63" s="2">
         <f t="shared" ca="1" si="1"/>
         <v>0.35601407572180044</v>
       </c>
-      <c r="K63" s="3">
+      <c r="K63" s="2">
         <f t="shared" ca="1" si="1"/>
         <v>1.2586804498197068</v>
       </c>
-      <c r="L63" s="3">
+      <c r="L63" s="2">
         <f t="shared" ca="1" si="1"/>
         <v>1.3682958000033096</v>
       </c>
-      <c r="M63" s="3">
+      <c r="M63" s="2">
         <f t="shared" ca="1" si="1"/>
         <v>0.57312888533829209</v>
       </c>

</xml_diff>

<commit_message>
New corrections to the Grassmann files
</commit_message>
<xml_diff>
--- a/Results/inputGrassmann.xlsx
+++ b/Results/inputGrassmann.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1176" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1217" uniqueCount="58">
   <si>
     <t>From</t>
   </si>
@@ -186,6 +186,12 @@
   </si>
   <si>
     <t>Chemical</t>
+  </si>
+  <si>
+    <t>Demand</t>
+  </si>
+  <si>
+    <t>Losses (dumped steam)</t>
   </si>
 </sst>
 </file>
@@ -1073,28 +1079,28 @@
         </row>
         <row r="33">
           <cell r="B33">
-            <v>74985640.741413206</v>
+            <v>61396802.568495102</v>
           </cell>
           <cell r="C33">
-            <v>113542.479238346</v>
+            <v>92966.401460435096</v>
           </cell>
           <cell r="D33">
-            <v>58390450.022182398</v>
+            <v>47808979.111884698</v>
           </cell>
           <cell r="E33">
-            <v>7631954.3425091403</v>
+            <v>6248897.6468799198</v>
           </cell>
           <cell r="F33">
-            <v>8849693.8974832892</v>
+            <v>7245959.4082699697</v>
           </cell>
           <cell r="G33">
-            <v>29387116.064199299</v>
+            <v>24061606.265032701</v>
           </cell>
           <cell r="H33">
-            <v>32047059.3378167</v>
+            <v>26239516.734276701</v>
           </cell>
           <cell r="I33">
-            <v>13551465.339397101</v>
+            <v>11095679.5691853</v>
           </cell>
         </row>
         <row r="35">
@@ -1253,6 +1259,16 @@
             <v>31891.461186351</v>
           </cell>
         </row>
+        <row r="51">
+          <cell r="B51">
+            <v>5046302.1311542504</v>
+          </cell>
+        </row>
+        <row r="52">
+          <cell r="B52">
+            <v>14916665.437722599</v>
+          </cell>
+        </row>
         <row r="54">
           <cell r="B54">
             <v>5913328.1486983597</v>
@@ -1383,6 +1399,26 @@
             <v>1238063.3902508901</v>
           </cell>
         </row>
+        <row r="492">
+          <cell r="B492">
+            <v>24073580.778595202</v>
+          </cell>
+        </row>
+        <row r="493">
+          <cell r="B493">
+            <v>16641852.723539799</v>
+          </cell>
+        </row>
+        <row r="495">
+          <cell r="B495">
+            <v>916736.18038832396</v>
+          </cell>
+        </row>
+        <row r="496">
+          <cell r="B496">
+            <v>586083.665372135</v>
+          </cell>
+        </row>
         <row r="498">
           <cell r="B498">
             <v>12778609.189100301</v>
@@ -1435,6 +1471,16 @@
             <v>85765.0929390971</v>
           </cell>
         </row>
+        <row r="502">
+          <cell r="B502">
+            <v>7090731.4277157597</v>
+          </cell>
+        </row>
+        <row r="503">
+          <cell r="B503">
+            <v>4817951.4790552296</v>
+          </cell>
+        </row>
         <row r="506">
           <cell r="B506">
             <v>1510382.3533040599</v>
@@ -1463,28 +1509,28 @@
         </row>
         <row r="507">
           <cell r="B507">
-            <v>24563823.770410299</v>
+            <v>20112387.1643636</v>
           </cell>
           <cell r="C507">
-            <v>17542528.193726901</v>
+            <v>14363485.187474299</v>
           </cell>
           <cell r="D507">
-            <v>5773557.4563260898</v>
+            <v>4727277.9662752096</v>
           </cell>
           <cell r="E507">
-            <v>1240355.05455598</v>
+            <v>1015578.89812562</v>
           </cell>
           <cell r="F507">
-            <v>7383.0658009284798</v>
+            <v>6045.1124888430104</v>
           </cell>
           <cell r="G507">
-            <v>15854811.5056113</v>
+            <v>12981615.1751993</v>
           </cell>
           <cell r="H507">
-            <v>8252907.4280332197</v>
+            <v>6757322.1081402302</v>
           </cell>
           <cell r="I507">
-            <v>456104.83676530898</v>
+            <v>373449.88102434803</v>
           </cell>
         </row>
         <row r="508">
@@ -1617,6 +1663,92 @@
             <v>218576.99275999799</v>
           </cell>
         </row>
+        <row r="526">
+          <cell r="B526">
+            <v>88589.105082808906</v>
+          </cell>
+        </row>
+        <row r="527">
+          <cell r="B527">
+            <v>118118.80677707899</v>
+          </cell>
+        </row>
+        <row r="528">
+          <cell r="B528">
+            <v>113900.27796361101</v>
+          </cell>
+        </row>
+        <row r="529">
+          <cell r="B529">
+            <v>76353.148832306499</v>
+          </cell>
+        </row>
+        <row r="530">
+          <cell r="B530">
+            <v>422819.16395156702</v>
+          </cell>
+        </row>
+        <row r="532">
+          <cell r="B532">
+            <v>59059.403388539897</v>
+          </cell>
+        </row>
+        <row r="533">
+          <cell r="B533">
+            <v>806554.19849585195</v>
+          </cell>
+          <cell r="C533">
+            <v>3912.9252321069598</v>
+          </cell>
+          <cell r="D533">
+            <v>425738.42593756597</v>
+          </cell>
+          <cell r="E533">
+            <v>126879.380558362</v>
+          </cell>
+          <cell r="F533">
+            <v>250023.466767818</v>
+          </cell>
+          <cell r="G533">
+            <v>53673.321406558702</v>
+          </cell>
+          <cell r="H533">
+            <v>199713.230180271</v>
+          </cell>
+          <cell r="I533">
+            <v>553167.64690902503</v>
+          </cell>
+        </row>
+        <row r="537">
+          <cell r="B537">
+            <v>602224.53664885997</v>
+          </cell>
+        </row>
+        <row r="538">
+          <cell r="B538">
+            <v>802966.04886513797</v>
+          </cell>
+        </row>
+        <row r="539">
+          <cell r="B539">
+            <v>774288.68997710303</v>
+          </cell>
+        </row>
+        <row r="540">
+          <cell r="B540">
+            <v>519623.05615863198</v>
+          </cell>
+        </row>
+        <row r="541">
+          <cell r="B541">
+            <v>2872386.6801319299</v>
+          </cell>
+        </row>
+        <row r="543">
+          <cell r="B543">
+            <v>401483.02443256899</v>
+          </cell>
+        </row>
         <row r="563">
           <cell r="B563">
             <v>937505.87795543496</v>
@@ -1849,6 +1981,32 @@
           </cell>
           <cell r="I573">
             <v>26573.301917962301</v>
+          </cell>
+        </row>
+        <row r="574">
+          <cell r="B574">
+            <v>153094.49264038299</v>
+          </cell>
+          <cell r="C574">
+            <v>53552.606991702</v>
+          </cell>
+          <cell r="D574">
+            <v>82924.813405991707</v>
+          </cell>
+          <cell r="E574">
+            <v>12639.381453554601</v>
+          </cell>
+          <cell r="F574">
+            <v>3977.6907891351698</v>
+          </cell>
+          <cell r="G574">
+            <v>70059.322509012403</v>
+          </cell>
+          <cell r="H574">
+            <v>65319.635519396099</v>
+          </cell>
+          <cell r="I574">
+            <v>17715.534611974901</v>
           </cell>
         </row>
         <row r="575">
@@ -2226,8 +2384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P178"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F171" sqref="F171"/>
+    <sheetView topLeftCell="A174" workbookViewId="0">
+      <selection activeCell="E218" sqref="E218"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3218,35 +3376,35 @@
       </c>
       <c r="F20" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$33,0,0)</f>
-        <v>74985640.741413206</v>
+        <v>61396802.568495102</v>
       </c>
       <c r="G20" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!C$33,0,0)</f>
-        <v>113542.479238346</v>
+        <v>92966.401460435096</v>
       </c>
       <c r="H20" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!D$33,0,0)</f>
-        <v>58390450.022182398</v>
+        <v>47808979.111884698</v>
       </c>
       <c r="I20" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!E$33,0,0)</f>
-        <v>7631954.3425091403</v>
+        <v>6248897.6468799198</v>
       </c>
       <c r="J20" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!F$33,0,0)</f>
-        <v>8849693.8974832892</v>
+        <v>7245959.4082699697</v>
       </c>
       <c r="K20" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$33,0,0)</f>
-        <v>29387116.064199299</v>
+        <v>24061606.265032701</v>
       </c>
       <c r="L20" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!H$33,0,0)</f>
-        <v>32047059.3378167</v>
+        <v>26239516.734276701</v>
       </c>
       <c r="M20" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!I$33,0,0)</f>
-        <v>13551465.339397101</v>
+        <v>11095679.5691853</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4150,11 +4308,11 @@
         <v>14</v>
       </c>
       <c r="F39" s="1">
-        <f t="shared" ref="F39:M39" ca="1" si="6">F28-F40</f>
-        <v>3587174.3074345794</v>
+        <f ca="1">OFFSET([1]aggregated_flows_exergy!B$52,47,0)-OFFSET([1]aggregated_flows_exergy!B$51,47,0)</f>
+        <v>2439757.8806079971</v>
       </c>
       <c r="G39" s="1">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ref="F39:M39" ca="1" si="6">G28-G40</f>
         <v>3869.4917156394704</v>
       </c>
       <c r="H39" s="1">
@@ -4300,35 +4458,35 @@
       </c>
       <c r="F42" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$33,47,0)</f>
-        <v>85027881.370633796</v>
+        <v>69619196.338307396</v>
       </c>
       <c r="G42" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!C$33,47,0)</f>
-        <v>97513.686740289195</v>
+        <v>79842.333989860403</v>
       </c>
       <c r="H42" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!D$33,47,0)</f>
-        <v>67968352.054360002</v>
+        <v>55651181.3558833</v>
       </c>
       <c r="I42" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!E$33,47,0)</f>
-        <v>8366530.3897493295</v>
+        <v>6850354.4071079204</v>
       </c>
       <c r="J42" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!F$33,47,0)</f>
-        <v>8595485.23978463</v>
+        <v>7037818.2413264299</v>
       </c>
       <c r="K42" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$33,47,0)</f>
-        <v>33842707.942338496</v>
+        <v>27709759.3269138</v>
       </c>
       <c r="L42" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!H$33,47,0)</f>
-        <v>36337013.453151204</v>
+        <v>29752048.776983202</v>
       </c>
       <c r="M42" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!I$33,47,0)</f>
-        <v>14848159.9751442</v>
+        <v>12157388.2344101</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5232,11 +5390,11 @@
         <v>14</v>
       </c>
       <c r="F61" s="1">
-        <f t="shared" ref="F61:M61" ca="1" si="10">F50-F62</f>
-        <v>3168711.4337122794</v>
+        <f ca="1">OFFSET([1]aggregated_flows_exergy!B$52,98,0)-OFFSET([1]aggregated_flows_exergy!B$51,98,0)</f>
+        <v>2185550.0717062652</v>
       </c>
       <c r="G61" s="1">
-        <f t="shared" ca="1" si="10"/>
+        <f t="shared" ref="F61:M61" ca="1" si="10">G50-G62</f>
         <v>4414.1165117695091</v>
       </c>
       <c r="H61" s="1">
@@ -5382,35 +5540,35 @@
       </c>
       <c r="F64" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$33,98,0)</f>
-        <v>86847883.883933797</v>
+        <v>71109379.443744496</v>
       </c>
       <c r="G64" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!C$33,98,0)</f>
-        <v>143629.70707072801</v>
+        <v>117601.245795877</v>
       </c>
       <c r="H64" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!D$33,98,0)</f>
-        <v>70314621.718478099</v>
+        <v>57572261.897650696</v>
       </c>
       <c r="I64" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!E$33,98,0)</f>
-        <v>7861503.5693475902</v>
+        <v>6436848.14541006</v>
       </c>
       <c r="J64" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!F$33,98,0)</f>
-        <v>8528128.8890376594</v>
+        <v>6982668.1548877899</v>
       </c>
       <c r="K64" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$33,98,0)</f>
-        <v>34609525.252822198</v>
+        <v>28337614.614304502</v>
       </c>
       <c r="L64" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!H$33,98,0)</f>
-        <v>37190767.520420298</v>
+        <v>30451086.211242601</v>
       </c>
       <c r="M64" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!I$33,98,0)</f>
-        <v>15047591.1106914</v>
+        <v>12320678.6181973</v>
       </c>
     </row>
     <row r="65" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6366,35 +6524,35 @@
       </c>
       <c r="F84" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$33,149,0)</f>
-        <v>78034528.441305697</v>
+        <v>63893173.264443099</v>
       </c>
       <c r="G84" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!C$33,149,0)</f>
-        <v>112367.76803012101</v>
+        <v>92004.570483020405</v>
       </c>
       <c r="H84" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!D$33,149,0)</f>
-        <v>62537804.98048</v>
+        <v>51204753.703371398</v>
       </c>
       <c r="I84" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!E$33,149,0)</f>
-        <v>7222854.3868966503</v>
+        <v>5913934.45983274</v>
       </c>
       <c r="J84" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!F$33,149,0)</f>
-        <v>8161501.3058983702</v>
+        <v>6682480.5307559697</v>
       </c>
       <c r="K84" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$33,149,0)</f>
-        <v>30579017.619305901</v>
+        <v>25037512.368340202</v>
       </c>
       <c r="L84" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!H$33,149,0)</f>
-        <v>33896944.197181597</v>
+        <v>27754166.930792801</v>
       </c>
       <c r="M84" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!I$33,149,0)</f>
-        <v>13558566.6248176</v>
+        <v>11101493.9653101</v>
       </c>
     </row>
     <row r="85" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7307,11 +7465,11 @@
         <v>14</v>
       </c>
       <c r="F104" s="1">
-        <f t="shared" ref="F104:M104" ca="1" si="17">F93-F105</f>
-        <v>3315917.48533053</v>
+        <f ca="1">OFFSET([1]aggregated_flows_exergy!B$52,196,0)-OFFSET([1]aggregated_flows_exergy!B$51,196,0)</f>
+        <v>2197045.0202281391</v>
       </c>
       <c r="G104" s="1">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ref="F104:M104" ca="1" si="17">G93-G105</f>
         <v>569528.78465562104</v>
       </c>
       <c r="H104" s="1">
@@ -7506,35 +7664,35 @@
       </c>
       <c r="F108" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$33,196,0)</f>
-        <v>70678670.3348234</v>
+        <v>57870337.913300298</v>
       </c>
       <c r="G108" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!C$33,196,0)</f>
-        <v>13914389.8740745</v>
+        <v>11392835.2083521</v>
       </c>
       <c r="H108" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!D$33,196,0)</f>
-        <v>47257120.678657196</v>
+        <v>38693222.856741801</v>
       </c>
       <c r="I108" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!E$33,196,0)</f>
-        <v>7122924.8182377601</v>
+        <v>5832114.0481239902</v>
       </c>
       <c r="J108" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!F$33,196,0)</f>
-        <v>2384234.9638538202</v>
+        <v>1952165.80008218</v>
       </c>
       <c r="K108" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$33,196,0)</f>
-        <v>33205372.740391199</v>
+        <v>27187921.503338601</v>
       </c>
       <c r="L108" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!H$33,196,0)</f>
-        <v>26269778.939317401</v>
+        <v>21509190.4944476</v>
       </c>
       <c r="M108" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!I$33,196,0)</f>
-        <v>11203518.655115001</v>
+        <v>9173225.9155138899</v>
       </c>
     </row>
     <row r="109" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -8438,11 +8596,11 @@
         <v>14</v>
       </c>
       <c r="F127" s="1">
-        <f t="shared" ref="F127:M127" ca="1" si="21">F116-F128</f>
-        <v>2579939.7216586601</v>
+        <f ca="1">OFFSET([1]aggregated_flows_exergy!B$52,250,0)-OFFSET([1]aggregated_flows_exergy!B$51,250,0)</f>
+        <v>1652882.0005122221</v>
       </c>
       <c r="G127" s="1">
-        <f t="shared" ca="1" si="21"/>
+        <f t="shared" ref="F127:M127" ca="1" si="21">G116-G128</f>
         <v>538607.76415555016</v>
       </c>
       <c r="H127" s="1">
@@ -8637,35 +8795,35 @@
       </c>
       <c r="F131" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$33,250,0)</f>
-        <v>56715896.063701302</v>
+        <v>46437886.785772704</v>
       </c>
       <c r="G131" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!C$33,250,0)</f>
-        <v>13076878.5585269</v>
+        <v>10707097.027266501</v>
       </c>
       <c r="H131" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!D$33,250,0)</f>
-        <v>35304167.136606999</v>
+        <v>28906374.344339099</v>
       </c>
       <c r="I131" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!E$33,250,0)</f>
-        <v>5944989.3436460197</v>
+        <v>4867643.10332892</v>
       </c>
       <c r="J131" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!F$33,250,0)</f>
-        <v>2389861.02492157</v>
+        <v>1956772.3108381</v>
       </c>
       <c r="K131" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$33,250,0)</f>
-        <v>22076688.0431557</v>
+        <v>18075968.491302099</v>
       </c>
       <c r="L131" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!H$33,250,0)</f>
-        <v>26404490.455758799</v>
+        <v>21619489.6970267</v>
       </c>
       <c r="M131" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!I$33,250,0)</f>
-        <v>8234717.5647872202</v>
+        <v>6742428.5974438898</v>
       </c>
     </row>
     <row r="132" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -9520,8 +9678,8 @@
         <v>14</v>
       </c>
       <c r="F149" s="1">
-        <f ca="1">OFFSET([1]aggregated_flows_exergy!B$37,250,0)</f>
-        <v>100510.32974474</v>
+        <f ca="1">OFFSET([1]aggregated_flows_exergy!B$37,304,0)</f>
+        <v>51285.1573181024</v>
       </c>
       <c r="G149" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!C$37,304,0)</f>
@@ -9569,11 +9727,11 @@
         <v>14</v>
       </c>
       <c r="F150" s="1">
-        <f t="shared" ref="F150:M150" ca="1" si="25">F139-F151</f>
-        <v>1607817.3618410798</v>
+        <f ca="1">OFFSET([1]aggregated_flows_exergy!B$52,304,0)-OFFSET([1]aggregated_flows_exergy!B$51,304,0)</f>
+        <v>1050266.4795077292</v>
       </c>
       <c r="G150" s="1">
-        <f t="shared" ca="1" si="25"/>
+        <f t="shared" ref="F150:M150" ca="1" si="25">G139-G151</f>
         <v>1343257.9746493902</v>
       </c>
       <c r="H150" s="1">
@@ -9768,35 +9926,35 @@
       </c>
       <c r="F154" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$33,304,0)</f>
-        <v>34707582.351323299</v>
+        <v>28417901.8834082</v>
       </c>
       <c r="G154" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!C$33,304,0)</f>
-        <v>29111863.0975594</v>
+        <v>23836234.422076199</v>
       </c>
       <c r="H154" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!D$33,304,0)</f>
-        <v>2406739.6460950701</v>
+        <v>1970592.20170749</v>
       </c>
       <c r="I154" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!E$33,304,0)</f>
-        <v>3168420.0912755001</v>
+        <v>2594241.5224393602</v>
       </c>
       <c r="J154" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!F$33,304,0)</f>
-        <v>20559.516393203099</v>
+        <v>16833.7371850993</v>
       </c>
       <c r="K154" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$33,304,0)</f>
-        <v>12024905.410964699</v>
+        <v>9845761.6167849507</v>
       </c>
       <c r="L154" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!H$33,304,0)</f>
-        <v>16526952.8940058</v>
+        <v>13531951.6357974</v>
       </c>
       <c r="M154" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!I$33,304,0)</f>
-        <v>6155724.0463526603</v>
+        <v>5040188.6308256797</v>
       </c>
     </row>
     <row r="155" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -10602,8 +10760,8 @@
         <v>14</v>
       </c>
       <c r="F171" s="1">
-        <f ca="1">OFFSET([1]aggregated_flows_exergy!B$27,304,0)-OFFSET([1]aggregated_flows_exergy!B$25,304,0)</f>
-        <v>374683.94077510608</v>
+        <f ca="1">OFFSET([1]aggregated_flows_exergy!B$27,358,0)-OFFSET([1]aggregated_flows_exergy!B$25,358,0)</f>
+        <v>552211.33448406984</v>
       </c>
       <c r="G171" s="1">
         <f t="shared" ref="G171:M171" ca="1" si="28">G168</f>
@@ -10700,11 +10858,11 @@
         <v>14</v>
       </c>
       <c r="F173" s="1">
-        <f t="shared" ref="F173:M173" ca="1" si="29">F162-F174</f>
-        <v>2118151.4635091601</v>
+        <f ca="1">OFFSET([1]aggregated_flows_exergy!B$52,358,0)-OFFSET([1]aggregated_flows_exergy!B$51,358,0)</f>
+        <v>1423429.3090673441</v>
       </c>
       <c r="G173" s="1">
-        <f t="shared" ca="1" si="29"/>
+        <f t="shared" ref="F173:M173" ca="1" si="29">G162-G174</f>
         <v>417860.39272822195</v>
       </c>
       <c r="H173" s="1">
@@ -10899,35 +11057,35 @@
       </c>
       <c r="F177" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$33,358,0)</f>
-        <v>48093546.9188288</v>
+        <v>39368160.996755503</v>
       </c>
       <c r="G177" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!C$33,358,0)</f>
-        <v>10404785.8210962</v>
+        <v>8516498.2028112002</v>
       </c>
       <c r="H177" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!D$33,358,0)</f>
-        <v>30915394.854255799</v>
+        <v>25306490.8437468</v>
       </c>
       <c r="I177" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!E$33,358,0)</f>
-        <v>5645480.2692780998</v>
+        <v>4621740.8767542196</v>
       </c>
       <c r="J177" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!F$33,358,0)</f>
-        <v>1127885.97419859</v>
+        <v>923431.07344337797</v>
       </c>
       <c r="K177" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$33,358,0)</f>
-        <v>22093516.357174601</v>
+        <v>18089746.895716101</v>
       </c>
       <c r="L177" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!H$33,358,0)</f>
-        <v>19642783.1618472</v>
+        <v>16083133.620776299</v>
       </c>
       <c r="M177" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!I$33,358,0)</f>
-        <v>6357247.3998068497</v>
+        <v>5195280.4802629203</v>
       </c>
     </row>
     <row r="178" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -10993,10 +11151,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M69"/>
+  <dimension ref="A1:O80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10:M10"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="Q68" sqref="Q68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -11952,7 +12110,7 @@
       </c>
       <c r="F20" s="2">
         <f ca="1">SUMIFS('Engines indvidual'!F$1:F$85,'Engines indvidual'!$B$1:$B$85,'Full system - simplified'!$B20,'Engines indvidual'!$D$1:$D$85,'Full system - simplified'!$D20,'Engines indvidual'!$E$1:$E$85,'Full system - simplified'!$E20)*0.000001</f>
-        <v>6.7558857411468587</v>
+        <v>4.6253079523142624</v>
       </c>
       <c r="G20" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$1:G$85,'Engines indvidual'!$B$1:$B$85,'Full system - simplified'!$B20,'Engines indvidual'!$D$1:$D$85,'Full system - simplified'!$D20,'Engines indvidual'!$E$1:$E$85,'Full system - simplified'!$E20)*0.000001</f>
@@ -12101,35 +12259,35 @@
       </c>
       <c r="F23" s="2">
         <f ca="1">SUMIFS('Engines indvidual'!F$1:F$85,'Engines indvidual'!$B$1:$B$85,'Full system - simplified'!$B23,'Engines indvidual'!$D$1:$D$85,'Full system - simplified'!$D23,'Engines indvidual'!$E$1:$E$85,'Full system - simplified'!$E23)*0.000001</f>
-        <v>324.89593443728648</v>
+        <v>266.01855161499009</v>
       </c>
       <c r="G23" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$1:G$85,'Engines indvidual'!$B$1:$B$85,'Full system - simplified'!$B23,'Engines indvidual'!$D$1:$D$85,'Full system - simplified'!$D23,'Engines indvidual'!$E$1:$E$85,'Full system - simplified'!$E23)*0.000001</f>
-        <v>0.46705364107948416</v>
+        <v>0.38241455172919286</v>
       </c>
       <c r="H23" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$1:H$85,'Engines indvidual'!$B$1:$B$85,'Full system - simplified'!$B23,'Engines indvidual'!$D$1:$D$85,'Full system - simplified'!$D23,'Engines indvidual'!$E$1:$E$85,'Full system - simplified'!$E23)*0.000001</f>
-        <v>259.2112287755005</v>
+        <v>212.23717606879009</v>
       </c>
       <c r="I23" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$1:I$85,'Engines indvidual'!$B$1:$B$85,'Full system - simplified'!$B23,'Engines indvidual'!$D$1:$D$85,'Full system - simplified'!$D23,'Engines indvidual'!$E$1:$E$85,'Full system - simplified'!$E23)*0.000001</f>
-        <v>31.082842688502708</v>
+        <v>25.450034659230639</v>
       </c>
       <c r="J23" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$1:J$85,'Engines indvidual'!$B$1:$B$85,'Full system - simplified'!$B23,'Engines indvidual'!$D$1:$D$85,'Full system - simplified'!$D23,'Engines indvidual'!$E$1:$E$85,'Full system - simplified'!$E23)*0.000001</f>
-        <v>34.134809332203943</v>
+        <v>27.948926335240159</v>
       </c>
       <c r="K23" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$1:K$85,'Engines indvidual'!$B$1:$B$85,'Full system - simplified'!$B23,'Engines indvidual'!$D$1:$D$85,'Full system - simplified'!$D23,'Engines indvidual'!$E$1:$E$85,'Full system - simplified'!$E23)*0.000001</f>
-        <v>128.41836687866589</v>
+        <v>105.14649257459118</v>
       </c>
       <c r="L23" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$1:L$85,'Engines indvidual'!$B$1:$B$85,'Full system - simplified'!$B23,'Engines indvidual'!$D$1:$D$85,'Full system - simplified'!$D23,'Engines indvidual'!$E$1:$E$85,'Full system - simplified'!$E23)*0.000001</f>
-        <v>139.47178450856981</v>
+        <v>114.19681865329531</v>
       </c>
       <c r="M23" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$1:M$85,'Engines indvidual'!$B$1:$B$85,'Full system - simplified'!$B23,'Engines indvidual'!$D$1:$D$85,'Full system - simplified'!$D23,'Engines indvidual'!$E$1:$E$85,'Full system - simplified'!$E23)*0.000001</f>
-        <v>57.005783050050297</v>
+        <v>46.675240387102797</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -12936,7 +13094,7 @@
       </c>
       <c r="F41" s="2">
         <f ca="1">SUMIFS('Engines indvidual'!F$87:F$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B41,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D41,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E41)*0.000001</f>
-        <v>2.0063645550916624</v>
+        <v>2.1838919488006261</v>
       </c>
       <c r="G41" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$87:G$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B41,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D41,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E41)*0.000001</f>
@@ -12985,7 +13143,7 @@
       </c>
       <c r="F42" s="2">
         <f ca="1">SUMIFS('Engines indvidual'!F$87:F$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B42,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D42,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E42)*0.000001</f>
-        <v>0.41813386860310636</v>
+        <v>0.36890869617646871</v>
       </c>
       <c r="G42" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$87:G$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B42,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D42,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E42)*0.000001</f>
@@ -13034,7 +13192,7 @@
       </c>
       <c r="F43" s="2">
         <f ca="1">SUMIFS('Engines indvidual'!F$87:F$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B43,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D43,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E43)*0.000001</f>
-        <v>9.6218260323394293</v>
+        <v>6.3236228093154345</v>
       </c>
       <c r="G43" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$87:G$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B43,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D43,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E43)*0.000001</f>
@@ -13232,35 +13390,35 @@
       </c>
       <c r="F47" s="2">
         <f ca="1">SUMIFS('Engines indvidual'!F$87:F$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B47,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D47,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E47)*0.000001</f>
-        <v>162.102148749848</v>
+        <v>132.72612658248119</v>
       </c>
       <c r="G47" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$87:G$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B47,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D47,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E47)*0.000001</f>
-        <v>56.103131530160795</v>
+        <v>45.936166657694798</v>
       </c>
       <c r="H47" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$87:H$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B47,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D47,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E47)*0.000001</f>
-        <v>84.968027461359256</v>
+        <v>69.570189402788401</v>
       </c>
       <c r="I47" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$87:I$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B47,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D47,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E47)*0.000001</f>
-        <v>16.236334253159278</v>
+        <v>13.29399867389227</v>
       </c>
       <c r="J47" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$87:J$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B47,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D47,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E47)*0.000001</f>
-        <v>4.7946555051685928</v>
+        <v>3.9257718481053794</v>
       </c>
       <c r="K47" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$87:K$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B47,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D47,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E47)*0.000001</f>
-        <v>67.306966194511588</v>
+        <v>55.109651611425647</v>
       </c>
       <c r="L47" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$87:L$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B47,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D47,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E47)*0.000001</f>
-        <v>69.201222289081997</v>
+        <v>56.6606318272717</v>
       </c>
       <c r="M47" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$87:M$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B47,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D47,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E47)*0.000001</f>
-        <v>25.593960266254879</v>
+        <v>20.955843143783458</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -13314,7 +13472,7 @@
         <v>7.3582583418218611E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>16</v>
       </c>
@@ -13363,7 +13521,7 @@
         <v>2.077945747621762</v>
       </c>
     </row>
-    <row r="51" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>16</v>
       </c>
@@ -13411,8 +13569,9 @@
         <f>([1]aggregated_flows_exergy!I$479-[1]aggregated_flows_exergy!I$482)*0.000001</f>
         <v>0.38136869532173989</v>
       </c>
-    </row>
-    <row r="52" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O51" s="2"/>
+    </row>
+    <row r="52" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>25</v>
       </c>
@@ -13460,8 +13619,9 @@
         <f>([1]aggregated_flows_exergy!I$498-[1]aggregated_flows_exergy!I$499)*0.000001</f>
         <v>0.53517502904116687</v>
       </c>
-    </row>
-    <row r="53" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O52" s="2"/>
+    </row>
+    <row r="53" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>25</v>
       </c>
@@ -13510,7 +13670,7 @@
         <v>9.5557648005575868E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>25</v>
       </c>
@@ -13559,7 +13719,7 @@
         <v>2.7157666356389398E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>25</v>
       </c>
@@ -13570,45 +13730,45 @@
         <v>25</v>
       </c>
       <c r="D55" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="E55" t="s">
         <v>55</v>
       </c>
       <c r="F55" s="2">
         <f>([1]aggregated_flows_exergy!B$507+[1]aggregated_flows_exergy!B$508)*0.000001</f>
-        <v>24.569303094623304</v>
+        <v>20.117866488576606</v>
       </c>
       <c r="G55" s="2">
         <f>([1]aggregated_flows_exergy!C$507+[1]aggregated_flows_exergy!C$508)*0.000001</f>
-        <v>17.545390051447367</v>
+        <v>14.366347045194765</v>
       </c>
       <c r="H55" s="2">
         <f>([1]aggregated_flows_exergy!D$507+[1]aggregated_flows_exergy!D$508)*0.000001</f>
-        <v>5.7757241790302363</v>
+        <v>4.7294446889793562</v>
       </c>
       <c r="I55" s="2">
         <f>([1]aggregated_flows_exergy!E$507+[1]aggregated_flows_exergy!E$508)*0.000001</f>
-        <v>1.2408035532605208</v>
+        <v>1.0160273968301607</v>
       </c>
       <c r="J55" s="2">
         <f>([1]aggregated_flows_exergy!F$507+[1]aggregated_flows_exergy!F$508)*0.000001</f>
-        <v>7.3853108847774717E-3</v>
+        <v>6.0473575726920021E-3</v>
       </c>
       <c r="K55" s="2">
         <f>([1]aggregated_flows_exergy!G$507+[1]aggregated_flows_exergy!G$508)*0.000001</f>
-        <v>15.858721929516458</v>
+        <v>12.985525599104458</v>
       </c>
       <c r="L55" s="2">
         <f>([1]aggregated_flows_exergy!H$507+[1]aggregated_flows_exergy!H$508)*0.000001</f>
-        <v>8.2544230421436922</v>
+        <v>6.7588377222507026</v>
       </c>
       <c r="M55" s="2">
         <f>([1]aggregated_flows_exergy!I$507+[1]aggregated_flows_exergy!I$508)*0.000001</f>
-        <v>0.45615812296268216</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>0.37350316722172117</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>25</v>
       </c>
@@ -13625,8 +13785,8 @@
         <v>14</v>
       </c>
       <c r="F56" s="2">
-        <f>[1]aggregated_flows_exergy!B$571*0.000001</f>
-        <v>3.4069030093520496</v>
+        <f>([1]aggregated_flows_exergy!B$492 - [1]aggregated_flows_exergy!B$493)*0.000001</f>
+        <v>7.4317280550554017</v>
       </c>
       <c r="G56" s="2">
         <f>[1]aggregated_flows_exergy!C$571*0.000001</f>
@@ -13657,7 +13817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>25</v>
       </c>
@@ -13674,8 +13834,8 @@
         <v>14</v>
       </c>
       <c r="F57" s="2">
-        <f>[1]aggregated_flows_exergy!B$572*0.000001</f>
-        <v>0.27643994972985997</v>
+        <f>([1]aggregated_flows_exergy!B$495 - [1]aggregated_flows_exergy!B$496)*0.000001</f>
+        <v>0.33065251501618892</v>
       </c>
       <c r="G57" s="2">
         <f>[1]aggregated_flows_exergy!C$572*0.000001</f>
@@ -13706,7 +13866,7 @@
         <v>0.27643994972985997</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>25</v>
       </c>
@@ -13723,8 +13883,8 @@
         <v>14</v>
       </c>
       <c r="F58" s="2">
-        <f>[1]aggregated_flows_exergy!B$570*0.000001</f>
-        <v>1.9583056043579798</v>
+        <f>([1]aggregated_flows_exergy!B$502 - [1]aggregated_flows_exergy!B$503)*0.000001</f>
+        <v>2.27277994866053</v>
       </c>
       <c r="G58" s="2">
         <f>[1]aggregated_flows_exergy!C$570*0.000001</f>
@@ -13755,7 +13915,7 @@
         <v>0.30529679934687598</v>
       </c>
     </row>
-    <row r="59" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>25</v>
       </c>
@@ -13772,8 +13932,8 @@
         <v>14</v>
       </c>
       <c r="F59" s="2">
-        <f>[1]aggregated_flows_exergy!B$576*0.000001</f>
-        <v>0.17739045768655498</v>
+        <f>([1]aggregated_flows_exergy!B$538 - [1]aggregated_flows_exergy!B$527)*0.000001</f>
+        <v>0.68484724208805892</v>
       </c>
       <c r="G59" s="2">
         <f>[1]aggregated_flows_exergy!C$576*0.000001</f>
@@ -13804,7 +13964,7 @@
         <v>1.6875526365414801E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>25</v>
       </c>
@@ -13821,8 +13981,8 @@
         <v>14</v>
       </c>
       <c r="F60" s="2">
-        <f>[1]aggregated_flows_exergy!B$575*0.000001</f>
-        <v>0.36513430088944998</v>
+        <f>([1]aggregated_flows_exergy!B$539 - [1]aggregated_flows_exergy!B$528)*0.000001</f>
+        <v>0.66038841201349208</v>
       </c>
       <c r="G60" s="2">
         <f>[1]aggregated_flows_exergy!C$575*0.000001</f>
@@ -13853,7 +14013,7 @@
         <v>4.4233127071141499E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>25</v>
       </c>
@@ -13870,8 +14030,8 @@
         <v>14</v>
       </c>
       <c r="F61" s="2">
-        <f>[1]aggregated_flows_exergy!B$577*0.000001</f>
-        <v>0.29389645906742901</v>
+        <f>([1]aggregated_flows_exergy!B$540 - [1]aggregated_flows_exergy!B$529)*0.000001</f>
+        <v>0.44326990732632549</v>
       </c>
       <c r="G61" s="2">
         <f>[1]aggregated_flows_exergy!C$577*0.000001</f>
@@ -13902,7 +14062,7 @@
         <v>4.3799125134392193E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>25</v>
       </c>
@@ -13919,8 +14079,8 @@
         <v>14</v>
       </c>
       <c r="F62" s="2">
-        <f>[1]aggregated_flows_exergy!B$573*0.000001</f>
-        <v>0.22964173896057499</v>
+        <f>([1]aggregated_flows_exergy!B$537 - [1]aggregated_flows_exergy!B$526)*0.000001</f>
+        <v>0.51363543156605107</v>
       </c>
       <c r="G62" s="2">
         <f>[1]aggregated_flows_exergy!C$573*0.000001</f>
@@ -13951,7 +14111,7 @@
         <v>2.65733019179623E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>25</v>
       </c>
@@ -13968,8 +14128,8 @@
         <v>14</v>
       </c>
       <c r="F63" s="2">
-        <f>[1]aggregated_flows_exergy!B$578*0.000001</f>
-        <v>1.5930956022585399</v>
+        <f>([1]aggregated_flows_exergy!B$541 - [1]aggregated_flows_exergy!B$530)*0.000001</f>
+        <v>2.4495675161803629</v>
       </c>
       <c r="G63" s="2">
         <f>[1]aggregated_flows_exergy!C$578*0.000001</f>
@@ -14000,7 +14160,7 @@
         <v>0.19045034132130198</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>25</v>
       </c>
@@ -14017,8 +14177,8 @@
         <v>14</v>
       </c>
       <c r="F64" s="2">
-        <f>[1]aggregated_flows_exergy!B$573*0.000001</f>
-        <v>0.22964173896057499</v>
+        <f>([1]aggregated_flows_exergy!B$543 - [1]aggregated_flows_exergy!B$532)*0.000001</f>
+        <v>0.34242362104402907</v>
       </c>
       <c r="G64" s="2">
         <f>[1]aggregated_flows_exergy!C$573*0.000001</f>
@@ -14292,6 +14452,469 @@
       <c r="M69" s="2">
         <f t="shared" ca="1" si="1"/>
         <v>0.57312888533829209</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>25</v>
+      </c>
+      <c r="B70" t="s">
+        <v>26</v>
+      </c>
+      <c r="C70" t="s">
+        <v>3</v>
+      </c>
+      <c r="D70" t="s">
+        <v>57</v>
+      </c>
+      <c r="E70" t="s">
+        <v>14</v>
+      </c>
+      <c r="F70" s="2">
+        <f>[1]aggregated_flows_exergy!B$533*0.000001</f>
+        <v>0.80655419849585186</v>
+      </c>
+      <c r="G70" s="2">
+        <f>[1]aggregated_flows_exergy!C$533*0.000001</f>
+        <v>3.9129252321069598E-3</v>
+      </c>
+      <c r="H70" s="2">
+        <f>[1]aggregated_flows_exergy!D$533*0.000001</f>
+        <v>0.42573842593756595</v>
+      </c>
+      <c r="I70" s="2">
+        <f>[1]aggregated_flows_exergy!E$533*0.000001</f>
+        <v>0.12687938055836198</v>
+      </c>
+      <c r="J70" s="2">
+        <f>[1]aggregated_flows_exergy!F$533*0.000001</f>
+        <v>0.250023466767818</v>
+      </c>
+      <c r="K70" s="2">
+        <f>[1]aggregated_flows_exergy!G$533*0.000001</f>
+        <v>5.3673321406558699E-2</v>
+      </c>
+      <c r="L70" s="2">
+        <f>[1]aggregated_flows_exergy!H$533*0.000001</f>
+        <v>0.19971323018027098</v>
+      </c>
+      <c r="M70" s="2">
+        <f>[1]aggregated_flows_exergy!I$533*0.000001</f>
+        <v>0.55316764690902498</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B72" t="s">
+        <v>41</v>
+      </c>
+      <c r="C72" t="s">
+        <v>40</v>
+      </c>
+      <c r="D72" t="s">
+        <v>56</v>
+      </c>
+      <c r="E72" t="s">
+        <v>14</v>
+      </c>
+      <c r="F72" s="2">
+        <f>[1]aggregated_flows_exergy!B$571*0.000001</f>
+        <v>3.4069030093520496</v>
+      </c>
+      <c r="G72" s="2">
+        <f>[1]aggregated_flows_exergy!C$571*0.000001</f>
+        <v>1.2194992725623299</v>
+      </c>
+      <c r="H72" s="2">
+        <f>[1]aggregated_flows_exergy!D$571*0.000001</f>
+        <v>1.8935791158047999</v>
+      </c>
+      <c r="I72" s="2">
+        <f>[1]aggregated_flows_exergy!E$571*0.000001</f>
+        <v>0.246404928112197</v>
+      </c>
+      <c r="J72" s="2">
+        <f>[1]aggregated_flows_exergy!F$571*0.000001</f>
+        <v>4.7419692872702396E-2</v>
+      </c>
+      <c r="K72" s="2">
+        <f>[1]aggregated_flows_exergy!G$571*0.000001</f>
+        <v>2.2944500609015397</v>
+      </c>
+      <c r="L72" s="2">
+        <f>[1]aggregated_flows_exergy!H$571*0.000001</f>
+        <v>1.1124529484505099</v>
+      </c>
+      <c r="M72" s="2">
+        <f>[1]aggregated_flows_exergy!I$571*0.000001</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B73" t="s">
+        <v>42</v>
+      </c>
+      <c r="C73" t="s">
+        <v>40</v>
+      </c>
+      <c r="D73" t="s">
+        <v>56</v>
+      </c>
+      <c r="E73" t="s">
+        <v>14</v>
+      </c>
+      <c r="F73" s="2">
+        <f>[1]aggregated_flows_exergy!B$572*0.000001</f>
+        <v>0.27643994972985997</v>
+      </c>
+      <c r="G73" s="2">
+        <f>[1]aggregated_flows_exergy!C$572*0.000001</f>
+        <v>9.06263288582497E-2</v>
+      </c>
+      <c r="H73" s="2">
+        <f>[1]aggregated_flows_exergy!D$572*0.000001</f>
+        <v>0.13064685866679099</v>
+      </c>
+      <c r="I73" s="2">
+        <f>[1]aggregated_flows_exergy!E$572*0.000001</f>
+        <v>2.7867139357235397E-2</v>
+      </c>
+      <c r="J73" s="2">
+        <f>[1]aggregated_flows_exergy!F$572*0.000001</f>
+        <v>2.72996228475842E-2</v>
+      </c>
+      <c r="K73" s="2">
+        <f>[1]aggregated_flows_exergy!G$572*0.000001</f>
+        <v>0</v>
+      </c>
+      <c r="L73" s="2">
+        <f>[1]aggregated_flows_exergy!H$572*0.000001</f>
+        <v>0</v>
+      </c>
+      <c r="M73" s="2">
+        <f>[1]aggregated_flows_exergy!I$572*0.000001</f>
+        <v>0.27643994972985997</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B74" t="s">
+        <v>43</v>
+      </c>
+      <c r="C74" t="s">
+        <v>40</v>
+      </c>
+      <c r="D74" t="s">
+        <v>56</v>
+      </c>
+      <c r="E74" t="s">
+        <v>14</v>
+      </c>
+      <c r="F74" s="2">
+        <f>[1]aggregated_flows_exergy!B$570*0.000001</f>
+        <v>1.9583056043579798</v>
+      </c>
+      <c r="G74" s="2">
+        <f>[1]aggregated_flows_exergy!C$570*0.000001</f>
+        <v>0.63937363885036791</v>
+      </c>
+      <c r="H74" s="2">
+        <f>[1]aggregated_flows_exergy!D$570*0.000001</f>
+        <v>1.09161802930435</v>
+      </c>
+      <c r="I74" s="2">
+        <f>[1]aggregated_flows_exergy!E$570*0.000001</f>
+        <v>0.17453951207662799</v>
+      </c>
+      <c r="J74" s="2">
+        <f>[1]aggregated_flows_exergy!F$570*0.000001</f>
+        <v>5.27744241266737E-2</v>
+      </c>
+      <c r="K74" s="2">
+        <f>[1]aggregated_flows_exergy!G$570*0.000001</f>
+        <v>0.84126451599489493</v>
+      </c>
+      <c r="L74" s="2">
+        <f>[1]aggregated_flows_exergy!H$570*0.000001</f>
+        <v>0.81174428901624096</v>
+      </c>
+      <c r="M74" s="2">
+        <f>[1]aggregated_flows_exergy!I$570*0.000001</f>
+        <v>0.30529679934687598</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B75" t="s">
+        <v>44</v>
+      </c>
+      <c r="C75" t="s">
+        <v>40</v>
+      </c>
+      <c r="D75" t="s">
+        <v>56</v>
+      </c>
+      <c r="E75" t="s">
+        <v>14</v>
+      </c>
+      <c r="F75" s="2">
+        <f>[1]aggregated_flows_exergy!B$576*0.000001</f>
+        <v>0.17739045768655498</v>
+      </c>
+      <c r="G75" s="2">
+        <f>[1]aggregated_flows_exergy!C$576*0.000001</f>
+        <v>6.2239265787400994E-2</v>
+      </c>
+      <c r="H75" s="2">
+        <f>[1]aggregated_flows_exergy!D$576*0.000001</f>
+        <v>9.6608521996453894E-2</v>
+      </c>
+      <c r="I75" s="2">
+        <f>[1]aggregated_flows_exergy!E$576*0.000001</f>
+        <v>1.43407038077223E-2</v>
+      </c>
+      <c r="J75" s="2">
+        <f>[1]aggregated_flows_exergy!F$576*0.000001</f>
+        <v>4.2019660949773399E-3</v>
+      </c>
+      <c r="K75" s="2">
+        <f>[1]aggregated_flows_exergy!G$576*0.000001</f>
+        <v>8.848073737441349E-2</v>
+      </c>
+      <c r="L75" s="2">
+        <f>[1]aggregated_flows_exergy!H$576*0.000001</f>
+        <v>7.2034193946725986E-2</v>
+      </c>
+      <c r="M75" s="2">
+        <f>[1]aggregated_flows_exergy!I$576*0.000001</f>
+        <v>1.6875526365414801E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B76" t="s">
+        <v>45</v>
+      </c>
+      <c r="C76" t="s">
+        <v>40</v>
+      </c>
+      <c r="D76" t="s">
+        <v>56</v>
+      </c>
+      <c r="E76" t="s">
+        <v>14</v>
+      </c>
+      <c r="F76" s="2">
+        <f>[1]aggregated_flows_exergy!B$575*0.000001</f>
+        <v>0.36513430088944998</v>
+      </c>
+      <c r="G76" s="2">
+        <f>[1]aggregated_flows_exergy!C$575*0.000001</f>
+        <v>0.12762239469109099</v>
+      </c>
+      <c r="H76" s="2">
+        <f>[1]aggregated_flows_exergy!D$575*0.000001</f>
+        <v>0.19749372237287499</v>
+      </c>
+      <c r="I76" s="2">
+        <f>[1]aggregated_flows_exergy!E$575*0.000001</f>
+        <v>3.0310478440709498E-2</v>
+      </c>
+      <c r="J76" s="2">
+        <f>[1]aggregated_flows_exergy!F$575*0.000001</f>
+        <v>9.7077053847736891E-3</v>
+      </c>
+      <c r="K76" s="2">
+        <f>[1]aggregated_flows_exergy!G$575*0.000001</f>
+        <v>0.163130953549875</v>
+      </c>
+      <c r="L76" s="2">
+        <f>[1]aggregated_flows_exergy!H$575*0.000001</f>
+        <v>0.15777022026843199</v>
+      </c>
+      <c r="M76" s="2">
+        <f>[1]aggregated_flows_exergy!I$575*0.000001</f>
+        <v>4.4233127071141499E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B77" t="s">
+        <v>46</v>
+      </c>
+      <c r="C77" t="s">
+        <v>40</v>
+      </c>
+      <c r="D77" t="s">
+        <v>56</v>
+      </c>
+      <c r="E77" t="s">
+        <v>14</v>
+      </c>
+      <c r="F77" s="2">
+        <f>[1]aggregated_flows_exergy!B$577*0.000001</f>
+        <v>0.29389645906742901</v>
+      </c>
+      <c r="G77" s="2">
+        <f>[1]aggregated_flows_exergy!C$577*0.000001</f>
+        <v>3.6964912978471001E-2</v>
+      </c>
+      <c r="H77" s="2">
+        <f>[1]aggregated_flows_exergy!D$577*0.000001</f>
+        <v>0.20780884410724598</v>
+      </c>
+      <c r="I77" s="2">
+        <f>[1]aggregated_flows_exergy!E$577*0.000001</f>
+        <v>2.8580759289889502E-2</v>
+      </c>
+      <c r="J77" s="2">
+        <f>[1]aggregated_flows_exergy!F$577*0.000001</f>
+        <v>2.0541942691823498E-2</v>
+      </c>
+      <c r="K77" s="2">
+        <f>[1]aggregated_flows_exergy!G$577*0.000001</f>
+        <v>0.128599540424509</v>
+      </c>
+      <c r="L77" s="2">
+        <f>[1]aggregated_flows_exergy!H$577*0.000001</f>
+        <v>0.121497793508528</v>
+      </c>
+      <c r="M77" s="2">
+        <f>[1]aggregated_flows_exergy!I$577*0.000001</f>
+        <v>4.3799125134392193E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B78" t="s">
+        <v>47</v>
+      </c>
+      <c r="C78" t="s">
+        <v>40</v>
+      </c>
+      <c r="D78" t="s">
+        <v>56</v>
+      </c>
+      <c r="E78" t="s">
+        <v>14</v>
+      </c>
+      <c r="F78" s="2">
+        <f>[1]aggregated_flows_exergy!B$573*0.000001</f>
+        <v>0.22964173896057499</v>
+      </c>
+      <c r="G78" s="2">
+        <f>[1]aggregated_flows_exergy!C$573*0.000001</f>
+        <v>8.0328910487552904E-2</v>
+      </c>
+      <c r="H78" s="2">
+        <f>[1]aggregated_flows_exergy!D$573*0.000001</f>
+        <v>0.12438722010898599</v>
+      </c>
+      <c r="I78" s="2">
+        <f>[1]aggregated_flows_exergy!E$573*0.000001</f>
+        <v>1.8959072180331899E-2</v>
+      </c>
+      <c r="J78" s="2">
+        <f>[1]aggregated_flows_exergy!F$573*0.000001</f>
+        <v>5.9665361837027402E-3</v>
+      </c>
+      <c r="K78" s="2">
+        <f>[1]aggregated_flows_exergy!G$573*0.000001</f>
+        <v>0.105088983763517</v>
+      </c>
+      <c r="L78" s="2">
+        <f>[1]aggregated_flows_exergy!H$573*0.000001</f>
+        <v>9.7979453279093298E-2</v>
+      </c>
+      <c r="M78" s="2">
+        <f>[1]aggregated_flows_exergy!I$573*0.000001</f>
+        <v>2.65733019179623E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B79" t="s">
+        <v>48</v>
+      </c>
+      <c r="C79" t="s">
+        <v>40</v>
+      </c>
+      <c r="D79" t="s">
+        <v>56</v>
+      </c>
+      <c r="E79" t="s">
+        <v>14</v>
+      </c>
+      <c r="F79" s="2">
+        <f>[1]aggregated_flows_exergy!B$578*0.000001</f>
+        <v>1.5930956022585399</v>
+      </c>
+      <c r="G79" s="2">
+        <f>[1]aggregated_flows_exergy!C$578*0.000001</f>
+        <v>0.43963520161171799</v>
+      </c>
+      <c r="H79" s="2">
+        <f>[1]aggregated_flows_exergy!D$578*0.000001</f>
+        <v>0.97548546689526094</v>
+      </c>
+      <c r="I79" s="2">
+        <f>[1]aggregated_flows_exergy!E$578*0.000001</f>
+        <v>0.14226219825891501</v>
+      </c>
+      <c r="J79" s="2">
+        <f>[1]aggregated_flows_exergy!F$578*0.000001</f>
+        <v>3.57127354926456E-2</v>
+      </c>
+      <c r="K79" s="2">
+        <f>[1]aggregated_flows_exergy!G$578*0.000001</f>
+        <v>0.71349585107152691</v>
+      </c>
+      <c r="L79" s="2">
+        <f>[1]aggregated_flows_exergy!H$578*0.000001</f>
+        <v>0.68914940986570206</v>
+      </c>
+      <c r="M79" s="2">
+        <f>[1]aggregated_flows_exergy!I$578*0.000001</f>
+        <v>0.19045034132130198</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B80" t="s">
+        <v>49</v>
+      </c>
+      <c r="C80" t="s">
+        <v>40</v>
+      </c>
+      <c r="D80" t="s">
+        <v>56</v>
+      </c>
+      <c r="E80" t="s">
+        <v>14</v>
+      </c>
+      <c r="F80" s="2">
+        <f>[1]aggregated_flows_exergy!B$574*0.000001</f>
+        <v>0.153094492640383</v>
+      </c>
+      <c r="G80" s="2">
+        <f>[1]aggregated_flows_exergy!C$574*0.000001</f>
+        <v>5.3552606991701994E-2</v>
+      </c>
+      <c r="H80" s="2">
+        <f>[1]aggregated_flows_exergy!D$574*0.000001</f>
+        <v>8.2924813405991699E-2</v>
+      </c>
+      <c r="I80" s="2">
+        <f>[1]aggregated_flows_exergy!E$574*0.000001</f>
+        <v>1.26393814535546E-2</v>
+      </c>
+      <c r="J80" s="2">
+        <f>[1]aggregated_flows_exergy!F$574*0.000001</f>
+        <v>3.9776907891351694E-3</v>
+      </c>
+      <c r="K80" s="2">
+        <f>[1]aggregated_flows_exergy!G$574*0.000001</f>
+        <v>7.0059322509012395E-2</v>
+      </c>
+      <c r="L80" s="2">
+        <f>[1]aggregated_flows_exergy!H$574*0.000001</f>
+        <v>6.5319635519396096E-2</v>
+      </c>
+      <c r="M80" s="2">
+        <f>[1]aggregated_flows_exergy!I$574*0.000001</f>
+        <v>1.7715534611974899E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Exergy AE fuel correction
Now it should work, goddammit
</commit_message>
<xml_diff>
--- a/Results/inputGrassmann.xlsx
+++ b/Results/inputGrassmann.xlsx
@@ -1349,28 +1349,28 @@
         </row>
         <row r="479">
           <cell r="B479">
-            <v>25290292.087912701</v>
+            <v>25290716.1527449</v>
           </cell>
           <cell r="C479">
-            <v>8183424.6592828603</v>
+            <v>8183609.8454913702</v>
           </cell>
           <cell r="D479">
-            <v>14551155.9824367</v>
+            <v>14551378.661381301</v>
           </cell>
           <cell r="E479">
-            <v>2000674.7769207</v>
+            <v>2000690.4713797499</v>
           </cell>
           <cell r="F479">
-            <v>555036.66927229904</v>
+            <v>555037.17449239804</v>
           </cell>
           <cell r="G479">
-            <v>14880632.387743199</v>
+            <v>14880633.0348625</v>
           </cell>
           <cell r="H479">
-            <v>8790227.6145967804</v>
+            <v>8790276.2725442592</v>
           </cell>
           <cell r="I479">
-            <v>1619432.0855726299</v>
+            <v>1619806.8453380801</v>
           </cell>
         </row>
         <row r="482">
@@ -1421,54 +1421,54 @@
         </row>
         <row r="498">
           <cell r="B498">
-            <v>12778609.189100301</v>
+            <v>12777750.0833482</v>
           </cell>
           <cell r="C498">
-            <v>5807360.4015310397</v>
+            <v>5806975.7929284004</v>
           </cell>
           <cell r="D498">
-            <v>5983411.3406982003</v>
+            <v>5982969.3711697096</v>
           </cell>
           <cell r="E498">
-            <v>881969.00801966595</v>
+            <v>881937.43372342095</v>
           </cell>
           <cell r="F498">
-            <v>105868.438851534</v>
+            <v>105867.48552670699</v>
           </cell>
           <cell r="G498">
-            <v>7689466.3215588601</v>
+            <v>7689465.0257392898</v>
           </cell>
           <cell r="H498">
-            <v>4468202.7455613203</v>
+            <v>4468102.3556815702</v>
           </cell>
           <cell r="I498">
-            <v>620940.12198026397</v>
+            <v>620182.70192738797</v>
           </cell>
         </row>
         <row r="499">
           <cell r="B499">
-            <v>1908032.45991977</v>
+            <v>1907911.5421368999</v>
           </cell>
           <cell r="C499">
-            <v>865498.17287425802</v>
+            <v>865443.97320277104</v>
           </cell>
           <cell r="D499">
-            <v>895648.65146392502</v>
+            <v>895586.55460169504</v>
           </cell>
           <cell r="E499">
-            <v>131158.04912547101</v>
+            <v>131153.56581102801</v>
           </cell>
           <cell r="F499">
-            <v>15727.586456110999</v>
+            <v>15727.448521395199</v>
           </cell>
           <cell r="G499">
-            <v>1174551.9956528901</v>
+            <v>1174551.79884191</v>
           </cell>
           <cell r="H499">
-            <v>647715.37132777902</v>
+            <v>647700.81869261002</v>
           </cell>
           <cell r="I499">
-            <v>85765.0929390971</v>
+            <v>85658.924602362997</v>
           </cell>
         </row>
         <row r="502">
@@ -1587,28 +1587,28 @@
         </row>
         <row r="510">
           <cell r="B510">
-            <v>19558135.423810601</v>
+            <v>19558097.134771701</v>
           </cell>
           <cell r="C510">
-            <v>7570370.2171184896</v>
+            <v>7569989.6122350805</v>
           </cell>
           <cell r="D510">
-            <v>9924112.0817571208</v>
+            <v>9924376.3903761599</v>
           </cell>
           <cell r="E510">
-            <v>1533495.57777747</v>
+            <v>1533573.4551047599</v>
           </cell>
           <cell r="F510">
-            <v>530157.54715742799</v>
+            <v>530157.67705560895</v>
           </cell>
           <cell r="G510">
-            <v>10327507.3938511</v>
+            <v>10327507.3859796</v>
           </cell>
           <cell r="H510">
-            <v>7281463.7215595497</v>
+            <v>7281463.7345353505</v>
           </cell>
           <cell r="I510">
-            <v>1949164.3083997399</v>
+            <v>1949126.01425656</v>
           </cell>
         </row>
         <row r="511">
@@ -1639,19 +1639,19 @@
         </row>
         <row r="516">
           <cell r="B516">
-            <v>1670406.5529900601</v>
+            <v>1670367.0534334299</v>
           </cell>
           <cell r="C516">
-            <v>329912.15759257699</v>
+            <v>329901.24579902901</v>
           </cell>
           <cell r="D516">
-            <v>1105981.9623406499</v>
+            <v>1105956.8007104199</v>
           </cell>
           <cell r="E516">
-            <v>197777.69542538599</v>
+            <v>197774.43004563701</v>
           </cell>
           <cell r="F516">
-            <v>36734.7376314594</v>
+            <v>36734.576878359498</v>
           </cell>
           <cell r="G516">
             <v>846005.47359948198</v>
@@ -1660,7 +1660,7 @@
             <v>605824.08663059596</v>
           </cell>
           <cell r="I516">
-            <v>218576.99275999799</v>
+            <v>218537.49320337101</v>
           </cell>
         </row>
         <row r="526">
@@ -1680,7 +1680,7 @@
         </row>
         <row r="529">
           <cell r="B529">
-            <v>76353.148832306499</v>
+            <v>76355.014271591106</v>
           </cell>
         </row>
         <row r="530">
@@ -1695,28 +1695,28 @@
         </row>
         <row r="533">
           <cell r="B533">
-            <v>806554.19849585195</v>
+            <v>807361.72195589298</v>
           </cell>
           <cell r="C533">
-            <v>3912.9252321069598</v>
+            <v>3913.2575424330698</v>
           </cell>
           <cell r="D533">
-            <v>425738.42593756597</v>
+            <v>426436.06333583198</v>
           </cell>
           <cell r="E533">
-            <v>126879.380558362</v>
+            <v>126987.932678293</v>
           </cell>
           <cell r="F533">
-            <v>250023.466767818</v>
+            <v>250024.46839933499</v>
           </cell>
           <cell r="G533">
-            <v>53673.321406558702</v>
+            <v>53674.609794178003</v>
           </cell>
           <cell r="H533">
-            <v>199713.230180271</v>
+            <v>199813.633035826</v>
           </cell>
           <cell r="I533">
-            <v>553167.64690902503</v>
+            <v>553873.47912588995</v>
           </cell>
         </row>
         <row r="537">
@@ -1736,7 +1736,7 @@
         </row>
         <row r="540">
           <cell r="B540">
-            <v>519623.05615863198</v>
+            <v>519636.34941190202</v>
           </cell>
         </row>
         <row r="541">
@@ -2063,28 +2063,28 @@
         </row>
         <row r="577">
           <cell r="B577">
-            <v>293896.45906742901</v>
+            <v>293903.75942200801</v>
           </cell>
           <cell r="C577">
-            <v>36964.912978471002</v>
+            <v>36966.927817431002</v>
           </cell>
           <cell r="D577">
-            <v>207808.844107246</v>
+            <v>207813.59028674199</v>
           </cell>
           <cell r="E577">
-            <v>28580.759289889502</v>
+            <v>28581.253586087001</v>
           </cell>
           <cell r="F577">
-            <v>20541.9426918235</v>
+            <v>20541.987731748901</v>
           </cell>
           <cell r="G577">
-            <v>128599.540424509</v>
+            <v>128599.540169755</v>
           </cell>
           <cell r="H577">
             <v>121497.793508528</v>
           </cell>
           <cell r="I577">
-            <v>43799.125134392198</v>
+            <v>43806.425743724998</v>
           </cell>
         </row>
         <row r="578">
@@ -2384,7 +2384,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P178"/>
   <sheetViews>
-    <sheetView topLeftCell="A174" workbookViewId="0">
+    <sheetView topLeftCell="A165" workbookViewId="0">
       <selection activeCell="E218" sqref="E218"/>
     </sheetView>
   </sheetViews>
@@ -3737,7 +3737,7 @@
       </c>
       <c r="J27" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!F$11,47,0)</f>
-        <v>1792053.8481864401</v>
+        <v>1792053.8481864301</v>
       </c>
       <c r="K27" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$11,47,0)</f>
@@ -4312,7 +4312,7 @@
         <v>2439757.8806079971</v>
       </c>
       <c r="G39" s="1">
-        <f t="shared" ref="F39:M39" ca="1" si="6">G28-G40</f>
+        <f t="shared" ref="G39:M39" ca="1" si="6">G28-G40</f>
         <v>3869.4917156394704</v>
       </c>
       <c r="H39" s="1">
@@ -5394,7 +5394,7 @@
         <v>2185550.0717062652</v>
       </c>
       <c r="G61" s="1">
-        <f t="shared" ref="F61:M61" ca="1" si="10">G50-G62</f>
+        <f t="shared" ref="G61:M61" ca="1" si="10">G50-G62</f>
         <v>4414.1165117695091</v>
       </c>
       <c r="H61" s="1">
@@ -5905,7 +5905,7 @@
       </c>
       <c r="K71" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$11,149,0)</f>
-        <v>5318984.4904121002</v>
+        <v>5318984.49041209</v>
       </c>
       <c r="L71" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!H$11,149,0)</f>
@@ -7123,7 +7123,7 @@
       </c>
       <c r="F97" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$19,196,0)-OFFSET([1]aggregated_flows_exergy!B$17,196,0)</f>
-        <v>65950.880138600245</v>
+        <v>65951.157412899658</v>
       </c>
       <c r="G97" s="1">
         <f t="shared" ref="G97:M98" ca="1" si="14">G88-G89</f>
@@ -7221,23 +7221,23 @@
       </c>
       <c r="F99" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$39,196,0)-OFFSET([1]aggregated_flows_exergy!B$38,196,0)</f>
-        <v>1101723.0782528599</v>
+        <v>1101845.0706053698</v>
       </c>
       <c r="G99" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!C$39,196,0)-OFFSET([1]aggregated_flows_exergy!C$38,196,0)</f>
-        <v>212311.04948227806</v>
+        <v>212394.10434858804</v>
       </c>
       <c r="H99" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!D$39,196,0)-OFFSET([1]aggregated_flows_exergy!D$38,196,0)</f>
-        <v>747219.06833164021</v>
+        <v>747240.89671444008</v>
       </c>
       <c r="I99" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!E$39,196,0)-OFFSET([1]aggregated_flows_exergy!E$38,196,0)</f>
-        <v>110370.75861095299</v>
+        <v>110385.07241441903</v>
       </c>
       <c r="J99" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!F$39,196,0)-OFFSET([1]aggregated_flows_exergy!F$38,196,0)</f>
-        <v>31822.201827983503</v>
+        <v>31824.997127923503</v>
       </c>
       <c r="K99" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$39,196,0)-OFFSET([1]aggregated_flows_exergy!G$38,196,0)</f>
@@ -7245,11 +7245,11 @@
       </c>
       <c r="L99" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!H$39,196,0)-OFFSET([1]aggregated_flows_exergy!H$38,196,0)</f>
-        <v>393518.55580547987</v>
+        <v>393635.53858103999</v>
       </c>
       <c r="M99" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!I$39,196,0)-OFFSET([1]aggregated_flows_exergy!I$38,196,0)</f>
-        <v>138095.50479504</v>
+        <v>138100.51437199197</v>
       </c>
     </row>
     <row r="100" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7270,23 +7270,23 @@
       </c>
       <c r="F100" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$36,196,0)</f>
-        <v>2054771.63374259</v>
+        <v>2054995.2894164801</v>
       </c>
       <c r="G100" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!C$36,196,0)</f>
-        <v>387898.09373049001</v>
+        <v>388048.11581345502</v>
       </c>
       <c r="H100" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!D$36,196,0)</f>
-        <v>1394718.2038554901</v>
+        <v>1394759.46289665</v>
       </c>
       <c r="I100" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!E$36,196,0)</f>
-        <v>211150.06501319801</v>
+        <v>211177.18101279199</v>
       </c>
       <c r="J100" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!F$36,196,0)</f>
-        <v>61005.271143411403</v>
+        <v>61010.529693578901</v>
       </c>
       <c r="K100" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$36,196,0)</f>
@@ -7294,11 +7294,11 @@
       </c>
       <c r="L100" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!H$36,196,0)</f>
-        <v>760248.48942852695</v>
+        <v>760462.75707879802</v>
       </c>
       <c r="M100" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!I$36,196,0)</f>
-        <v>281530.65534055</v>
+        <v>281540.04336416599</v>
       </c>
     </row>
     <row r="101" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7319,23 +7319,23 @@
       </c>
       <c r="F101" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$30,196,0)-OFFSET([1]aggregated_flows_exergy!B$29,196,0)</f>
-        <v>1387044.9235483985</v>
+        <v>1387194.7406708002</v>
       </c>
       <c r="G101" s="1">
         <f t="shared" ref="G101:M101" ca="1" si="15">G100</f>
-        <v>387898.09373049001</v>
+        <v>388048.11581345502</v>
       </c>
       <c r="H101" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>1394718.2038554901</v>
+        <v>1394759.46289665</v>
       </c>
       <c r="I101" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>211150.06501319801</v>
+        <v>211177.18101279199</v>
       </c>
       <c r="J101" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>61005.271143411403</v>
+        <v>61010.529693578901</v>
       </c>
       <c r="K101" s="1">
         <f t="shared" ca="1" si="15"/>
@@ -7343,11 +7343,11 @@
       </c>
       <c r="L101" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>760248.48942852695</v>
+        <v>760462.75707879802</v>
       </c>
       <c r="M101" s="1">
         <f t="shared" ca="1" si="15"/>
-        <v>281530.65534055</v>
+        <v>281540.04336416599</v>
       </c>
     </row>
     <row r="102" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7368,23 +7368,23 @@
       </c>
       <c r="F102" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$27,196,0)-OFFSET([1]aggregated_flows_exergy!B$25,196,0)</f>
-        <v>783506.16754168016</v>
+        <v>783591.82487909985</v>
       </c>
       <c r="G102" s="1">
         <f t="shared" ref="G102:M102" ca="1" si="16">G99</f>
-        <v>212311.04948227806</v>
+        <v>212394.10434858804</v>
       </c>
       <c r="H102" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>747219.06833164021</v>
+        <v>747240.89671444008</v>
       </c>
       <c r="I102" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>110370.75861095299</v>
+        <v>110385.07241441903</v>
       </c>
       <c r="J102" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>31822.201827983503</v>
+        <v>31824.997127923503</v>
       </c>
       <c r="K102" s="1">
         <f t="shared" ca="1" si="16"/>
@@ -7392,11 +7392,11 @@
       </c>
       <c r="L102" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>393518.55580547987</v>
+        <v>393635.53858103999</v>
       </c>
       <c r="M102" s="1">
         <f t="shared" ca="1" si="16"/>
-        <v>138095.50479504</v>
+        <v>138100.51437199197</v>
       </c>
     </row>
     <row r="103" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7469,7 +7469,7 @@
         <v>2197045.0202281391</v>
       </c>
       <c r="G104" s="1">
-        <f t="shared" ref="F104:M104" ca="1" si="17">G93-G105</f>
+        <f t="shared" ref="G104:M104" ca="1" si="17">G93-G105</f>
         <v>569528.78465562104</v>
       </c>
       <c r="H104" s="1">
@@ -7715,23 +7715,23 @@
       </c>
       <c r="F109" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$32,196,0)</f>
-        <v>34031.803294918704</v>
+        <v>34210.670407571903</v>
       </c>
       <c r="G109" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!C$32,196,0)</f>
-        <v>6615.4289487986298</v>
+        <v>6735.5789636586796</v>
       </c>
       <c r="H109" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!D$32,196,0)</f>
-        <v>23051.609677726399</v>
+        <v>23084.3505233205</v>
       </c>
       <c r="I109" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!E$32,196,0)</f>
-        <v>3302.1708450951501</v>
+        <v>3323.9177554246498</v>
       </c>
       <c r="J109" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!F$32,196,0)</f>
-        <v>1062.5938232984799</v>
+        <v>1066.8231651680101</v>
       </c>
       <c r="K109" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$32,196,0)</f>
@@ -7739,11 +7739,11 @@
       </c>
       <c r="L109" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!H$32,196,0)</f>
-        <v>11647.5355245467</v>
+        <v>11819.378366966401</v>
       </c>
       <c r="M109" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!I$32,196,0)</f>
-        <v>4383.6284375721998</v>
+        <v>4390.6527078057698</v>
       </c>
     </row>
     <row r="110" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -8009,7 +8009,7 @@
       </c>
       <c r="F115" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$11,250,0)</f>
-        <v>10661018.799557099</v>
+        <v>10661018.801758699</v>
       </c>
       <c r="G115" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!C$11,250,0)</f>
@@ -8017,7 +8017,7 @@
       </c>
       <c r="H115" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!D$11,250,0)</f>
-        <v>6614575.6473976905</v>
+        <v>6614575.6495993501</v>
       </c>
       <c r="I115" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!E$11,250,0)</f>
@@ -8029,7 +8029,7 @@
       </c>
       <c r="K115" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$11,250,0)</f>
-        <v>4216866.5961706201</v>
+        <v>4216866.5983722899</v>
       </c>
       <c r="L115" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!H$11,250,0)</f>
@@ -8058,7 +8058,7 @@
       </c>
       <c r="F116" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$6,250,0)</f>
-        <v>6300100.07001842</v>
+        <v>6300100.0715899002</v>
       </c>
       <c r="G116" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!C$6,250,0)</f>
@@ -8066,7 +8066,7 @@
       </c>
       <c r="H116" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!D$6,250,0)</f>
-        <v>3991341.6959548299</v>
+        <v>3991341.6975263101</v>
       </c>
       <c r="I116" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!E$6,250,0)</f>
@@ -8078,7 +8078,7 @@
       </c>
       <c r="K116" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$6,250,0)</f>
-        <v>2523517.9589656801</v>
+        <v>2523517.96053715</v>
       </c>
       <c r="L116" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!H$6,250,0)</f>
@@ -8107,7 +8107,7 @@
       </c>
       <c r="F117" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$48,250,0)</f>
-        <v>124645.87588512601</v>
+        <v>124645.875957368</v>
       </c>
       <c r="G117" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!C$48,250,0)</f>
@@ -8115,7 +8115,7 @@
       </c>
       <c r="H117" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!D$48,250,0)</f>
-        <v>77892.227512252895</v>
+        <v>77892.227584494205</v>
       </c>
       <c r="I117" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!E$48,250,0)</f>
@@ -8127,7 +8127,7 @@
       </c>
       <c r="K117" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$48,250,0)</f>
-        <v>52343.341004908798</v>
+        <v>52343.3410771501</v>
       </c>
       <c r="L117" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!H$48,250,0)</f>
@@ -8254,7 +8254,7 @@
       </c>
       <c r="F120" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$19,250,0)-OFFSET([1]aggregated_flows_exergy!B$17,250,0)</f>
-        <v>77448.958696259186</v>
+        <v>77449.447014350444</v>
       </c>
       <c r="G120" s="1">
         <f t="shared" ref="G120:M121" ca="1" si="18">G111-G112</f>
@@ -8352,27 +8352,27 @@
       </c>
       <c r="F122" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$39,250,0)-OFFSET([1]aggregated_flows_exergy!B$38,250,0)</f>
-        <v>669692.85056812037</v>
+        <v>669725.96186701022</v>
       </c>
       <c r="G122" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!C$39,250,0)-OFFSET([1]aggregated_flows_exergy!C$38,250,0)</f>
-        <v>155664.02301188902</v>
+        <v>155694.57242605399</v>
       </c>
       <c r="H122" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!D$39,250,0)-OFFSET([1]aggregated_flows_exergy!D$38,250,0)</f>
-        <v>419870.86432055011</v>
+        <v>419871.02060012007</v>
       </c>
       <c r="I122" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!E$39,250,0)-OFFSET([1]aggregated_flows_exergy!E$38,250,0)</f>
-        <v>69528.070773151994</v>
+        <v>69530.130293231981</v>
       </c>
       <c r="J122" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!F$39,250,0)-OFFSET([1]aggregated_flows_exergy!F$38,250,0)</f>
-        <v>24629.892462532502</v>
+        <v>24630.238547595902</v>
       </c>
       <c r="K122" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$39,250,0)-OFFSET([1]aggregated_flows_exergy!G$38,250,0)</f>
-        <v>291682.74740769994</v>
+        <v>291682.72155058989</v>
       </c>
       <c r="L122" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!H$39,250,0)-OFFSET([1]aggregated_flows_exergy!H$38,250,0)</f>
@@ -8380,7 +8380,7 @@
       </c>
       <c r="M122" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!I$39,250,0)-OFFSET([1]aggregated_flows_exergy!I$38,250,0)</f>
-        <v>80250.681584269012</v>
+        <v>80283.818740269024</v>
       </c>
     </row>
     <row r="123" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -8401,27 +8401,27 @@
       </c>
       <c r="F123" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$36,250,0)</f>
-        <v>1293127.3205410701</v>
+        <v>1293193.6040334001</v>
       </c>
       <c r="G123" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!C$36,250,0)</f>
-        <v>295470.14728823601</v>
+        <v>295531.33556773397</v>
       </c>
       <c r="H123" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!D$36,250,0)</f>
-        <v>811474.91659138398</v>
+        <v>811475.26492723904</v>
       </c>
       <c r="I123" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!E$36,250,0)</f>
-        <v>137171.20693591301</v>
+        <v>137175.242228446</v>
       </c>
       <c r="J123" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!F$36,250,0)</f>
-        <v>49011.049725535398</v>
+        <v>49011.761309984402</v>
       </c>
       <c r="K123" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$36,250,0)</f>
-        <v>533099.73253091495</v>
+        <v>533099.67352231301</v>
       </c>
       <c r="L123" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!H$36,250,0)</f>
@@ -8429,7 +8429,7 @@
       </c>
       <c r="M123" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!I$36,250,0)</f>
-        <v>166716.027949168</v>
+        <v>166782.37045010601</v>
       </c>
     </row>
     <row r="124" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -8450,27 +8450,27 @@
       </c>
       <c r="F124" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$30,250,0)-OFFSET([1]aggregated_flows_exergy!B$29,250,0)</f>
-        <v>840271.95979640074</v>
+        <v>840314.5594927799</v>
       </c>
       <c r="G124" s="1">
         <f t="shared" ref="G124:M124" ca="1" si="19">G123</f>
-        <v>295470.14728823601</v>
+        <v>295531.33556773397</v>
       </c>
       <c r="H124" s="1">
         <f t="shared" ca="1" si="19"/>
-        <v>811474.91659138398</v>
+        <v>811475.26492723904</v>
       </c>
       <c r="I124" s="1">
         <f t="shared" ca="1" si="19"/>
-        <v>137171.20693591301</v>
+        <v>137175.242228446</v>
       </c>
       <c r="J124" s="1">
         <f t="shared" ca="1" si="19"/>
-        <v>49011.049725535398</v>
+        <v>49011.761309984402</v>
       </c>
       <c r="K124" s="1">
         <f t="shared" ca="1" si="19"/>
-        <v>533099.73253091495</v>
+        <v>533099.67352231301</v>
       </c>
       <c r="L124" s="1">
         <f t="shared" ca="1" si="19"/>
@@ -8478,7 +8478,7 @@
       </c>
       <c r="M124" s="1">
         <f t="shared" ca="1" si="19"/>
-        <v>166716.027949168</v>
+        <v>166782.37045010601</v>
       </c>
     </row>
     <row r="125" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -8499,27 +8499,27 @@
       </c>
       <c r="F125" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$27,250,0)-OFFSET([1]aggregated_flows_exergy!B$25,250,0)</f>
-        <v>473490.50599977002</v>
+        <v>473512.47267782991</v>
       </c>
       <c r="G125" s="1">
         <f t="shared" ref="G125:M125" ca="1" si="20">G122</f>
-        <v>155664.02301188902</v>
+        <v>155694.57242605399</v>
       </c>
       <c r="H125" s="1">
         <f t="shared" ca="1" si="20"/>
-        <v>419870.86432055011</v>
+        <v>419871.02060012007</v>
       </c>
       <c r="I125" s="1">
         <f t="shared" ca="1" si="20"/>
-        <v>69528.070773151994</v>
+        <v>69530.130293231981</v>
       </c>
       <c r="J125" s="1">
         <f t="shared" ca="1" si="20"/>
-        <v>24629.892462532502</v>
+        <v>24630.238547595902</v>
       </c>
       <c r="K125" s="1">
         <f t="shared" ca="1" si="20"/>
-        <v>291682.74740769994</v>
+        <v>291682.72155058989</v>
       </c>
       <c r="L125" s="1">
         <f t="shared" ca="1" si="20"/>
@@ -8527,7 +8527,7 @@
       </c>
       <c r="M125" s="1">
         <f t="shared" ca="1" si="20"/>
-        <v>80250.681584269012</v>
+        <v>80283.818740269024</v>
       </c>
     </row>
     <row r="126" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -8597,15 +8597,15 @@
       </c>
       <c r="F127" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$52,250,0)-OFFSET([1]aggregated_flows_exergy!B$51,250,0)</f>
-        <v>1652882.0005122221</v>
+        <v>1652882.0007841219</v>
       </c>
       <c r="G127" s="1">
-        <f t="shared" ref="F127:M127" ca="1" si="21">G116-G128</f>
+        <f t="shared" ref="G127:M127" ca="1" si="21">G116-G128</f>
         <v>538607.76415555016</v>
       </c>
       <c r="H127" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>1649750.4187997901</v>
+        <v>1649750.4191241199</v>
       </c>
       <c r="I127" s="1">
         <f t="shared" ca="1" si="21"/>
@@ -8617,7 +8617,7 @@
       </c>
       <c r="K127" s="1">
         <f t="shared" ca="1" si="21"/>
-        <v>1038439.6327808101</v>
+        <v>1038439.6331051199</v>
       </c>
       <c r="L127" s="1">
         <f t="shared" ca="1" si="21"/>
@@ -8646,7 +8646,7 @@
       </c>
       <c r="F128" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$97,203,0)</f>
-        <v>3720160.3483597599</v>
+        <v>3720160.34960692</v>
       </c>
       <c r="G128" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!C$97,203,0)</f>
@@ -8654,7 +8654,7 @@
       </c>
       <c r="H128" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!D$97,203,0)</f>
-        <v>2341591.2771550398</v>
+        <v>2341591.2784021902</v>
       </c>
       <c r="I128" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!E$97,203,0)</f>
@@ -8666,7 +8666,7 @@
       </c>
       <c r="K128" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$97,203,0)</f>
-        <v>1485078.32618487</v>
+        <v>1485078.3274320301</v>
       </c>
       <c r="L128" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!H$97,203,0)</f>
@@ -8795,7 +8795,7 @@
       </c>
       <c r="F131" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$33,250,0)</f>
-        <v>46437886.785772704</v>
+        <v>46437886.819303699</v>
       </c>
       <c r="G131" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!C$33,250,0)</f>
@@ -8803,7 +8803,7 @@
       </c>
       <c r="H131" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!D$33,250,0)</f>
-        <v>28906374.344339099</v>
+        <v>28906374.377870101</v>
       </c>
       <c r="I131" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!E$33,250,0)</f>
@@ -8815,7 +8815,7 @@
       </c>
       <c r="K131" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$33,250,0)</f>
-        <v>18075968.491302099</v>
+        <v>18075968.524833102</v>
       </c>
       <c r="L131" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!H$33,250,0)</f>
@@ -8846,27 +8846,27 @@
       </c>
       <c r="F132" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$32,250,0)</f>
-        <v>25272.620960436001</v>
+        <v>25322.247177941099</v>
       </c>
       <c r="G132" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!C$32,250,0)</f>
-        <v>5800.8246294685896</v>
+        <v>5846.58388386147</v>
       </c>
       <c r="H132" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!D$32,250,0)</f>
-        <v>15914.156870950699</v>
+        <v>15914.450295446601</v>
       </c>
       <c r="I132" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!E$32,250,0)</f>
-        <v>2612.1019046177498</v>
+        <v>2615.1220186515602</v>
       </c>
       <c r="J132" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!F$32,250,0)</f>
-        <v>945.53755539920996</v>
+        <v>946.09097998166703</v>
       </c>
       <c r="K132" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$32,250,0)</f>
-        <v>11149.225374761199</v>
+        <v>11149.221413473701</v>
       </c>
       <c r="L132" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!H$32,250,0)</f>
@@ -8874,7 +8874,7 @@
       </c>
       <c r="M132" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!I$32,250,0)</f>
-        <v>2868.22565196914</v>
+        <v>2917.85583076174</v>
       </c>
     </row>
     <row r="133" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -9385,7 +9385,7 @@
       </c>
       <c r="F143" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$19,304,0)-OFFSET([1]aggregated_flows_exergy!B$17,304,0)</f>
-        <v>62346.42901254911</v>
+        <v>62346.436756860465</v>
       </c>
       <c r="G143" s="1">
         <f t="shared" ref="G143:M144" ca="1" si="22">G134-G135</f>
@@ -9483,19 +9483,19 @@
       </c>
       <c r="F145" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$39,304,0)-OFFSET([1]aggregated_flows_exergy!B$38,304,0)</f>
-        <v>526204.76527693984</v>
+        <v>526206.46888146992</v>
       </c>
       <c r="G145" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!C$39,304,0)-OFFSET([1]aggregated_flows_exergy!C$38,304,0)</f>
-        <v>418394.97272141592</v>
+        <v>418396.50951915595</v>
       </c>
       <c r="H145" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!D$39,304,0)-OFFSET([1]aggregated_flows_exergy!D$38,304,0)</f>
-        <v>43412.694124975009</v>
+        <v>43412.75931341399</v>
       </c>
       <c r="I145" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!E$39,304,0)-OFFSET([1]aggregated_flows_exergy!E$38,304,0)</f>
-        <v>64067.826565525</v>
+        <v>64067.928183868993</v>
       </c>
       <c r="J145" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!F$39,304,0)-OFFSET([1]aggregated_flows_exergy!F$38,304,0)</f>
@@ -9503,11 +9503,11 @@
       </c>
       <c r="K145" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$39,304,0)-OFFSET([1]aggregated_flows_exergy!G$38,304,0)</f>
-        <v>198564.50093476602</v>
+        <v>198565.96273602999</v>
       </c>
       <c r="L145" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!H$39,304,0)-OFFSET([1]aggregated_flows_exergy!H$38,304,0)</f>
-        <v>250051.78783883899</v>
+        <v>250052.02964210301</v>
       </c>
       <c r="M145" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!I$39,304,0)-OFFSET([1]aggregated_flows_exergy!I$38,304,0)</f>
@@ -9532,19 +9532,19 @@
       </c>
       <c r="F146" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$36,304,0)</f>
-        <v>990351.90530164097</v>
+        <v>990354.74446897605</v>
       </c>
       <c r="G146" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!C$36,304,0)</f>
-        <v>781080.17116329796</v>
+        <v>781082.71976682101</v>
       </c>
       <c r="H146" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!D$36,304,0)</f>
-        <v>84884.875264931703</v>
+        <v>84884.989919770102</v>
       </c>
       <c r="I146" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!E$36,304,0)</f>
-        <v>123727.99393161001</v>
+        <v>123728.169840584</v>
       </c>
       <c r="J146" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!F$36,304,0)</f>
@@ -9552,11 +9552,11 @@
       </c>
       <c r="K146" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$36,304,0)</f>
-        <v>350636.97542100499</v>
+        <v>350639.39890294801</v>
       </c>
       <c r="L146" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!H$36,304,0)</f>
-        <v>483049.05584452499</v>
+        <v>483049.47152991802</v>
       </c>
       <c r="M146" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!I$36,304,0)</f>
@@ -9581,19 +9581,19 @@
       </c>
       <c r="F147" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$30,304,0)-OFFSET([1]aggregated_flows_exergy!B$29,304,0)</f>
-        <v>661622.60695285071</v>
+        <v>661624.57941978984</v>
       </c>
       <c r="G147" s="1">
         <f t="shared" ref="G147:M147" ca="1" si="23">G146</f>
-        <v>781080.17116329796</v>
+        <v>781082.71976682101</v>
       </c>
       <c r="H147" s="1">
         <f t="shared" ca="1" si="23"/>
-        <v>84884.875264931703</v>
+        <v>84884.989919770102</v>
       </c>
       <c r="I147" s="1">
         <f t="shared" ca="1" si="23"/>
-        <v>123727.99393161001</v>
+        <v>123728.169840584</v>
       </c>
       <c r="J147" s="1">
         <f t="shared" ca="1" si="23"/>
@@ -9601,11 +9601,11 @@
       </c>
       <c r="K147" s="1">
         <f t="shared" ca="1" si="23"/>
-        <v>350636.97542100499</v>
+        <v>350639.39890294801</v>
       </c>
       <c r="L147" s="1">
         <f t="shared" ca="1" si="23"/>
-        <v>483049.05584452499</v>
+        <v>483049.47152991802</v>
       </c>
       <c r="M147" s="1">
         <f t="shared" ca="1" si="23"/>
@@ -9630,19 +9630,19 @@
       </c>
       <c r="F148" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$27,304,0)-OFFSET([1]aggregated_flows_exergy!B$25,304,0)</f>
-        <v>374683.94077510608</v>
+        <v>374685.20692756597</v>
       </c>
       <c r="G148" s="1">
         <f t="shared" ref="G148:M148" ca="1" si="24">G145</f>
-        <v>418394.97272141592</v>
+        <v>418396.50951915595</v>
       </c>
       <c r="H148" s="1">
         <f t="shared" ca="1" si="24"/>
-        <v>43412.694124975009</v>
+        <v>43412.75931341399</v>
       </c>
       <c r="I148" s="1">
         <f t="shared" ca="1" si="24"/>
-        <v>64067.826565525</v>
+        <v>64067.928183868993</v>
       </c>
       <c r="J148" s="1">
         <f t="shared" ca="1" si="24"/>
@@ -9650,11 +9650,11 @@
       </c>
       <c r="K148" s="1">
         <f t="shared" ca="1" si="24"/>
-        <v>198564.50093476602</v>
+        <v>198565.96273602999</v>
       </c>
       <c r="L148" s="1">
         <f t="shared" ca="1" si="24"/>
-        <v>250051.78783883899</v>
+        <v>250052.02964210301</v>
       </c>
       <c r="M148" s="1">
         <f t="shared" ca="1" si="24"/>
@@ -9731,7 +9731,7 @@
         <v>1050266.4795077292</v>
       </c>
       <c r="G150" s="1">
-        <f t="shared" ref="F150:M150" ca="1" si="25">G139-G151</f>
+        <f t="shared" ref="G150:M150" ca="1" si="25">G139-G151</f>
         <v>1343257.9746493902</v>
       </c>
       <c r="H150" s="1">
@@ -9977,19 +9977,19 @@
       </c>
       <c r="F155" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$32,304,0)</f>
-        <v>2251.4518449797101</v>
+        <v>2252.6424958021098</v>
       </c>
       <c r="G155" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!C$32,304,0)</f>
-        <v>1313.95161636226</v>
+        <v>1315.0170844702</v>
       </c>
       <c r="H155" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!D$32,304,0)</f>
-        <v>708.989482691435</v>
+        <v>709.03746278363303</v>
       </c>
       <c r="I155" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!E$32,304,0)</f>
-        <v>224.018132301527</v>
+        <v>224.09533492378</v>
       </c>
       <c r="J155" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!F$32,304,0)</f>
@@ -9997,11 +9997,11 @@
       </c>
       <c r="K155" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$32,304,0)</f>
-        <v>566.48143924465205</v>
+        <v>567.52606750606401</v>
       </c>
       <c r="L155" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!H$32,304,0)</f>
-        <v>1578.56615345454</v>
+        <v>1578.7121760155301</v>
       </c>
       <c r="M155" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!I$32,304,0)</f>
@@ -10271,23 +10271,23 @@
       </c>
       <c r="F161" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$11,358,0)</f>
-        <v>7564422.3322999403</v>
+        <v>7564208.3778254101</v>
       </c>
       <c r="G161" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!C$11,358,0)</f>
-        <v>1712230.6672650201</v>
+        <v>1712170.09403572</v>
       </c>
       <c r="H161" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!D$11,358,0)</f>
-        <v>4818325.6093286304</v>
+        <v>4818184.4148128796</v>
       </c>
       <c r="I161" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!E$11,358,0)</f>
-        <v>852827.37431075203</v>
+        <v>852815.74152794597</v>
       </c>
       <c r="J161" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!F$11,358,0)</f>
-        <v>181038.681395566</v>
+        <v>181038.12744887199</v>
       </c>
       <c r="K161" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$11,358,0)</f>
@@ -10299,7 +10299,7 @@
       </c>
       <c r="M161" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!I$11,358,0)</f>
-        <v>1003814.07091647</v>
+        <v>1003600.1164419299</v>
       </c>
     </row>
     <row r="162" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -10320,23 +10320,23 @@
       </c>
       <c r="F162" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$6,358,0)</f>
-        <v>4507132.9475496802</v>
+        <v>4507020.7679879405</v>
       </c>
       <c r="G162" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!C$6,358,0)</f>
-        <v>935949.33179852297</v>
+        <v>935918.01815133495</v>
       </c>
       <c r="H162" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!D$6,358,0)</f>
-        <v>2949038.3968099798</v>
+        <v>2948965.0713365199</v>
       </c>
       <c r="I162" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!E$6,358,0)</f>
-        <v>521541.49517139897</v>
+        <v>521534.17648099398</v>
       </c>
       <c r="J162" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!F$6,358,0)</f>
-        <v>100603.72376979599</v>
+        <v>100603.50201911799</v>
       </c>
       <c r="K162" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$6,358,0)</f>
@@ -10348,7 +10348,7 @@
       </c>
       <c r="M162" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!I$6,358,0)</f>
-        <v>556927.30678354204</v>
+        <v>556815.12722180504</v>
       </c>
     </row>
     <row r="163" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -10369,23 +10369,23 @@
       </c>
       <c r="F163" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$48,358,0)</f>
-        <v>101056.329907345</v>
+        <v>101054.222518782</v>
       </c>
       <c r="G163" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!C$48,358,0)</f>
-        <v>20986.629572596201</v>
+        <v>20986.051189273399</v>
       </c>
       <c r="H163" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!D$48,358,0)</f>
-        <v>63968.509609004002</v>
+        <v>63967.193697837502</v>
       </c>
       <c r="I163" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!E$48,358,0)</f>
-        <v>13968.5751451206</v>
+        <v>13968.399335829499</v>
       </c>
       <c r="J163" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!F$48,358,0)</f>
-        <v>2132.6155806236102</v>
+        <v>2132.5782958417599</v>
       </c>
       <c r="K163" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$48,358,0)</f>
@@ -10397,7 +10397,7 @@
       </c>
       <c r="M163" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!I$48,358,0)</f>
-        <v>11350.0783143031</v>
+        <v>11347.970925740899</v>
       </c>
     </row>
     <row r="164" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -10516,7 +10516,7 @@
       </c>
       <c r="F166" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$19,358,0)-OFFSET([1]aggregated_flows_exergy!B$17,358,0)</f>
-        <v>30631.377113630995</v>
+        <v>30644.227503340691</v>
       </c>
       <c r="G166" s="1">
         <f t="shared" ref="G166:M167" ca="1" si="26">G157-G158</f>
@@ -10614,23 +10614,23 @@
       </c>
       <c r="F168" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$39,358,0)-OFFSET([1]aggregated_flows_exergy!B$38,358,0)</f>
-        <v>839717.71142380964</v>
+        <v>840813.81527059991</v>
       </c>
       <c r="G168" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!C$39,358,0)-OFFSET([1]aggregated_flows_exergy!C$38,358,0)</f>
-        <v>175104.15710064</v>
+        <v>175406.96834320598</v>
       </c>
       <c r="H168" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!D$39,358,0)-OFFSET([1]aggregated_flows_exergy!D$38,358,0)</f>
-        <v>546242.12892598985</v>
+        <v>546963.54275872977</v>
       </c>
       <c r="I168" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!E$39,358,0)-OFFSET([1]aggregated_flows_exergy!E$38,358,0)</f>
-        <v>100247.18168384198</v>
+        <v>100317.17710215598</v>
       </c>
       <c r="J168" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!F$39,358,0)-OFFSET([1]aggregated_flows_exergy!F$38,358,0)</f>
-        <v>18124.243713322809</v>
+        <v>18126.127066490109</v>
       </c>
       <c r="K168" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$39,358,0)-OFFSET([1]aggregated_flows_exergy!G$38,358,0)</f>
@@ -10642,7 +10642,7 @@
       </c>
       <c r="M168" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!I$39,358,0)-OFFSET([1]aggregated_flows_exergy!I$38,358,0)</f>
-        <v>90980.722164362989</v>
+        <v>92076.826011151978</v>
       </c>
     </row>
     <row r="169" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -10663,23 +10663,23 @@
       </c>
       <c r="F169" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$36,358,0)</f>
-        <v>1501740.0512274101</v>
+        <v>1503630.81370769</v>
       </c>
       <c r="G169" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!C$36,358,0)</f>
-        <v>306853.11262497201</v>
+        <v>307376.744754138</v>
       </c>
       <c r="H169" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!D$36,358,0)</f>
-        <v>977601.92454036104</v>
+        <v>978837.355683767</v>
       </c>
       <c r="I169" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!E$36,358,0)</f>
-        <v>184266.683959163</v>
+        <v>184394.720265852</v>
       </c>
       <c r="J169" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!F$36,358,0)</f>
-        <v>33018.330102906701</v>
+        <v>33021.993003928903</v>
       </c>
       <c r="K169" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$36,358,0)</f>
@@ -10691,7 +10691,7 @@
       </c>
       <c r="M169" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!I$36,358,0)</f>
-        <v>175852.612991876</v>
+        <v>177743.37547215799</v>
       </c>
     </row>
     <row r="170" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -10712,23 +10712,23 @@
       </c>
       <c r="F170" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$30,358,0)-OFFSET([1]aggregated_flows_exergy!B$29,358,0)</f>
-        <v>1013775.4450661298</v>
+        <v>1015037.6974259503</v>
       </c>
       <c r="G170" s="1">
         <f t="shared" ref="G170:M170" ca="1" si="27">G169</f>
-        <v>306853.11262497201</v>
+        <v>307376.744754138</v>
       </c>
       <c r="H170" s="1">
         <f t="shared" ca="1" si="27"/>
-        <v>977601.92454036104</v>
+        <v>978837.355683767</v>
       </c>
       <c r="I170" s="1">
         <f t="shared" ca="1" si="27"/>
-        <v>184266.683959163</v>
+        <v>184394.720265852</v>
       </c>
       <c r="J170" s="1">
         <f t="shared" ca="1" si="27"/>
-        <v>33018.330102906701</v>
+        <v>33021.993003928903</v>
       </c>
       <c r="K170" s="1">
         <f t="shared" ca="1" si="27"/>
@@ -10740,7 +10740,7 @@
       </c>
       <c r="M170" s="1">
         <f t="shared" ca="1" si="27"/>
-        <v>175852.612991876</v>
+        <v>177743.37547215799</v>
       </c>
     </row>
     <row r="171" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -10761,23 +10761,23 @@
       </c>
       <c r="F171" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$27,358,0)-OFFSET([1]aggregated_flows_exergy!B$25,358,0)</f>
-        <v>552211.33448406984</v>
+        <v>552894.57382022985</v>
       </c>
       <c r="G171" s="1">
         <f t="shared" ref="G171:M171" ca="1" si="28">G168</f>
-        <v>175104.15710064</v>
+        <v>175406.96834320598</v>
       </c>
       <c r="H171" s="1">
         <f t="shared" ca="1" si="28"/>
-        <v>546242.12892598985</v>
+        <v>546963.54275872977</v>
       </c>
       <c r="I171" s="1">
         <f t="shared" ca="1" si="28"/>
-        <v>100247.18168384198</v>
+        <v>100317.17710215598</v>
       </c>
       <c r="J171" s="1">
         <f t="shared" ca="1" si="28"/>
-        <v>18124.243713322809</v>
+        <v>18126.127066490109</v>
       </c>
       <c r="K171" s="1">
         <f t="shared" ca="1" si="28"/>
@@ -10789,7 +10789,7 @@
       </c>
       <c r="M171" s="1">
         <f t="shared" ca="1" si="28"/>
-        <v>90980.722164362989</v>
+        <v>92076.826011151978</v>
       </c>
     </row>
     <row r="172" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -10859,23 +10859,23 @@
       </c>
       <c r="F173" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$52,358,0)-OFFSET([1]aggregated_flows_exergy!B$51,358,0)</f>
-        <v>1423429.3090673441</v>
+        <v>1423395.3524084298</v>
       </c>
       <c r="G173" s="1">
-        <f t="shared" ref="F173:M173" ca="1" si="29">G162-G174</f>
-        <v>417860.39272822195</v>
+        <f t="shared" ref="G173:M173" ca="1" si="29">G162-G174</f>
+        <v>417845.64068413293</v>
       </c>
       <c r="H173" s="1">
         <f t="shared" ca="1" si="29"/>
-        <v>1407700.8442262898</v>
+        <v>1407666.82671201</v>
       </c>
       <c r="I173" s="1">
         <f t="shared" ca="1" si="29"/>
-        <v>244811.86580681696</v>
+        <v>244807.64591156296</v>
       </c>
       <c r="J173" s="1">
         <f t="shared" ca="1" si="29"/>
-        <v>47778.360747856095</v>
+        <v>47778.222104484892</v>
       </c>
       <c r="K173" s="1">
         <f t="shared" ca="1" si="29"/>
@@ -10887,7 +10887,7 @@
       </c>
       <c r="M173" s="1">
         <f t="shared" ca="1" si="29"/>
-        <v>294464.40664212301</v>
+        <v>294411.27854512405</v>
       </c>
     </row>
     <row r="174" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -10908,23 +10908,23 @@
       </c>
       <c r="F174" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$97,311,0)</f>
-        <v>2388981.4840405202</v>
+        <v>2388922.43257578</v>
       </c>
       <c r="G174" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!C$97,311,0)</f>
-        <v>518088.93907030101</v>
+        <v>518072.37746720202</v>
       </c>
       <c r="H174" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!D$97,311,0)</f>
-        <v>1541337.55258369</v>
+        <v>1541298.2446245099</v>
       </c>
       <c r="I174" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!E$97,311,0)</f>
-        <v>276729.62936458201</v>
+        <v>276726.53056943102</v>
       </c>
       <c r="J174" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!F$97,311,0)</f>
-        <v>52825.363021939898</v>
+        <v>52825.279914633102</v>
       </c>
       <c r="K174" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$97,311,0)</f>
@@ -10936,7 +10936,7 @@
       </c>
       <c r="M174" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!I$97,311,0)</f>
-        <v>262462.90014141903</v>
+        <v>262403.84867668099</v>
       </c>
     </row>
     <row r="175" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -11057,23 +11057,23 @@
       </c>
       <c r="F177" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$33,358,0)</f>
-        <v>39368160.996755503</v>
+        <v>39367037.916057102</v>
       </c>
       <c r="G177" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!C$33,358,0)</f>
-        <v>8516498.2028112002</v>
+        <v>8516187.6653823592</v>
       </c>
       <c r="H177" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!D$33,358,0)</f>
-        <v>25306490.8437468</v>
+        <v>25305761.044893399</v>
       </c>
       <c r="I177" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!E$33,358,0)</f>
-        <v>4621740.8767542196</v>
+        <v>4621664.9650956597</v>
       </c>
       <c r="J177" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!F$33,358,0)</f>
-        <v>923431.07344337797</v>
+        <v>923424.24068572104</v>
       </c>
       <c r="K177" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$33,358,0)</f>
@@ -11085,7 +11085,7 @@
       </c>
       <c r="M177" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!I$33,358,0)</f>
-        <v>5195280.4802629203</v>
+        <v>5194157.3995644897</v>
       </c>
     </row>
     <row r="178" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -11108,23 +11108,23 @@
       </c>
       <c r="F178" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!B$32,358,0)</f>
-        <v>22736.154863363201</v>
+        <v>22765.360934730201</v>
       </c>
       <c r="G178" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!C$32,358,0)</f>
-        <v>4934.8574148915804</v>
+        <v>4952.5037810834901</v>
       </c>
       <c r="H178" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!D$32,358,0)</f>
-        <v>14677.1621649999</v>
+        <v>14718.890776705901</v>
       </c>
       <c r="I178" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!E$32,358,0)</f>
-        <v>2592.6795734237799</v>
+        <v>2597.0336874781401</v>
       </c>
       <c r="J178" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!F$32,358,0)</f>
-        <v>531.45571004789599</v>
+        <v>496.932689462653</v>
       </c>
       <c r="K178" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!G$32,358,0)</f>
@@ -11136,7 +11136,7 @@
       </c>
       <c r="M178" s="1">
         <f ca="1">OFFSET([1]aggregated_flows_exergy!I$32,358,0)</f>
-        <v>2287.4876331321302</v>
+        <v>2316.69370449915</v>
       </c>
     </row>
   </sheetData>
@@ -11153,8 +11153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="Q68" sqref="Q68"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="O41" sqref="O41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -11489,11 +11489,11 @@
       </c>
       <c r="J7" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$1:J$85,'Engines indvidual'!$B$1:$B$85,'Full system - simplified'!$B7,'Engines indvidual'!$D$1:$D$85,'Full system - simplified'!$D7,'Engines indvidual'!$E$1:$E$85,'Full system - simplified'!$E7)*0.000001</f>
-        <v>7.0845154212318002</v>
+        <v>7.0845154212317896</v>
       </c>
       <c r="K7" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$1:K$85,'Engines indvidual'!$B$1:$B$85,'Full system - simplified'!$B7,'Engines indvidual'!$D$1:$D$85,'Full system - simplified'!$D7,'Engines indvidual'!$E$1:$E$85,'Full system - simplified'!$E7)*0.000001</f>
-        <v>22.176646742267582</v>
+        <v>22.176646742267572</v>
       </c>
       <c r="L7" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$1:L$85,'Engines indvidual'!$B$1:$B$85,'Full system - simplified'!$B7,'Engines indvidual'!$D$1:$D$85,'Full system - simplified'!$D7,'Engines indvidual'!$E$1:$E$85,'Full system - simplified'!$E7)*0.000001</f>
@@ -12358,7 +12358,7 @@
         <v>7</v>
       </c>
       <c r="F26" s="2">
-        <f ca="1">SUMIFS('Engines indvidual'!F$87:F$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B26,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D26,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E26)*0.000001</f>
+        <f ca="1">SUMIFS('Engines indvidual'!F$87:F$178,'Engines indvidual'!$B$87:$B$178,'Full system - simplified'!$B26,'Engines indvidual'!$D$87:$D$178,'Full system - simplified'!$D26,'Engines indvidual'!$E$87:$E$178,'Full system - simplified'!$E26)*0.000001</f>
         <v>5.3390023466401496E-3</v>
       </c>
       <c r="G26" s="3">
@@ -12407,7 +12407,7 @@
         <v>7</v>
       </c>
       <c r="F27" s="2">
-        <f ca="1">SUMIFS('Engines indvidual'!F$87:F$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B27,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D27,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E27)*0.000001</f>
+        <f ca="1">SUMIFS('Engines indvidual'!F$87:F$178,'Engines indvidual'!$B$87:$B$178,'Full system - simplified'!$B27,'Engines indvidual'!$D$87:$D$178,'Full system - simplified'!$D27,'Engines indvidual'!$E$87:$E$178,'Full system - simplified'!$E27)*0.000001</f>
         <v>7.9139880154120394</v>
       </c>
       <c r="G27" s="3">
@@ -12456,7 +12456,7 @@
         <v>7</v>
       </c>
       <c r="F28" s="2">
-        <f ca="1">SUMIFS('Engines indvidual'!F$87:F$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B28,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D28,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E28)*0.000001</f>
+        <f ca="1">SUMIFS('Engines indvidual'!F$87:F$178,'Engines indvidual'!$B$87:$B$178,'Full system - simplified'!$B28,'Engines indvidual'!$D$87:$D$178,'Full system - simplified'!$D28,'Engines indvidual'!$E$87:$E$178,'Full system - simplified'!$E28)*0.000001</f>
         <v>7.6539575759840881</v>
       </c>
       <c r="G28" s="3">
@@ -12505,7 +12505,7 @@
         <v>7</v>
       </c>
       <c r="F29" s="2">
-        <f ca="1">SUMIFS('Engines indvidual'!F$87:F$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B29,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D29,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E29)*0.000001</f>
+        <f ca="1">SUMIFS('Engines indvidual'!F$87:F$178,'Engines indvidual'!$B$87:$B$178,'Full system - simplified'!$B29,'Engines indvidual'!$D$87:$D$178,'Full system - simplified'!$D29,'Engines indvidual'!$E$87:$E$178,'Full system - simplified'!$E29)*0.000001</f>
         <v>7.0942529442990301</v>
       </c>
       <c r="G29" s="3">
@@ -12554,7 +12554,7 @@
         <v>12</v>
       </c>
       <c r="F30" s="2">
-        <f ca="1">SUMIFS('Engines indvidual'!F$87:F$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B30,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D30,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E30)*0.000001</f>
+        <f ca="1">SUMIFS('Engines indvidual'!F$87:F$178,'Engines indvidual'!$B$87:$B$178,'Full system - simplified'!$B30,'Engines indvidual'!$D$87:$D$178,'Full system - simplified'!$D30,'Engines indvidual'!$E$87:$E$178,'Full system - simplified'!$E30)*0.000001</f>
         <v>9.5364176727926981</v>
       </c>
       <c r="G30" s="3">
@@ -12603,28 +12603,28 @@
         <v>7</v>
       </c>
       <c r="F31" s="2">
-        <f ca="1">SUMIFS('Engines indvidual'!F$87:F$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B31,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D31,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E31)*0.000001</f>
-        <v>36.262821022740511</v>
+        <f ca="1">SUMIFS('Engines indvidual'!F$87:F$178,'Engines indvidual'!$B$87:$B$178,'Full system - simplified'!$B31,'Engines indvidual'!$D$87:$D$178,'Full system - simplified'!$D31,'Engines indvidual'!$E$87:$E$178,'Full system - simplified'!$E31)*0.000001</f>
+        <v>36.262607070467581</v>
       </c>
       <c r="G31" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$87:G$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B31,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D31,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E31)*0.000001</f>
-        <v>11.77607902491666</v>
+        <v>11.77601845168736</v>
       </c>
       <c r="H31" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$87:H$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B31,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D31,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E31)*0.000001</f>
-        <v>19.814986182287427</v>
+        <v>19.814844989973334</v>
       </c>
       <c r="I31" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$87:I$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B31,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D31,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E31)*0.000001</f>
-        <v>3.5923805906475161</v>
+        <v>3.5923689578647098</v>
       </c>
       <c r="J31" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$87:J$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B31,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D31,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E31)*0.000001</f>
-        <v>1.0793752248889839</v>
+        <v>1.07937467094229</v>
       </c>
       <c r="K31" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$87:K$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B31,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D31,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E31)*0.000001</f>
-        <v>15.70523713262302</v>
+        <v>15.705237134824689</v>
       </c>
       <c r="L31" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$87:L$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B31,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D31,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E31)*0.000001</f>
@@ -12632,7 +12632,7 @@
       </c>
       <c r="M31" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$87:M$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B31,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D31,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E31)*0.000001</f>
-        <v>5.5967586600801198</v>
+        <v>5.596544705605579</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -12652,28 +12652,28 @@
         <v>7</v>
       </c>
       <c r="F32" s="2">
-        <f ca="1">SUMIFS('Engines indvidual'!F$87:F$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B32,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D32,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E32)*0.000001</f>
-        <v>21.042478099276252</v>
+        <f ca="1">SUMIFS('Engines indvidual'!F$87:F$178,'Engines indvidual'!$B$87:$B$178,'Full system - simplified'!$B32,'Engines indvidual'!$D$87:$D$178,'Full system - simplified'!$D32,'Engines indvidual'!$E$87:$E$178,'Full system - simplified'!$E32)*0.000001</f>
+        <v>21.042365921285988</v>
       </c>
       <c r="G32" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$87:G$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B32,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D32,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E32)*0.000001</f>
-        <v>6.3783446079999528</v>
+        <v>6.3783132943527656</v>
       </c>
       <c r="H32" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$87:H$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B32,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D32,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E32)*0.000001</f>
-        <v>11.93621371945814</v>
+        <v>11.936140395556158</v>
       </c>
       <c r="I32" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$87:I$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B32,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D32,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E32)*0.000001</f>
-        <v>2.156508836437427</v>
+        <v>2.1565015177470221</v>
       </c>
       <c r="J32" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$87:J$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B32,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D32,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E32)*0.000001</f>
-        <v>0.57141093538073773</v>
+        <v>0.57141071363005969</v>
       </c>
       <c r="K32" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$87:K$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B32,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D32,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E32)*0.000001</f>
-        <v>9.1655041587943096</v>
+        <v>9.1655041603657779</v>
       </c>
       <c r="L32" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$87:L$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B32,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D32,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E32)*0.000001</f>
@@ -12681,7 +12681,7 @@
       </c>
       <c r="M32" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$87:M$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B32,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D32,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E32)*0.000001</f>
-        <v>3.0110521096751639</v>
+        <v>3.0109399301134268</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -12701,28 +12701,28 @@
         <v>14</v>
       </c>
       <c r="F33" s="2">
-        <f ca="1">SUMIFS('Engines indvidual'!F$87:F$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B33,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D33,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E33)*0.000001</f>
-        <v>0.46280325141239226</v>
+        <f ca="1">SUMIFS('Engines indvidual'!F$87:F$178,'Engines indvidual'!$B$87:$B$178,'Full system - simplified'!$B33,'Engines indvidual'!$D$87:$D$178,'Full system - simplified'!$D33,'Engines indvidual'!$E$87:$E$178,'Full system - simplified'!$E33)*0.000001</f>
+        <v>0.46280114409607126</v>
       </c>
       <c r="G33" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$87:G$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B33,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D33,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E33)*0.000001</f>
-        <v>0.13173394659608048</v>
+        <v>0.13173336821275769</v>
       </c>
       <c r="H33" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$87:H$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B33,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D33,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E33)*0.000001</f>
-        <v>0.25937056143788328</v>
+        <v>0.25936924559895808</v>
       </c>
       <c r="I33" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$87:I$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B33,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D33,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E33)*0.000001</f>
-        <v>6.0169376848747298E-2</v>
+        <v>6.0169201039456194E-2</v>
       </c>
       <c r="J33" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$87:J$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B33,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D33,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E33)*0.000001</f>
-        <v>1.1529366529681392E-2</v>
+        <v>1.1529329244899543E-2</v>
       </c>
       <c r="K33" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$87:K$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B33,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D33,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E33)*0.000001</f>
-        <v>0.20909684040336357</v>
+        <v>0.20909684047560489</v>
       </c>
       <c r="L33" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$87:L$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B33,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D33,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E33)*0.000001</f>
@@ -12730,7 +12730,7 @@
       </c>
       <c r="M33" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$87:M$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B33,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D33,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E33)*0.000001</f>
-        <v>5.9520332170721404E-2</v>
+        <v>5.95182247821592E-2</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -12750,7 +12750,7 @@
         <v>7</v>
       </c>
       <c r="F34" s="2">
-        <f ca="1">SUMIFS('Engines indvidual'!F$87:F$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B34,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D34,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E34)*0.000001</f>
+        <f ca="1">SUMIFS('Engines indvidual'!F$87:F$178,'Engines indvidual'!$B$87:$B$178,'Full system - simplified'!$B34,'Engines indvidual'!$D$87:$D$178,'Full system - simplified'!$D34,'Engines indvidual'!$E$87:$E$178,'Full system - simplified'!$E34)*0.000001</f>
         <v>7.9139880154120394</v>
       </c>
       <c r="G34" s="3">
@@ -12799,7 +12799,7 @@
         <v>7</v>
       </c>
       <c r="F35" s="2">
-        <f ca="1">SUMIFS('Engines indvidual'!F$87:F$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B35,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D35,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E35)*0.000001</f>
+        <f ca="1">SUMIFS('Engines indvidual'!F$87:F$178,'Engines indvidual'!$B$87:$B$178,'Full system - simplified'!$B35,'Engines indvidual'!$D$87:$D$178,'Full system - simplified'!$D35,'Engines indvidual'!$E$87:$E$178,'Full system - simplified'!$E35)*0.000001</f>
         <v>0</v>
       </c>
       <c r="G35" s="3">
@@ -12848,8 +12848,8 @@
         <v>14</v>
       </c>
       <c r="F36" s="2">
-        <f ca="1">SUMIFS('Engines indvidual'!F$87:F$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B36,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D36,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E36)*0.000001</f>
-        <v>0.23637764496103952</v>
+        <f ca="1">SUMIFS('Engines indvidual'!F$87:F$178,'Engines indvidual'!$B$87:$B$178,'Full system - simplified'!$B36,'Engines indvidual'!$D$87:$D$178,'Full system - simplified'!$D36,'Engines indvidual'!$E$87:$E$178,'Full system - simplified'!$E36)*0.000001</f>
+        <v>0.23639126868745125</v>
       </c>
       <c r="G36" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$87:G$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B36,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D36,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E36)*0.000001</f>
@@ -12897,7 +12897,7 @@
         <v>14</v>
       </c>
       <c r="F37" s="2">
-        <f ca="1">SUMIFS('Engines indvidual'!F$87:F$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B37,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D37,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E37)*0.000001</f>
+        <f ca="1">SUMIFS('Engines indvidual'!F$87:F$178,'Engines indvidual'!$B$87:$B$178,'Full system - simplified'!$B37,'Engines indvidual'!$D$87:$D$178,'Full system - simplified'!$D37,'Engines indvidual'!$E$87:$E$178,'Full system - simplified'!$E37)*0.000001</f>
         <v>0.36023136970580405</v>
       </c>
       <c r="G37" s="3">
@@ -12946,36 +12946,36 @@
         <v>14</v>
       </c>
       <c r="F38" s="2">
-        <f ca="1">SUMIFS('Engines indvidual'!F$87:F$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B38,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D38,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E38)*0.000001</f>
-        <v>3.1373384055217297</v>
+        <f ca="1">SUMIFS('Engines indvidual'!F$87:F$178,'Engines indvidual'!$B$87:$B$178,'Full system - simplified'!$B38,'Engines indvidual'!$D$87:$D$178,'Full system - simplified'!$D38,'Engines indvidual'!$E$87:$E$178,'Full system - simplified'!$E38)*0.000001</f>
+        <v>3.1385913166244492</v>
       </c>
       <c r="G38" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$87:G$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B38,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D38,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E38)*0.000001</f>
-        <v>0.96147420231622294</v>
+        <v>0.96189215463700395</v>
       </c>
       <c r="H38" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$87:H$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B38,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D38,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E38)*0.000001</f>
-        <v>1.756744755703155</v>
+        <v>1.7574882193867036</v>
       </c>
       <c r="I38" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$87:I$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B38,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D38,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E38)*0.000001</f>
-        <v>0.34421383763347191</v>
+        <v>0.34430030799367595</v>
       </c>
       <c r="J38" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$87:J$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B38,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D38,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E38)*0.000001</f>
-        <v>7.4905609868858525E-2</v>
+        <v>7.4910634607029236E-2</v>
       </c>
       <c r="K38" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$87:K$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B38,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D38,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E38)*0.000001</f>
-        <v>1.4758357184061859</v>
+        <v>1.4758371543503399</v>
       </c>
       <c r="L38" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$87:L$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B38,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D38,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E38)*0.000001</f>
-        <v>1.2745873020685159</v>
+        <v>1.27470452664734</v>
       </c>
       <c r="M38" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$87:M$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B38,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D38,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E38)*0.000001</f>
-        <v>0.38691538504700607</v>
+        <v>0.38804963562674705</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -12995,36 +12995,36 @@
         <v>14</v>
       </c>
       <c r="F39" s="2">
-        <f ca="1">SUMIFS('Engines indvidual'!F$87:F$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B39,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D39,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E39)*0.000001</f>
-        <v>5.8399909108127108</v>
+        <f ca="1">SUMIFS('Engines indvidual'!F$87:F$178,'Engines indvidual'!$B$87:$B$178,'Full system - simplified'!$B39,'Engines indvidual'!$D$87:$D$178,'Full system - simplified'!$D39,'Engines indvidual'!$E$87:$E$178,'Full system - simplified'!$E39)*0.000001</f>
+        <v>5.8421744516265459</v>
       </c>
       <c r="G39" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$87:G$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B39,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D39,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E39)*0.000001</f>
-        <v>1.7713015248069959</v>
+        <v>1.7720389159021479</v>
       </c>
       <c r="H39" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$87:H$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B39,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D39,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E39)*0.000001</f>
-        <v>3.2686799202521661</v>
+        <v>3.2699570734274257</v>
       </c>
       <c r="I39" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$87:I$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B39,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D39,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E39)*0.000001</f>
-        <v>0.65631594983988406</v>
+        <v>0.65647531334767395</v>
       </c>
       <c r="J39" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$87:J$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B39,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D39,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E39)*0.000001</f>
-        <v>0.1436935159136537</v>
+        <v>0.1437031489492924</v>
       </c>
       <c r="K39" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$87:K$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B39,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D39,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E39)*0.000001</f>
-        <v>2.6080520744797098</v>
+        <v>2.6080544389530509</v>
       </c>
       <c r="L39" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$87:L$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B39,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D39,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E39)*0.000001</f>
-        <v>2.4511736660152832</v>
+        <v>2.451388349350947</v>
       </c>
       <c r="M39" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$87:M$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B39,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D39,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E39)*0.000001</f>
-        <v>0.78076517031770287</v>
+        <v>0.78273166332253896</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -13044,36 +13044,36 @@
         <v>14</v>
       </c>
       <c r="F40" s="2">
-        <f ca="1">SUMIFS('Engines indvidual'!F$87:F$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B40,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D40,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E40)*0.000001</f>
-        <v>3.9027149353637798</v>
+        <f ca="1">SUMIFS('Engines indvidual'!F$87:F$178,'Engines indvidual'!$B$87:$B$178,'Full system - simplified'!$B40,'Engines indvidual'!$D$87:$D$178,'Full system - simplified'!$D40,'Engines indvidual'!$E$87:$E$178,'Full system - simplified'!$E40)*0.000001</f>
+        <v>3.9041715770093202</v>
       </c>
       <c r="G40" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$87:G$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B40,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D40,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E40)*0.000001</f>
-        <v>1.7713015248069959</v>
+        <v>1.7720389159021479</v>
       </c>
       <c r="H40" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$87:H$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B40,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D40,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E40)*0.000001</f>
-        <v>3.2686799202521661</v>
+        <v>3.2699570734274257</v>
       </c>
       <c r="I40" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$87:I$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B40,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D40,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E40)*0.000001</f>
-        <v>0.65631594983988406</v>
+        <v>0.65647531334767395</v>
       </c>
       <c r="J40" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$87:J$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B40,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D40,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E40)*0.000001</f>
-        <v>0.1436935159136537</v>
+        <v>0.1437031489492924</v>
       </c>
       <c r="K40" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$87:K$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B40,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D40,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E40)*0.000001</f>
-        <v>2.6080520744797098</v>
+        <v>2.6080544389530509</v>
       </c>
       <c r="L40" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$87:L$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B40,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D40,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E40)*0.000001</f>
-        <v>2.4511736660152832</v>
+        <v>2.451388349350947</v>
       </c>
       <c r="M40" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$87:M$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B40,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D40,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E40)*0.000001</f>
-        <v>0.78076517031770287</v>
+        <v>0.78273166332253896</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -13093,36 +13093,36 @@
         <v>14</v>
       </c>
       <c r="F41" s="2">
-        <f ca="1">SUMIFS('Engines indvidual'!F$87:F$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B41,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D41,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E41)*0.000001</f>
-        <v>2.1838919488006261</v>
+        <f ca="1">SUMIFS('Engines indvidual'!F$87:F$178,'Engines indvidual'!$B$87:$B$178,'Full system - simplified'!$B41,'Engines indvidual'!$D$87:$D$178,'Full system - simplified'!$D41,'Engines indvidual'!$E$87:$E$178,'Full system - simplified'!$E41)*0.000001</f>
+        <v>2.1846840783047257</v>
       </c>
       <c r="G41" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$87:G$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B41,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D41,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E41)*0.000001</f>
-        <v>0.96147420231622294</v>
+        <v>0.96189215463700395</v>
       </c>
       <c r="H41" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$87:H$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B41,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D41,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E41)*0.000001</f>
-        <v>1.756744755703155</v>
+        <v>1.7574882193867036</v>
       </c>
       <c r="I41" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$87:I$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B41,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D41,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E41)*0.000001</f>
-        <v>0.34421383763347191</v>
+        <v>0.34430030799367595</v>
       </c>
       <c r="J41" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$87:J$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B41,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D41,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E41)*0.000001</f>
-        <v>7.4905609868858525E-2</v>
+        <v>7.4910634607029236E-2</v>
       </c>
       <c r="K41" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$87:K$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B41,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D41,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E41)*0.000001</f>
-        <v>1.4758357184061859</v>
+        <v>1.4758371543503399</v>
       </c>
       <c r="L41" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$87:L$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B41,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D41,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E41)*0.000001</f>
-        <v>1.2745873020685159</v>
+        <v>1.27470452664734</v>
       </c>
       <c r="M41" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$87:M$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B41,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D41,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E41)*0.000001</f>
-        <v>0.38691538504700607</v>
+        <v>0.38804963562674705</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -13142,7 +13142,7 @@
         <v>14</v>
       </c>
       <c r="F42" s="2">
-        <f ca="1">SUMIFS('Engines indvidual'!F$87:F$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B42,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D42,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E42)*0.000001</f>
+        <f ca="1">SUMIFS('Engines indvidual'!F$87:F$178,'Engines indvidual'!$B$87:$B$178,'Full system - simplified'!$B42,'Engines indvidual'!$D$87:$D$178,'Full system - simplified'!$D42,'Engines indvidual'!$E$87:$E$178,'Full system - simplified'!$E42)*0.000001</f>
         <v>0.36890869617646871</v>
       </c>
       <c r="G42" s="3">
@@ -13191,28 +13191,28 @@
         <v>14</v>
       </c>
       <c r="F43" s="2">
-        <f ca="1">SUMIFS('Engines indvidual'!F$87:F$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B43,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D43,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E43)*0.000001</f>
-        <v>6.3236228093154345</v>
+        <f ca="1">SUMIFS('Engines indvidual'!F$87:F$178,'Engines indvidual'!$B$87:$B$178,'Full system - simplified'!$B43,'Engines indvidual'!$D$87:$D$178,'Full system - simplified'!$D43,'Engines indvidual'!$E$87:$E$178,'Full system - simplified'!$E43)*0.000001</f>
+        <v>6.3235888529284194</v>
       </c>
       <c r="G43" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$87:G$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B43,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D43,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E43)*0.000001</f>
-        <v>2.8692549161887833</v>
+        <v>2.8692401641446943</v>
       </c>
       <c r="H43" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$87:H$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B43,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D43,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E43)*0.000001</f>
-        <v>5.5040193618164501</v>
+        <v>5.503985344626499</v>
       </c>
       <c r="I43" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$87:I$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B43,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D43,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E43)*0.000001</f>
-        <v>1.0110670874328809</v>
+        <v>1.011062867537627</v>
       </c>
       <c r="J43" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$87:J$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B43,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D43,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E43)*0.000001</f>
-        <v>0.23748466690132874</v>
+        <v>0.23748452825795754</v>
       </c>
       <c r="K43" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$87:K$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B43,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D43,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E43)*0.000001</f>
-        <v>4.3085586678437124</v>
+        <v>4.3085586681680219</v>
       </c>
       <c r="L43" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$87:L$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B43,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D43,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E43)*0.000001</f>
@@ -13220,7 +13220,7 @@
       </c>
       <c r="M43" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$87:M$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B43,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D43,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E43)*0.000001</f>
-        <v>1.412210108168291</v>
+        <v>1.4121569800712916</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -13240,28 +13240,28 @@
         <v>7</v>
       </c>
       <c r="F44" s="2">
-        <f ca="1">SUMIFS('Engines indvidual'!F$87:F$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B44,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D44,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E44)*0.000001</f>
-        <v>11.420652066936821</v>
+        <f ca="1">SUMIFS('Engines indvidual'!F$87:F$178,'Engines indvidual'!$B$87:$B$178,'Full system - simplified'!$B44,'Engines indvidual'!$D$87:$D$178,'Full system - simplified'!$D44,'Engines indvidual'!$E$87:$E$178,'Full system - simplified'!$E44)*0.000001</f>
+        <v>11.42059301671924</v>
       </c>
       <c r="G44" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!G$87:G$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B44,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D44,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E44)*0.000001</f>
-        <v>3.5090896918111696</v>
+        <v>3.5090731302080709</v>
       </c>
       <c r="H44" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!H$87:H$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B44,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D44,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E44)*0.000001</f>
-        <v>6.4321943576416905</v>
+        <v>6.4321550509296594</v>
       </c>
       <c r="I44" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!I$87:I$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B44,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D44,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E44)*0.000001</f>
-        <v>1.1454417490045459</v>
+        <v>1.1454386502093947</v>
       </c>
       <c r="J44" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!J$87:J$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B44,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D44,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E44)*0.000001</f>
-        <v>0.33392626847940904</v>
+        <v>0.33392618537210222</v>
       </c>
       <c r="K44" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!K$87:K$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B44,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D44,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E44)*0.000001</f>
-        <v>4.8569454909505971</v>
+        <v>4.8569454921977577</v>
       </c>
       <c r="L44" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!L$87:L$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B44,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D44,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E44)*0.000001</f>
@@ -13269,7 +13269,7 @@
       </c>
       <c r="M44" s="3">
         <f ca="1">SUMIFS('Engines indvidual'!M$87:M$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B44,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D44,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E44)*0.000001</f>
-        <v>1.5988420015068729</v>
+        <v>1.5987829500421351</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -13289,7 +13289,7 @@
         <v>12</v>
       </c>
       <c r="F45" s="2">
-        <f ca="1">SUMIFS('Engines indvidual'!F$87:F$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B45,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D45,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E45)*0.000001</f>
+        <f ca="1">SUMIFS('Engines indvidual'!F$87:F$178,'Engines indvidual'!$B$87:$B$178,'Full system - simplified'!$B45,'Engines indvidual'!$D$87:$D$178,'Full system - simplified'!$D45,'Engines indvidual'!$E$87:$E$178,'Full system - simplified'!$E45)*0.000001</f>
         <v>62.015060713286694</v>
       </c>
       <c r="G45" s="3">
@@ -13338,7 +13338,7 @@
         <v>14</v>
       </c>
       <c r="F46" s="2">
-        <f ca="1">SUMIFS('Engines indvidual'!F$87:F$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B46,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D46,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E46)*0.000001</f>
+        <f ca="1">SUMIFS('Engines indvidual'!F$87:F$178,'Engines indvidual'!$B$87:$B$178,'Full system - simplified'!$B46,'Engines indvidual'!$D$87:$D$178,'Full system - simplified'!$D46,'Engines indvidual'!$E$87:$E$178,'Full system - simplified'!$E46)*0.000001</f>
         <v>0.85095044339192205</v>
       </c>
       <c r="G46" s="3">
@@ -13389,36 +13389,36 @@
         <v>55</v>
       </c>
       <c r="F47" s="2">
-        <f ca="1">SUMIFS('Engines indvidual'!F$87:F$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B47,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D47,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E47)*0.000001</f>
-        <v>132.72612658248119</v>
+        <f ca="1">SUMIFS('Engines indvidual'!F$87:F$178,'Engines indvidual'!$B$87:$B$178,'Full system - simplified'!$B47,'Engines indvidual'!$D$87:$D$178,'Full system - simplified'!$D47,'Engines indvidual'!$E$87:$E$178,'Full system - simplified'!$E47)*0.000001</f>
+        <v>172.0931645320693</v>
       </c>
       <c r="G47" s="3">
-        <f ca="1">SUMIFS('Engines indvidual'!G$87:G$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B47,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D47,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E47)*0.000001</f>
-        <v>45.936166657694798</v>
+        <f ca="1">SUMIFS('Engines indvidual'!G$87:G$178,'Engines indvidual'!$B$87:$B$178,'Full system - simplified'!$B47,'Engines indvidual'!$D$87:$D$178,'Full system - simplified'!$D47,'Engines indvidual'!$E$87:$E$178,'Full system - simplified'!$E47)*0.000001</f>
+        <v>54.452354323077152</v>
       </c>
       <c r="H47" s="3">
-        <f ca="1">SUMIFS('Engines indvidual'!H$87:H$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B47,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D47,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E47)*0.000001</f>
-        <v>69.570189402788401</v>
+        <f ca="1">SUMIFS('Engines indvidual'!H$87:H$178,'Engines indvidual'!$B$87:$B$178,'Full system - simplified'!$B47,'Engines indvidual'!$D$87:$D$178,'Full system - simplified'!$D47,'Engines indvidual'!$E$87:$E$178,'Full system - simplified'!$E47)*0.000001</f>
+        <v>94.875950481212797</v>
       </c>
       <c r="I47" s="3">
-        <f ca="1">SUMIFS('Engines indvidual'!I$87:I$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B47,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D47,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E47)*0.000001</f>
-        <v>13.29399867389227</v>
+        <f ca="1">SUMIFS('Engines indvidual'!I$87:I$178,'Engines indvidual'!$B$87:$B$178,'Full system - simplified'!$B47,'Engines indvidual'!$D$87:$D$178,'Full system - simplified'!$D47,'Engines indvidual'!$E$87:$E$178,'Full system - simplified'!$E47)*0.000001</f>
+        <v>17.91566363898793</v>
       </c>
       <c r="J47" s="3">
-        <f ca="1">SUMIFS('Engines indvidual'!J$87:J$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B47,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D47,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E47)*0.000001</f>
-        <v>3.9257718481053794</v>
+        <f ca="1">SUMIFS('Engines indvidual'!J$87:J$178,'Engines indvidual'!$B$87:$B$178,'Full system - simplified'!$B47,'Engines indvidual'!$D$87:$D$178,'Full system - simplified'!$D47,'Engines indvidual'!$E$87:$E$178,'Full system - simplified'!$E47)*0.000001</f>
+        <v>4.8491960887910999</v>
       </c>
       <c r="K47" s="3">
-        <f ca="1">SUMIFS('Engines indvidual'!K$87:K$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B47,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D47,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E47)*0.000001</f>
-        <v>55.109651611425647</v>
+        <f ca="1">SUMIFS('Engines indvidual'!K$87:K$178,'Engines indvidual'!$B$87:$B$178,'Full system - simplified'!$B47,'Engines indvidual'!$D$87:$D$178,'Full system - simplified'!$D47,'Engines indvidual'!$E$87:$E$178,'Full system - simplified'!$E47)*0.000001</f>
+        <v>73.199398540672746</v>
       </c>
       <c r="L47" s="3">
-        <f ca="1">SUMIFS('Engines indvidual'!L$87:L$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B47,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D47,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E47)*0.000001</f>
-        <v>56.6606318272717</v>
+        <f ca="1">SUMIFS('Engines indvidual'!L$87:L$178,'Engines indvidual'!$B$87:$B$178,'Full system - simplified'!$B47,'Engines indvidual'!$D$87:$D$178,'Full system - simplified'!$D47,'Engines indvidual'!$E$87:$E$178,'Full system - simplified'!$E47)*0.000001</f>
+        <v>72.743765448047995</v>
       </c>
       <c r="M47" s="3">
-        <f ca="1">SUMIFS('Engines indvidual'!M$87:M$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B47,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D47,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E47)*0.000001</f>
-        <v>20.955843143783458</v>
+        <f ca="1">SUMIFS('Engines indvidual'!M$87:M$178,'Engines indvidual'!$B$87:$B$178,'Full system - simplified'!$B47,'Engines indvidual'!$D$87:$D$178,'Full system - simplified'!$D47,'Engines indvidual'!$E$87:$E$178,'Full system - simplified'!$E47)*0.000001</f>
+        <v>26.150000543347947</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -13440,36 +13440,36 @@
         <v>14</v>
       </c>
       <c r="F48" s="2">
-        <f ca="1">SUMIFS('Engines indvidual'!F$87:F$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B48,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D48,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E48)*0.000001</f>
-        <v>6.1555876100334417E-2</v>
+        <f ca="1">SUMIFS('Engines indvidual'!F$87:F$178,'Engines indvidual'!$B$87:$B$178,'Full system - simplified'!$B48,'Engines indvidual'!$D$87:$D$178,'Full system - simplified'!$D48,'Engines indvidual'!$E$87:$E$178,'Full system - simplified'!$E48)*0.000001</f>
+        <v>8.4550921016045305E-2</v>
       </c>
       <c r="G48" s="3">
-        <f ca="1">SUMIFS('Engines indvidual'!G$87:G$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B48,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D48,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E48)*0.000001</f>
-        <v>1.373020519462948E-2</v>
+        <f ca="1">SUMIFS('Engines indvidual'!G$87:G$178,'Engines indvidual'!$B$87:$B$178,'Full system - simplified'!$B48,'Engines indvidual'!$D$87:$D$178,'Full system - simplified'!$D48,'Engines indvidual'!$E$87:$E$178,'Full system - simplified'!$E48)*0.000001</f>
+        <v>1.8849683713073842E-2</v>
       </c>
       <c r="H48" s="3">
-        <f ca="1">SUMIFS('Engines indvidual'!H$87:H$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B48,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D48,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E48)*0.000001</f>
-        <v>3.9674756031368531E-2</v>
+        <f ca="1">SUMIFS('Engines indvidual'!H$87:H$178,'Engines indvidual'!$B$87:$B$178,'Full system - simplified'!$B48,'Engines indvidual'!$D$87:$D$178,'Full system - simplified'!$D48,'Engines indvidual'!$E$87:$E$178,'Full system - simplified'!$E48)*0.000001</f>
+        <v>5.4426729058256636E-2</v>
       </c>
       <c r="I48" s="3">
-        <f ca="1">SUMIFS('Engines indvidual'!I$87:I$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B48,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D48,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E48)*0.000001</f>
-        <v>6.1382908820144261E-3</v>
+        <f ca="1">SUMIFS('Engines indvidual'!I$87:I$178,'Engines indvidual'!$B$87:$B$178,'Full system - simplified'!$B48,'Engines indvidual'!$D$87:$D$178,'Full system - simplified'!$D48,'Engines indvidual'!$E$87:$E$178,'Full system - simplified'!$E48)*0.000001</f>
+        <v>8.7601687964781304E-3</v>
       </c>
       <c r="J48" s="3">
-        <f ca="1">SUMIFS('Engines indvidual'!J$87:J$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B48,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D48,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E48)*0.000001</f>
-        <v>2.0126239923221869E-3</v>
+        <f ca="1">SUMIFS('Engines indvidual'!J$87:J$178,'Engines indvidual'!$B$87:$B$178,'Full system - simplified'!$B48,'Engines indvidual'!$D$87:$D$178,'Full system - simplified'!$D48,'Engines indvidual'!$E$87:$E$178,'Full system - simplified'!$E48)*0.000001</f>
+        <v>2.5143394482368274E-3</v>
       </c>
       <c r="K48" s="3">
-        <f ca="1">SUMIFS('Engines indvidual'!K$87:K$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B48,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D48,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E48)*0.000001</f>
-        <v>2.9716346146805548E-2</v>
+        <f ca="1">SUMIFS('Engines indvidual'!K$87:K$178,'Engines indvidual'!$B$87:$B$178,'Full system - simplified'!$B48,'Engines indvidual'!$D$87:$D$178,'Full system - simplified'!$D48,'Engines indvidual'!$E$87:$E$178,'Full system - simplified'!$E48)*0.000001</f>
+        <v>4.1376724853766263E-2</v>
       </c>
       <c r="L48" s="3">
-        <f ca="1">SUMIFS('Engines indvidual'!L$87:L$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B48,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D48,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E48)*0.000001</f>
-        <v>2.4481271611707139E-2</v>
+        <f ca="1">SUMIFS('Engines indvidual'!L$87:L$178,'Engines indvidual'!$B$87:$B$178,'Full system - simplified'!$B48,'Engines indvidual'!$D$87:$D$178,'Full system - simplified'!$D48,'Engines indvidual'!$E$87:$E$178,'Full system - simplified'!$E48)*0.000001</f>
+        <v>3.3442589666931991E-2</v>
       </c>
       <c r="M48" s="3">
-        <f ca="1">SUMIFS('Engines indvidual'!M$87:M$176,'Engines indvidual'!$B$87:$B$176,'Full system - simplified'!$B48,'Engines indvidual'!$D$87:$D$176,'Full system - simplified'!$D48,'Engines indvidual'!$E$87:$E$176,'Full system - simplified'!$E48)*0.000001</f>
-        <v>7.3582583418218611E-3</v>
+        <f ca="1">SUMIFS('Engines indvidual'!M$87:M$178,'Engines indvidual'!$B$87:$B$178,'Full system - simplified'!$B48,'Engines indvidual'!$D$87:$D$178,'Full system - simplified'!$D48,'Engines indvidual'!$E$87:$E$178,'Full system - simplified'!$E48)*0.000001</f>
+        <v>9.7316064953471802E-3</v>
       </c>
     </row>
     <row r="50" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -13490,35 +13490,35 @@
       </c>
       <c r="F50" s="2">
         <f t="shared" ref="F50:M50" ca="1" si="0">F13+F17+F36+F40-F51</f>
-        <v>7.3593339603355172</v>
+        <v>7.3603801608752697</v>
       </c>
       <c r="G50" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.4569712855244032</v>
+        <v>1.4575234904110455</v>
       </c>
       <c r="H50" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>8.6274107299374592</v>
+        <v>8.6284652041681174</v>
       </c>
       <c r="I50" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.3640920780791912</v>
+        <v>1.3642357471279312</v>
       </c>
       <c r="J50" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.97414992816775625</v>
+        <v>0.974159055983296</v>
       </c>
       <c r="K50" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>5.0972009778770051</v>
+        <v>5.0972026952310463</v>
       </c>
       <c r="L50" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>5.2474772962100262</v>
+        <v>5.2476433215982112</v>
       </c>
       <c r="M50" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.077945747621762</v>
+        <v>2.079537480861148</v>
       </c>
     </row>
     <row r="51" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -13539,35 +13539,35 @@
       </c>
       <c r="F51" s="2">
         <f>([1]aggregated_flows_exergy!B$479-[1]aggregated_flows_exergy!B$482)*0.000001</f>
-        <v>3.2444042199455012</v>
+        <v>3.2448282847777006</v>
       </c>
       <c r="G51" s="2">
         <f>([1]aggregated_flows_exergy!C$479-[1]aggregated_flows_exergy!C$482)*0.000001</f>
-        <v>0.46158876188278009</v>
+        <v>0.46177394809128997</v>
       </c>
       <c r="H51" s="2">
         <f>([1]aggregated_flows_exergy!D$479-[1]aggregated_flows_exergy!D$482)*0.000001</f>
-        <v>2.3266007049292994</v>
+        <v>2.3268233838739003</v>
       </c>
       <c r="I51" s="2">
         <f>([1]aggregated_flows_exergy!E$479-[1]aggregated_flows_exergy!E$482)*0.000001</f>
-        <v>0.31211331308048007</v>
+        <v>0.31212900753953005</v>
       </c>
       <c r="J51" s="2">
         <f>([1]aggregated_flows_exergy!F$479-[1]aggregated_flows_exergy!F$482)*0.000001</f>
-        <v>0.14410144005283701</v>
+        <v>0.14410194527293602</v>
       </c>
       <c r="K51" s="2">
         <f>([1]aggregated_flows_exergy!G$479-[1]aggregated_flows_exergy!G$482)*0.000001</f>
-        <v>1.5253791035369988</v>
+        <v>1.5253797506562992</v>
       </c>
       <c r="L51" s="2">
         <f>([1]aggregated_flows_exergy!H$479-[1]aggregated_flows_exergy!H$482)*0.000001</f>
-        <v>1.3376564210866801</v>
+        <v>1.3377050790341589</v>
       </c>
       <c r="M51" s="2">
         <f>([1]aggregated_flows_exergy!I$479-[1]aggregated_flows_exergy!I$482)*0.000001</f>
-        <v>0.38136869532173989</v>
+        <v>0.38174345508718999</v>
       </c>
       <c r="O51" s="2"/>
     </row>
@@ -13589,35 +13589,35 @@
       </c>
       <c r="F52" s="2">
         <f>([1]aggregated_flows_exergy!B$498-[1]aggregated_flows_exergy!B$499)*0.000001</f>
-        <v>10.870576729180531</v>
+        <v>10.869838541211299</v>
       </c>
       <c r="G52" s="2">
         <f>([1]aggregated_flows_exergy!C$498-[1]aggregated_flows_exergy!C$499)*0.000001</f>
-        <v>4.9418622286567819</v>
+        <v>4.941531819725629</v>
       </c>
       <c r="H52" s="2">
         <f>([1]aggregated_flows_exergy!D$498-[1]aggregated_flows_exergy!D$499)*0.000001</f>
-        <v>5.0877626892342755</v>
+        <v>5.0873828165680139</v>
       </c>
       <c r="I52" s="2">
         <f>([1]aggregated_flows_exergy!E$498-[1]aggregated_flows_exergy!E$499)*0.000001</f>
-        <v>0.75081095889419491</v>
+        <v>0.75078386791239293</v>
       </c>
       <c r="J52" s="2">
         <f>([1]aggregated_flows_exergy!F$498-[1]aggregated_flows_exergy!F$499)*0.000001</f>
-        <v>9.014085239542298E-2</v>
+        <v>9.0140037005311785E-2</v>
       </c>
       <c r="K52" s="2">
         <f>([1]aggregated_flows_exergy!G$498-[1]aggregated_flows_exergy!G$499)*0.000001</f>
-        <v>6.5149143259059699</v>
+        <v>6.5149132268973791</v>
       </c>
       <c r="L52" s="2">
         <f>([1]aggregated_flows_exergy!H$498-[1]aggregated_flows_exergy!H$499)*0.000001</f>
-        <v>3.820487374233541</v>
+        <v>3.8204015369889599</v>
       </c>
       <c r="M52" s="2">
         <f>([1]aggregated_flows_exergy!I$498-[1]aggregated_flows_exergy!I$499)*0.000001</f>
-        <v>0.53517502904116687</v>
+        <v>0.53452377732502487</v>
       </c>
       <c r="O52" s="2"/>
     </row>
@@ -13639,35 +13639,35 @@
       </c>
       <c r="F53" s="2">
         <f>([1]aggregated_flows_exergy!B$510-[1]aggregated_flows_exergy!B$509-SUM([1]aggregated_flows_exergy!B$511:'[1]aggregated_flows_exergy'!B$516))*0.000001</f>
-        <v>5.7096501334865497</v>
+        <v>5.7096513436834009</v>
       </c>
       <c r="G53" s="2">
         <f>([1]aggregated_flows_exergy!C$510-[1]aggregated_flows_exergy!C$509-SUM([1]aggregated_flows_exergy!C$511:'[1]aggregated_flows_exergy'!C$516))*0.000001</f>
-        <v>4.6630771794128885</v>
+        <v>4.6627074863230265</v>
       </c>
       <c r="H53" s="2">
         <f>([1]aggregated_flows_exergy!D$510-[1]aggregated_flows_exergy!D$509-SUM([1]aggregated_flows_exergy!D$511:'[1]aggregated_flows_exergy'!D$516))*0.000001</f>
-        <v>0.90369818450296857</v>
+        <v>0.90398765443135798</v>
       </c>
       <c r="I53" s="2">
         <f>([1]aggregated_flows_exergy!E$510-[1]aggregated_flows_exergy!E$509-SUM([1]aggregated_flows_exergy!E$511:'[1]aggregated_flows_exergy'!E$516))*0.000001</f>
-        <v>0.17069798557507224</v>
+        <v>0.17077912828211114</v>
       </c>
       <c r="J53" s="2">
         <f>([1]aggregated_flows_exergy!F$510-[1]aggregated_flows_exergy!F$509-SUM([1]aggregated_flows_exergy!F$511:'[1]aggregated_flows_exergy'!F$516))*0.000001</f>
-        <v>-2.7823216004492946E-2</v>
+        <v>-2.7822925353212163E-2</v>
       </c>
       <c r="K53" s="2">
         <f>([1]aggregated_flows_exergy!G$510-[1]aggregated_flows_exergy!G$509-SUM([1]aggregated_flows_exergy!G$511:'[1]aggregated_flows_exergy'!G$516))*0.000001</f>
-        <v>3.7689686011003198</v>
+        <v>3.7689685929079437</v>
       </c>
       <c r="L53" s="2">
         <f>([1]aggregated_flows_exergy!H$510-[1]aggregated_flows_exergy!H$509-SUM([1]aggregated_flows_exergy!H$511:'[1]aggregated_flows_exergy'!H$516))*0.000001</f>
-        <v>1.8451238843803666</v>
+        <v>1.8451238973561674</v>
       </c>
       <c r="M53" s="2">
         <f>([1]aggregated_flows_exergy!I$510-[1]aggregated_flows_exergy!I$509-SUM([1]aggregated_flows_exergy!I$511:'[1]aggregated_flows_exergy'!I$516))*0.000001</f>
-        <v>9.5557648005575868E-2</v>
+        <v>9.5558853419022857E-2</v>
       </c>
     </row>
     <row r="54" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -14031,27 +14031,27 @@
       </c>
       <c r="F61" s="2">
         <f>([1]aggregated_flows_exergy!B$540 - [1]aggregated_flows_exergy!B$529)*0.000001</f>
-        <v>0.44326990732632549</v>
+        <v>0.44328133514031093</v>
       </c>
       <c r="G61" s="2">
         <f>[1]aggregated_flows_exergy!C$577*0.000001</f>
-        <v>3.6964912978471001E-2</v>
+        <v>3.6966927817431001E-2</v>
       </c>
       <c r="H61" s="2">
         <f>[1]aggregated_flows_exergy!D$577*0.000001</f>
-        <v>0.20780884410724598</v>
+        <v>0.20781359028674198</v>
       </c>
       <c r="I61" s="2">
         <f>[1]aggregated_flows_exergy!E$577*0.000001</f>
-        <v>2.8580759289889502E-2</v>
+        <v>2.8581253586086999E-2</v>
       </c>
       <c r="J61" s="2">
         <f>[1]aggregated_flows_exergy!F$577*0.000001</f>
-        <v>2.0541942691823498E-2</v>
+        <v>2.0541987731748899E-2</v>
       </c>
       <c r="K61" s="2">
         <f>[1]aggregated_flows_exergy!G$577*0.000001</f>
-        <v>0.128599540424509</v>
+        <v>0.128599540169755</v>
       </c>
       <c r="L61" s="2">
         <f>[1]aggregated_flows_exergy!H$577*0.000001</f>
@@ -14059,7 +14059,7 @@
       </c>
       <c r="M61" s="2">
         <f>[1]aggregated_flows_exergy!I$577*0.000001</f>
-        <v>4.3799125134392193E-2</v>
+        <v>4.3806425743724994E-2</v>
       </c>
     </row>
     <row r="62" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -14472,35 +14472,35 @@
       </c>
       <c r="F70" s="2">
         <f>[1]aggregated_flows_exergy!B$533*0.000001</f>
-        <v>0.80655419849585186</v>
+        <v>0.80736172195589295</v>
       </c>
       <c r="G70" s="2">
         <f>[1]aggregated_flows_exergy!C$533*0.000001</f>
-        <v>3.9129252321069598E-3</v>
+        <v>3.9132575424330697E-3</v>
       </c>
       <c r="H70" s="2">
         <f>[1]aggregated_flows_exergy!D$533*0.000001</f>
-        <v>0.42573842593756595</v>
+        <v>0.42643606333583195</v>
       </c>
       <c r="I70" s="2">
         <f>[1]aggregated_flows_exergy!E$533*0.000001</f>
-        <v>0.12687938055836198</v>
+        <v>0.126987932678293</v>
       </c>
       <c r="J70" s="2">
         <f>[1]aggregated_flows_exergy!F$533*0.000001</f>
-        <v>0.250023466767818</v>
+        <v>0.25002446839933495</v>
       </c>
       <c r="K70" s="2">
         <f>[1]aggregated_flows_exergy!G$533*0.000001</f>
-        <v>5.3673321406558699E-2</v>
+        <v>5.3674609794177999E-2</v>
       </c>
       <c r="L70" s="2">
         <f>[1]aggregated_flows_exergy!H$533*0.000001</f>
-        <v>0.19971323018027098</v>
+        <v>0.199813633035826</v>
       </c>
       <c r="M70" s="2">
         <f>[1]aggregated_flows_exergy!I$533*0.000001</f>
-        <v>0.55316764690902498</v>
+        <v>0.55387347912588991</v>
       </c>
     </row>
     <row r="72" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -14748,27 +14748,27 @@
       </c>
       <c r="F77" s="2">
         <f>[1]aggregated_flows_exergy!B$577*0.000001</f>
-        <v>0.29389645906742901</v>
+        <v>0.29390375942200797</v>
       </c>
       <c r="G77" s="2">
         <f>[1]aggregated_flows_exergy!C$577*0.000001</f>
-        <v>3.6964912978471001E-2</v>
+        <v>3.6966927817431001E-2</v>
       </c>
       <c r="H77" s="2">
         <f>[1]aggregated_flows_exergy!D$577*0.000001</f>
-        <v>0.20780884410724598</v>
+        <v>0.20781359028674198</v>
       </c>
       <c r="I77" s="2">
         <f>[1]aggregated_flows_exergy!E$577*0.000001</f>
-        <v>2.8580759289889502E-2</v>
+        <v>2.8581253586086999E-2</v>
       </c>
       <c r="J77" s="2">
         <f>[1]aggregated_flows_exergy!F$577*0.000001</f>
-        <v>2.0541942691823498E-2</v>
+        <v>2.0541987731748899E-2</v>
       </c>
       <c r="K77" s="2">
         <f>[1]aggregated_flows_exergy!G$577*0.000001</f>
-        <v>0.128599540424509</v>
+        <v>0.128599540169755</v>
       </c>
       <c r="L77" s="2">
         <f>[1]aggregated_flows_exergy!H$577*0.000001</f>
@@ -14776,7 +14776,7 @@
       </c>
       <c r="M77" s="2">
         <f>[1]aggregated_flows_exergy!I$577*0.000001</f>
-        <v>4.3799125134392193E-2</v>
+        <v>4.3806425743724994E-2</v>
       </c>
     </row>
     <row r="78" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>